<commit_message>
Aded new versions as of 19-10-2023
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="728" documentId="8_{9E989A0F-969E-4ED2-9560-FEB0541538CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{529ECFF6-861B-48A6-8DB1-B48F7F6C6551}"/>
+  <xr:revisionPtr revIDLastSave="743" documentId="8_{9E989A0F-969E-4ED2-9560-FEB0541538CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65A7A794-4174-4C03-83D4-02EDEC4234F8}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -91,6 +91,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="L27" authorId="0" shapeId="0" xr:uid="{134DA49D-E84E-4882-A21A-C0FA2F9A36E6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+50k Bikas da
+11270 extra ply
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="M27" authorId="0" shapeId="0" xr:uid="{F8374CFC-2A6A-41D3-A4EE-2F8672A0B170}">
       <text>
         <r>
@@ -113,7 +139,8 @@
           <t xml:space="preserve">
 Jacky - 24k
 Toughened Glass - 16k
-Sandeep da - 10k</t>
+Sandeep da - 10k
+6k - Sahid da</t>
         </r>
       </text>
     </comment>
@@ -585,6 +612,32 @@
         </r>
       </text>
     </comment>
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+additional ply :
+6 - 12 mm -7  X 4
+1 - 6mm - 7 X 4</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -786,12 +839,40 @@
         </r>
       </text>
     </comment>
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{795FE048-63B4-4A28-BEA6-9ED2DFB591E9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+4k extra tiles
+2k remaining kitchen renovation extra
+Sahid:
+Total Kitchn and bathroomc omplete - 1.02L
+Tiles 27.5K</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="103">
   <si>
     <t>Provider</t>
   </si>
@@ -1091,13 +1172,22 @@
   </si>
   <si>
     <t>Self Consumed</t>
+  </si>
+  <si>
+    <t>Payment - 10</t>
+  </si>
+  <si>
+    <t>Payment - 11</t>
+  </si>
+  <si>
+    <t>Payment - 12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1124,6 +1214,12 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="17">
@@ -1715,6 +1811,10 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person43.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/persons/person5.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -2035,7 +2135,7 @@
   <dimension ref="C7:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="P27" activeCellId="1" sqref="I17 P27"/>
+      <selection activeCell="H17" sqref="H17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2214,22 +2314,22 @@
       </c>
       <c r="F14">
         <f>Furniture!F16</f>
-        <v>487000</v>
+        <v>488270</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F17:F24)</f>
-        <v>252500</v>
+        <f>SUM(Furniture!F17:F27)</f>
+        <v>263770</v>
       </c>
       <c r="H14">
         <v>26500</v>
       </c>
       <c r="I14">
         <f>SUM(L25:L27)</f>
-        <v>226000</v>
+        <v>237270</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>234500</v>
+        <v>224500</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.3">
@@ -2244,19 +2344,19 @@
         <v>294300</v>
       </c>
       <c r="G15">
-        <f>SUM('Bathroom &amp; Kitchen'!F18:F25)</f>
-        <v>221300</v>
+        <f>SUM('Bathroom &amp; Kitchen'!F18:F27)</f>
+        <v>227300</v>
       </c>
       <c r="H15">
         <v>129000</v>
       </c>
       <c r="I15">
         <f>SUM(M25:M27)</f>
-        <v>92300</v>
+        <v>98300</v>
       </c>
       <c r="J15" s="4">
         <f t="shared" si="0"/>
-        <v>73000</v>
+        <v>67000</v>
       </c>
     </row>
     <row r="16" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2293,11 +2393,11 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1569650</v>
+        <v>1570920</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1199150</v>
+        <v>1216420</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
@@ -2305,11 +2405,11 @@
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>924315</v>
+        <v>941585</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="0"/>
-        <v>370500</v>
+        <v>354500</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.3">
@@ -2335,7 +2435,7 @@
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>81815</v>
+        <v>83085</v>
       </c>
     </row>
     <row r="23" spans="3:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2507,23 +2607,23 @@
       <c r="J27" s="40">
         <v>40505</v>
       </c>
-      <c r="K27" s="28">
+      <c r="K27" s="40">
         <v>15000</v>
       </c>
       <c r="L27" s="40">
-        <v>50000</v>
+        <v>61270</v>
       </c>
       <c r="M27" s="40">
-        <v>50000</v>
+        <v>56000</v>
       </c>
       <c r="N27" s="28"/>
       <c r="O27" s="28">
         <f>SUM(G27:N27)</f>
-        <v>185505</v>
+        <v>202775</v>
       </c>
       <c r="P27" s="28">
         <f t="shared" si="1"/>
-        <v>205685</v>
+        <v>188415</v>
       </c>
     </row>
   </sheetData>
@@ -2537,7 +2637,7 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD019853-AAD7-4C4A-AE9D-387A8C77D1D3}">
-  <dimension ref="D7:G26"/>
+  <dimension ref="D7:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
@@ -2739,31 +2839,54 @@
       <c r="F24" s="41">
         <v>50000</v>
       </c>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="G24" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D25" s="55"/>
       <c r="E25" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="56"/>
-      <c r="E26" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="41">
+        <v>6000</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="55"/>
+      <c r="E26" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="55"/>
+      <c r="E27" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="12"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="56"/>
+      <c r="E28" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F26" s="14">
-        <f>F17-SUM(F18:F25)</f>
-        <v>73000</v>
-      </c>
-      <c r="G26" s="21"/>
+      <c r="F28" s="14">
+        <f>F17-SUM(F18:F27)</f>
+        <v>67000</v>
+      </c>
+      <c r="G28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D26"/>
+    <mergeCell ref="D9:D28"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3556,7 +3679,7 @@
   <dimension ref="D7:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3873,10 +3996,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:G25"/>
+  <dimension ref="D7:G28"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3966,7 +4089,7 @@
         <v>86</v>
       </c>
       <c r="F15" s="12">
-        <v>10000</v>
+        <v>11270</v>
       </c>
       <c r="G15" s="20"/>
     </row>
@@ -3977,7 +4100,7 @@
       </c>
       <c r="F16" s="14">
         <f>SUM(F9:F15)</f>
-        <v>487000</v>
+        <v>488270</v>
       </c>
       <c r="G16" s="20"/>
     </row>
@@ -4065,33 +4188,62 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="58"/>
       <c r="E24" s="19" t="s">
         <v>80</v>
       </c>
-      <c r="F24" s="12">
-        <v>0</v>
+      <c r="F24" s="41">
+        <v>11270</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D25" s="59"/>
-      <c r="E25" s="1" t="s">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="58"/>
+      <c r="E25" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" s="41"/>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="58"/>
+      <c r="E26" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D27" s="58"/>
+      <c r="E27" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="F27" s="12">
+        <v>0</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D28" s="59"/>
+      <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F25" s="14">
-        <f>F16-SUM(F17:F24)</f>
-        <v>234500</v>
-      </c>
-      <c r="G25" s="21"/>
+      <c r="F28" s="14">
+        <f>F16-SUM(F17:F27)</f>
+        <v>224500</v>
+      </c>
+      <c r="G28" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D25"/>
+    <mergeCell ref="D9:D28"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Changes made on 04-11-2023
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="743" documentId="8_{9E989A0F-969E-4ED2-9560-FEB0541538CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65A7A794-4174-4C03-83D4-02EDEC4234F8}"/>
+  <xr:revisionPtr revIDLastSave="809" documentId="8_{9E989A0F-969E-4ED2-9560-FEB0541538CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{294157D9-35CF-464E-9E9B-4CD7D3CA97A3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -87,7 +87,8 @@
           <t xml:space="preserve">
 Switchboard &amp; all -31700
 chanchal - 5k
-Chanchal extra - 3805(Electrical including - Profile casing)</t>
+Chanchal extra - 3805(Electrical including - Profile casing)
+5454- Electric World 2nd lot lights and switch boards</t>
         </r>
       </text>
     </comment>
@@ -113,7 +114,8 @@
           <t xml:space="preserve">
 50k Bikas da
 11270 extra ply
-</t>
+21725 Extra materials 2nd payment
+44325 - Laminates1st payment</t>
         </r>
       </text>
     </comment>
@@ -188,7 +190,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
       <text>
         <r>
           <rPr>
@@ -213,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
       <text>
         <r>
           <rPr>
@@ -238,7 +240,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
       <text>
         <r>
           <rPr>
@@ -262,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
       <text>
         <r>
           <rPr>
@@ -286,7 +288,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
       <text>
         <r>
           <rPr>
@@ -310,7 +312,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
       <text>
         <r>
           <rPr>
@@ -334,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
       <text>
         <r>
           <rPr>
@@ -358,7 +360,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
       <text>
         <r>
           <rPr>
@@ -379,6 +381,30 @@
           </rPr>
           <t xml:space="preserve">
 Hanging Lights</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Electric world for second lot light and electric boards</t>
         </r>
       </text>
     </comment>
@@ -416,7 +442,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{3D8C32C3-C87D-4F9C-B839-E9E4ABFE74A7}">
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{1728EA6E-B823-4E8B-AD10-CFF18DA70F4F}">
       <text>
         <r>
           <rPr>
@@ -436,7 +462,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Tentative</t>
+1800 delivery charge
+</t>
         </r>
       </text>
     </comment>
@@ -635,6 +662,54 @@
 additional ply :
 6 - 12 mm -7  X 4
 1 - 6mm - 7 X 4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Extra set materials</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+laminates 1s payment</t>
         </r>
       </text>
     </comment>
@@ -872,7 +947,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="110">
   <si>
     <t>Provider</t>
   </si>
@@ -1096,9 +1171,6 @@
     <t>5w light - 40 - 255</t>
   </si>
   <si>
-    <t>3w light - 40 - 140</t>
-  </si>
-  <si>
     <t>10w light - 2 - 355</t>
   </si>
   <si>
@@ -1144,9 +1216,6 @@
     <t>Profiles - 25 mm - 16 - 115 each (200 extra gari vara)</t>
   </si>
   <si>
-    <t>Profiles - 12 mm - 10  - 120 each (200 extra gari vara)</t>
-  </si>
-  <si>
     <t>Drivers - 13- 440 -(10 ampere smps)</t>
   </si>
   <si>
@@ -1181,6 +1250,33 @@
   </si>
   <si>
     <t>Payment - 12</t>
+  </si>
+  <si>
+    <t>Payment - 13</t>
+  </si>
+  <si>
+    <t>Payment - 14</t>
+  </si>
+  <si>
+    <t>Payment -3</t>
+  </si>
+  <si>
+    <t>Payment -4</t>
+  </si>
+  <si>
+    <t>Payment -5</t>
+  </si>
+  <si>
+    <t>5w light - 3 - 240</t>
+  </si>
+  <si>
+    <t>3w light - 47 - 140</t>
+  </si>
+  <si>
+    <t>2w light - 9 -100</t>
+  </si>
+  <si>
+    <t>Driver - 5 - 120 (2 ampere smps)</t>
   </si>
 </sst>
 </file>
@@ -1505,7 +1601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1638,6 +1734,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1812,6 +1911,22 @@
 </file>
 
 <file path=xl/persons/person43.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person44.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person45.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person46.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person47.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2135,7 +2250,7 @@
   <dimension ref="C7:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:I17"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2212,19 +2327,19 @@
         <v>65000</v>
       </c>
       <c r="G10">
-        <f>SUM(Paint!F11:F13)</f>
-        <v>21000</v>
+        <f>SUM(Paint!F11:F15)</f>
+        <v>36000</v>
       </c>
       <c r="H10">
         <v>6000</v>
       </c>
       <c r="I10">
         <f>SUM(H25:H27)</f>
-        <v>15000</v>
+        <v>30000</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="0"/>
-        <v>44000</v>
+        <v>29000</v>
       </c>
     </row>
     <row r="11" spans="4:10" x14ac:dyDescent="0.3">
@@ -2259,11 +2374,11 @@
         <v>29</v>
       </c>
       <c r="F12">
-        <f>'Electric &amp; Lights'!F24</f>
-        <v>135571</v>
+        <f>'Electric &amp; Lights'!F26</f>
+        <v>141025</v>
       </c>
       <c r="G12">
-        <f>SUM('Electric &amp; Lights'!F25:F32)</f>
+        <f>SUM('Electric &amp; Lights'!F27:F34)</f>
         <v>130571</v>
       </c>
       <c r="H12">
@@ -2271,11 +2386,11 @@
       </c>
       <c r="I12">
         <f>SUM(J25:J27)</f>
-        <v>98876</v>
+        <v>104330</v>
       </c>
       <c r="J12" s="4">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>10454</v>
       </c>
     </row>
     <row r="13" spans="4:10" x14ac:dyDescent="0.3">
@@ -2314,22 +2429,22 @@
       </c>
       <c r="F14">
         <f>Furniture!F16</f>
-        <v>488270</v>
+        <v>488720</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F17:F27)</f>
-        <v>263770</v>
+        <f>SUM(Furniture!F17:F29)</f>
+        <v>329820</v>
       </c>
       <c r="H14">
         <v>26500</v>
       </c>
       <c r="I14">
         <f>SUM(L25:L27)</f>
-        <v>237270</v>
+        <v>303320</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>224500</v>
+        <v>158900</v>
       </c>
     </row>
     <row r="15" spans="4:10" x14ac:dyDescent="0.3">
@@ -2337,7 +2452,7 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F15">
         <f>'Bathroom &amp; Kitchen'!F17</f>
@@ -2393,11 +2508,11 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1570920</v>
+        <v>1576824</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1216420</v>
+        <v>1297470</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
@@ -2405,11 +2520,11 @@
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>941585</v>
+        <v>1028089</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="0"/>
-        <v>354500</v>
+        <v>279354</v>
       </c>
     </row>
     <row r="18" spans="3:16" x14ac:dyDescent="0.3">
@@ -2435,7 +2550,7 @@
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>83085</v>
+        <v>88989</v>
       </c>
     </row>
     <row r="23" spans="3:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -2600,18 +2715,20 @@
         <v>45216</v>
       </c>
       <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
+      <c r="H27" s="40">
+        <v>15000</v>
+      </c>
       <c r="I27" s="40">
         <v>30000</v>
       </c>
       <c r="J27" s="40">
-        <v>40505</v>
+        <v>45959</v>
       </c>
       <c r="K27" s="40">
         <v>15000</v>
       </c>
       <c r="L27" s="40">
-        <v>61270</v>
+        <v>127320</v>
       </c>
       <c r="M27" s="40">
         <v>56000</v>
@@ -2619,11 +2736,11 @@
       <c r="N27" s="28"/>
       <c r="O27" s="28">
         <f>SUM(G27:N27)</f>
-        <v>202775</v>
+        <v>289279</v>
       </c>
       <c r="P27" s="28">
         <f t="shared" si="1"/>
-        <v>188415</v>
+        <v>101911</v>
       </c>
     </row>
   </sheetData>
@@ -2701,7 +2818,7 @@
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="55"/>
       <c r="E12" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F12" s="32">
         <v>92300</v>
@@ -2711,7 +2828,7 @@
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="55"/>
       <c r="E13" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F13" s="32">
         <v>12000</v>
@@ -2721,7 +2838,7 @@
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="55"/>
       <c r="E14" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F14" s="32">
         <v>20000</v>
@@ -2731,7 +2848,7 @@
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="55"/>
       <c r="E15" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F15" s="32">
         <v>5500</v>
@@ -2834,7 +2951,7 @@
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="55"/>
       <c r="E24" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F24" s="41">
         <v>50000</v>
@@ -2846,7 +2963,7 @@
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D25" s="55"/>
       <c r="E25" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" s="41">
         <v>6000</v>
@@ -2858,7 +2975,7 @@
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D26" s="55"/>
       <c r="E26" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F26" s="41"/>
       <c r="G26" s="20"/>
@@ -2866,7 +2983,7 @@
     <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D27" s="55"/>
       <c r="E27" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F27" s="12"/>
       <c r="G27" s="20"/>
@@ -2959,7 +3076,7 @@
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="F12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G12">
         <v>5500</v>
@@ -2967,7 +3084,7 @@
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="F13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G13">
         <v>155</v>
@@ -3028,7 +3145,7 @@
   <dimension ref="D7:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3146,10 +3263,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5512692-EDEE-4A22-9F00-43BA354170EF}">
-  <dimension ref="D7:G14"/>
+  <dimension ref="D7:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3222,33 +3339,54 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="55"/>
       <c r="E13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="12">
-        <v>0</v>
+        <v>103</v>
+      </c>
+      <c r="F13" s="41">
+        <v>15000</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="56"/>
-      <c r="E14" s="13" t="s">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="55"/>
+      <c r="E14" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F14" s="41"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="55"/>
+      <c r="E15" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D16" s="56"/>
+      <c r="E16" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="14">
-        <f>F10-SUM(F11:F13)</f>
-        <v>44000</v>
-      </c>
-      <c r="G14" s="21"/>
+      <c r="F16" s="14">
+        <f>F10-SUM(F11:F15)</f>
+        <v>29000</v>
+      </c>
+      <c r="G16" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="D9:D16"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3365,10 +3503,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1544B4-216C-4DA0-B248-9403EAEF3872}">
-  <dimension ref="D7:G34"/>
+  <dimension ref="D7:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3408,11 +3546,11 @@
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="55"/>
-      <c r="E10" t="s">
-        <v>75</v>
-      </c>
-      <c r="F10" s="4">
-        <v>710</v>
+      <c r="E10" s="60" t="s">
+        <v>106</v>
+      </c>
+      <c r="F10" s="12">
+        <v>720</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -3422,64 +3560,68 @@
         <v>74</v>
       </c>
       <c r="F11" s="4">
-        <v>5600</v>
+        <v>710</v>
       </c>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="55"/>
       <c r="E12" t="s">
-        <v>76</v>
+        <v>107</v>
       </c>
       <c r="F12" s="4">
-        <v>870</v>
+        <v>6580</v>
       </c>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="55"/>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="F13" s="4">
-        <v>10240</v>
+        <v>900</v>
       </c>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="55"/>
       <c r="E14" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="F14" s="4">
-        <v>1680</v>
+        <v>870</v>
       </c>
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="55"/>
       <c r="E15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F15" s="4">
-        <v>2040</v>
+        <v>10240</v>
       </c>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D16" s="55"/>
       <c r="E16" t="s">
-        <v>90</v>
-      </c>
-      <c r="F16" s="4"/>
+        <v>86</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1680</v>
+      </c>
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="55"/>
       <c r="E17" t="s">
-        <v>94</v>
-      </c>
-      <c r="F17" s="4"/>
+        <v>88</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2040</v>
+      </c>
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
@@ -3487,115 +3629,109 @@
       <c r="E18" t="s">
         <v>92</v>
       </c>
-      <c r="F18" s="4">
-        <v>2940</v>
-      </c>
+      <c r="F18" s="4"/>
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="55"/>
       <c r="E19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F19" s="4">
-        <v>5720</v>
+        <v>2940</v>
       </c>
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="55"/>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>89</v>
       </c>
       <c r="F20" s="4">
-        <v>25721</v>
+        <v>5720</v>
       </c>
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D21" s="55"/>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>109</v>
       </c>
       <c r="F21" s="4">
-        <v>29500</v>
+        <v>600</v>
       </c>
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D22" s="55"/>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>71</v>
       </c>
       <c r="F22" s="4">
-        <v>25000</v>
+        <v>25721</v>
       </c>
       <c r="G22" s="20"/>
     </row>
-    <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D23" s="55"/>
       <c r="E23" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="F23" s="4">
-        <v>15350</v>
+        <v>31754</v>
       </c>
       <c r="G23" s="20"/>
     </row>
-    <row r="24" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="55"/>
-      <c r="E24" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" s="3">
-        <f>SUM(F9:F23)</f>
-        <v>135571</v>
+      <c r="E24" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="4">
+        <v>25000</v>
       </c>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D25" s="55"/>
       <c r="E25" t="s">
-        <v>32</v>
-      </c>
-      <c r="F25" s="41">
-        <v>16345</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+        <v>91</v>
+      </c>
+      <c r="F25" s="4">
+        <v>15350</v>
+      </c>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="55"/>
-      <c r="E26" t="s">
-        <v>34</v>
-      </c>
-      <c r="F26" s="41">
-        <v>11088</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>36</v>
-      </c>
+      <c r="E26" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="3">
+        <f>SUM(F9:F25)</f>
+        <v>141025</v>
+      </c>
+      <c r="G26" s="20"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D27" s="55"/>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" s="41">
-        <v>4100</v>
+        <v>16345</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D28" s="55"/>
       <c r="E28" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F28" s="41">
-        <v>6903</v>
+        <v>11088</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>36</v>
@@ -3604,10 +3740,10 @@
     <row r="29" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D29" s="55"/>
       <c r="E29" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
       <c r="F29" s="41">
-        <v>36280</v>
+        <v>4100</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>36</v>
@@ -3616,10 +3752,10 @@
     <row r="30" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D30" s="55"/>
       <c r="E30" t="s">
-        <v>70</v>
+        <v>35</v>
       </c>
       <c r="F30" s="41">
-        <v>8805</v>
+        <v>6903</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>36</v>
@@ -3628,10 +3764,10 @@
     <row r="31" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D31" s="55"/>
       <c r="E31" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="F31" s="41">
-        <v>31700</v>
+        <v>36280</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>36</v>
@@ -3640,35 +3776,75 @@
     <row r="32" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D32" s="55"/>
       <c r="E32" t="s">
+        <v>70</v>
+      </c>
+      <c r="F32" s="41">
+        <v>8805</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D33" s="55"/>
+      <c r="E33" t="s">
+        <v>76</v>
+      </c>
+      <c r="F33" s="41">
+        <v>31700</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="55"/>
+      <c r="E34" t="s">
+        <v>78</v>
+      </c>
+      <c r="F34" s="41">
+        <v>15350</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="55"/>
+      <c r="E35" t="s">
         <v>79</v>
       </c>
-      <c r="F32" s="41">
-        <v>15350</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="55"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="56"/>
-      <c r="E34" s="1" t="s">
+      <c r="F35" s="41">
+        <v>5454</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="55"/>
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" s="4"/>
+      <c r="G36" s="20"/>
+    </row>
+    <row r="37" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D37" s="56"/>
+      <c r="E37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="3">
-        <f>F24-SUM(F25:F32)</f>
+      <c r="F37" s="3">
+        <f>F26-SUM(F27:F36)</f>
         <v>5000</v>
       </c>
-      <c r="G34" s="21"/>
+      <c r="G37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D34"/>
+    <mergeCell ref="D9:D37"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -3996,10 +4172,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:G28"/>
+  <dimension ref="D7:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4030,7 +4206,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F9" s="10">
         <v>157000</v>
@@ -4040,10 +4216,10 @@
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="58"/>
       <c r="E10" s="19" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F10" s="12">
-        <v>100000</v>
+        <v>90450</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -4053,14 +4229,14 @@
         <v>22</v>
       </c>
       <c r="F11" s="12">
-        <v>40000</v>
+        <v>50000</v>
       </c>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="58"/>
       <c r="E12" s="19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F12" s="12"/>
       <c r="G12" s="20"/>
@@ -4068,7 +4244,7 @@
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="58"/>
       <c r="E13" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F13" s="12"/>
       <c r="G13" s="20"/>
@@ -4086,7 +4262,7 @@
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="58"/>
       <c r="E15" s="19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F15" s="12">
         <v>11270</v>
@@ -4100,7 +4276,7 @@
       </c>
       <c r="F16" s="14">
         <f>SUM(F9:F15)</f>
-        <v>488270</v>
+        <v>488720</v>
       </c>
       <c r="G16" s="20"/>
     </row>
@@ -4149,7 +4325,7 @@
         <v>14000</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
@@ -4167,7 +4343,7 @@
     <row r="22" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D22" s="58"/>
       <c r="E22" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F22" s="41">
         <v>27000</v>
@@ -4179,7 +4355,7 @@
     <row r="23" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D23" s="58"/>
       <c r="E23" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F23" s="41">
         <v>50000</v>
@@ -4191,7 +4367,7 @@
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="58"/>
       <c r="E24" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F24" s="41">
         <v>11270</v>
@@ -4203,45 +4379,69 @@
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D25" s="58"/>
       <c r="E25" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="F25" s="41"/>
-      <c r="G25" s="20"/>
+        <v>98</v>
+      </c>
+      <c r="F25" s="41">
+        <v>21725</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D26" s="58"/>
       <c r="E26" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="41"/>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="F26" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D27" s="58"/>
       <c r="E27" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="58"/>
+      <c r="E28" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="F28" s="41"/>
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="58"/>
+      <c r="E29" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="F27" s="12">
+      <c r="F29" s="12">
         <v>0</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D28" s="59"/>
-      <c r="E28" s="1" t="s">
+    <row r="30" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="59"/>
+      <c r="E30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="14">
-        <f>F16-SUM(F17:F27)</f>
-        <v>224500</v>
-      </c>
-      <c r="G28" s="21"/>
+      <c r="F30" s="14">
+        <f>F16-SUM(F17:F29)</f>
+        <v>158900</v>
+      </c>
+      <c r="G30" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D28"/>
+    <mergeCell ref="D9:D30"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated 18 11 2023
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranen\OneDrive\Documents\Sounak\InterioWorkSounak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="912" documentId="8_{9E989A0F-969E-4ED2-9560-FEB0541538CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C7A29E58-D354-454C-AE23-24FE1B51B8E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE82297B-F648-4E26-98EB-A6EF2D5157B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Furniture" sheetId="6" r:id="rId9"/>
     <sheet name="Bathroom &amp; Kitchen" sheetId="7" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +120,8 @@
 44325 - Laminates1st payment
 21560 - Additional Ply 2nd lot
 7250 - Glue and screws
-18600 - 3600 locks and 15000 vikas da</t>
+18600 - 3600 locks and 15000 vikas da
+44325 - Laminates final Payment</t>
         </r>
       </text>
     </comment>
@@ -470,6 +471,7 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>sounak nandi</author>
+    <author>Ranendu Banerjee</author>
   </authors>
   <commentList>
     <comment ref="F9" authorId="0" shapeId="0" xr:uid="{95673EC6-1FAC-4D13-B2E1-7144010F49A5}">
@@ -861,6 +863,54 @@
           </rPr>
           <t xml:space="preserve">
 3600 for locks and 15000 Bikas da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ranendu Banerjee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Remaining Laminates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Ranendu Banerjee:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Delivery o flaminates</t>
         </r>
       </text>
     </comment>
@@ -1122,7 +1172,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
   <si>
     <t>Provider</t>
   </si>
@@ -1479,6 +1529,12 @@
   </si>
   <si>
     <t>Lights &amp; Electricals</t>
+  </si>
+  <si>
+    <t>Self - Sri</t>
+  </si>
+  <si>
+    <t>Bank(3717) Self(1283)</t>
   </si>
 </sst>
 </file>
@@ -2610,23 +2666,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
   <dimension ref="C7:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B8" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="16.44140625" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
-    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1"/>
-    <col min="15" max="15" width="9.21875" customWidth="1"/>
-    <col min="16" max="16" width="10.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5703125" customWidth="1"/>
+    <col min="15" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:10" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:10" ht="79.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="22" t="s">
         <v>25</v>
       </c>
@@ -2649,7 +2705,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D9" s="5">
         <v>1</v>
       </c>
@@ -2676,7 +2732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D10" s="5">
         <v>2</v>
       </c>
@@ -2689,21 +2745,21 @@
       </c>
       <c r="G10">
         <f>SUM(Paint!F11:F15)</f>
-        <v>36000</v>
+        <v>41000</v>
       </c>
       <c r="H10">
-        <v>6000</v>
+        <v>7283</v>
       </c>
       <c r="I10">
         <f>SUM(H25:H27)</f>
-        <v>30000</v>
+        <v>33717</v>
       </c>
       <c r="J10" s="4">
         <f t="shared" si="0"/>
-        <v>29000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+        <v>24000</v>
+      </c>
+    </row>
+    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D11" s="5">
         <v>3</v>
       </c>
@@ -2727,7 +2783,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D12" s="5">
         <v>4</v>
       </c>
@@ -2754,7 +2810,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D13" s="5">
         <v>5</v>
       </c>
@@ -2781,7 +2837,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D14" s="5">
         <v>6</v>
       </c>
@@ -2794,21 +2850,21 @@
       </c>
       <c r="G14">
         <f>SUM(Furniture!F18:F34)</f>
-        <v>377230</v>
+        <v>423355</v>
       </c>
       <c r="H14">
-        <v>26500</v>
+        <v>28300</v>
       </c>
       <c r="I14">
         <f>SUM(L25:L27)</f>
-        <v>350730</v>
+        <v>395055</v>
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>158500</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+        <v>112375</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D15" s="5">
         <v>7</v>
       </c>
@@ -2835,7 +2891,7 @@
         <v>67000</v>
       </c>
     </row>
-    <row r="16" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="5">
         <v>8</v>
       </c>
@@ -2862,7 +2918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="1"/>
       <c r="E17" s="27" t="s">
         <v>6</v>
@@ -2873,22 +2929,22 @@
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1356793</v>
+        <v>1407918</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>274835</v>
+        <v>277918</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>1081958</v>
+        <v>1130000</v>
       </c>
       <c r="J17" s="3">
         <f t="shared" si="0"/>
-        <v>285500</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+        <v>234375</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E18" s="29" t="s">
         <v>36</v>
       </c>
@@ -2896,25 +2952,25 @@
         <v>1213000</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E19" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F19" s="28">
         <f>H17</f>
-        <v>274835</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+        <v>277918</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
       <c r="E20" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>154458</v>
-      </c>
-    </row>
-    <row r="23" spans="3:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>151375</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C23" s="56" t="s">
         <v>45</v>
       </c>
@@ -2932,7 +2988,7 @@
       <c r="O23" s="56"/>
       <c r="P23" s="56"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C24" s="33" t="s">
         <v>46</v>
       </c>
@@ -2976,7 +3032,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C25" s="28">
         <v>1</v>
       </c>
@@ -3016,7 +3072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C26" s="28">
         <v>2</v>
       </c>
@@ -3061,7 +3117,7 @@
         <v>61190</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
       <c r="C27" s="28">
         <v>3</v>
       </c>
@@ -3077,7 +3133,7 @@
       </c>
       <c r="G27" s="28"/>
       <c r="H27" s="40">
-        <v>15000</v>
+        <v>18717</v>
       </c>
       <c r="I27" s="40">
         <v>30000</v>
@@ -3089,7 +3145,7 @@
         <v>15000</v>
       </c>
       <c r="L27" s="40">
-        <v>174730</v>
+        <v>219055</v>
       </c>
       <c r="M27" s="40">
         <v>57600</v>
@@ -3097,11 +3153,11 @@
       <c r="N27" s="28"/>
       <c r="O27" s="28">
         <f>SUM(G27:N27)</f>
-        <v>343148</v>
+        <v>391190</v>
       </c>
       <c r="P27" s="28">
         <f t="shared" si="1"/>
-        <v>48042</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3121,16 +3177,16 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -3144,7 +3200,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="64" t="s">
         <v>62</v>
       </c>
@@ -3156,7 +3212,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="65"/>
       <c r="E10" s="11" t="s">
         <v>24</v>
@@ -3166,7 +3222,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>67</v>
@@ -3176,7 +3232,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>80</v>
@@ -3186,7 +3242,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>81</v>
@@ -3196,7 +3252,7 @@
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>84</v>
@@ -3206,7 +3262,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
         <v>83</v>
@@ -3216,7 +3272,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>20</v>
@@ -3226,7 +3282,7 @@
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="65"/>
       <c r="E17" s="13" t="s">
         <v>6</v>
@@ -3237,7 +3293,7 @@
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="65"/>
       <c r="E18" s="11" t="s">
         <v>32</v>
@@ -3249,7 +3305,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="65"/>
       <c r="E19" s="11" t="s">
         <v>34</v>
@@ -3261,7 +3317,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="65"/>
       <c r="E20" s="11" t="s">
         <v>33</v>
@@ -3273,7 +3329,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="65"/>
       <c r="E21" s="11" t="s">
         <v>35</v>
@@ -3285,7 +3341,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="65"/>
       <c r="E22" s="11" t="s">
         <v>69</v>
@@ -3297,7 +3353,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="65"/>
       <c r="E23" s="11" t="s">
         <v>70</v>
@@ -3309,7 +3365,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="65"/>
       <c r="E24" s="11" t="s">
         <v>76</v>
@@ -3321,7 +3377,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="65"/>
       <c r="E25" s="11" t="s">
         <v>78</v>
@@ -3333,7 +3389,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="65"/>
       <c r="E26" s="11" t="s">
         <v>79</v>
@@ -3345,7 +3401,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="65"/>
       <c r="E27" s="11" t="s">
         <v>98</v>
@@ -3353,7 +3409,7 @@
       <c r="F27" s="41"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="65"/>
       <c r="E28" s="11" t="s">
         <v>99</v>
@@ -3361,7 +3417,7 @@
       <c r="F28" s="41"/>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D29" s="65"/>
       <c r="E29" s="11" t="s">
         <v>100</v>
@@ -3369,7 +3425,7 @@
       <c r="F29" s="12"/>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D30" s="66"/>
       <c r="E30" s="13" t="s">
         <v>13</v>
@@ -3398,14 +3454,14 @@
       <selection activeCell="D19" sqref="D19:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" s="61" t="s">
         <v>54</v>
       </c>
@@ -3413,7 +3469,7 @@
       <c r="F7" s="62"/>
       <c r="G7" s="63"/>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D8" s="57" t="s">
         <v>55</v>
       </c>
@@ -3427,7 +3483,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="58"/>
       <c r="E9" s="60"/>
       <c r="F9" s="28" t="s">
@@ -3437,7 +3493,7 @@
         <v>12300</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="58"/>
       <c r="E10" s="60"/>
       <c r="F10" s="47" t="s">
@@ -3447,7 +3503,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="51"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
@@ -3457,7 +3513,7 @@
         <v>16345</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="51"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28" t="s">
@@ -3467,7 +3523,7 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="51"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28" t="s">
@@ -3477,7 +3533,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="52"/>
       <c r="E14" s="53"/>
       <c r="F14" s="53" t="s">
@@ -3488,8 +3544,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="55" t="s">
         <v>66</v>
       </c>
@@ -3503,7 +3559,7 @@
         <v>23500</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="51"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
@@ -3513,19 +3569,19 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="51"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="50"/>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="51"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D23" s="52"/>
       <c r="E23" s="53"/>
       <c r="F23" s="53" t="s">
@@ -3554,17 +3610,17 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="23.109375" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -3578,7 +3634,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="64" t="s">
         <v>2</v>
       </c>
@@ -3590,7 +3646,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" t="s">
         <v>4</v>
@@ -3600,7 +3656,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" s="1" t="s">
         <v>6</v>
@@ -3611,7 +3667,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="65"/>
       <c r="E12" t="s">
         <v>7</v>
@@ -3623,7 +3679,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="65"/>
       <c r="E13" t="s">
         <v>8</v>
@@ -3635,7 +3691,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="65"/>
       <c r="E14" t="s">
         <v>9</v>
@@ -3647,7 +3703,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="66"/>
       <c r="E15" s="1" t="s">
         <v>10</v>
@@ -3672,19 +3728,19 @@
   <dimension ref="D7:G16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.21875" customWidth="1"/>
-    <col min="5" max="5" width="27.21875" customWidth="1"/>
-    <col min="6" max="6" width="31.5546875" customWidth="1"/>
-    <col min="7" max="7" width="32.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="27.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.5703125" customWidth="1"/>
+    <col min="7" max="7" width="32.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="58.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -3698,7 +3754,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
         <v>11</v>
       </c>
@@ -3710,7 +3766,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
@@ -3721,7 +3777,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>32</v>
@@ -3733,7 +3789,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>31</v>
@@ -3745,7 +3801,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>103</v>
@@ -3757,15 +3813,19 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="41"/>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="41">
+        <v>5000</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
         <v>105</v>
@@ -3777,14 +3837,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="66"/>
       <c r="E16" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F16" s="14">
         <f>F10-SUM(F11:F15)</f>
-        <v>29000</v>
+        <v>24000</v>
       </c>
       <c r="G16" s="21"/>
     </row>
@@ -3806,16 +3866,16 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="79.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="79.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -3829,7 +3889,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
         <v>15</v>
       </c>
@@ -3841,7 +3901,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
@@ -3852,7 +3912,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>32</v>
@@ -3864,7 +3924,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>34</v>
@@ -3876,7 +3936,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>33</v>
@@ -3888,7 +3948,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="66"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
@@ -3915,16 +3975,16 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="49.33203125" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="49.28515625" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="64.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="64.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -3938,7 +3998,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="64" t="s">
         <v>61</v>
       </c>
@@ -3950,7 +4010,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="65"/>
       <c r="E10" s="11" t="s">
         <v>106</v>
@@ -3960,7 +4020,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="65"/>
       <c r="E11" t="s">
         <v>74</v>
@@ -3970,7 +4030,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="65"/>
       <c r="E12" t="s">
         <v>107</v>
@@ -3980,7 +4040,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="65"/>
       <c r="E13" t="s">
         <v>108</v>
@@ -3990,7 +4050,7 @@
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="65"/>
       <c r="E14" t="s">
         <v>75</v>
@@ -4000,7 +4060,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" s="65"/>
       <c r="E15" t="s">
         <v>87</v>
@@ -4010,7 +4070,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D16" s="65"/>
       <c r="E16" t="s">
         <v>86</v>
@@ -4020,7 +4080,7 @@
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="65"/>
       <c r="E17" t="s">
         <v>88</v>
@@ -4030,7 +4090,7 @@
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="65"/>
       <c r="E18" t="s">
         <v>115</v>
@@ -4040,7 +4100,7 @@
       </c>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="65"/>
       <c r="E19" t="s">
         <v>92</v>
@@ -4048,7 +4108,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="65"/>
       <c r="E20" t="s">
         <v>90</v>
@@ -4058,7 +4118,7 @@
       </c>
       <c r="G20" s="20"/>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="65"/>
       <c r="E21" t="s">
         <v>89</v>
@@ -4068,7 +4128,7 @@
       </c>
       <c r="G21" s="20"/>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="65"/>
       <c r="E22" t="s">
         <v>109</v>
@@ -4078,7 +4138,7 @@
       </c>
       <c r="G22" s="20"/>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="65"/>
       <c r="E23" t="s">
         <v>71</v>
@@ -4088,7 +4148,7 @@
       </c>
       <c r="G23" s="20"/>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="65"/>
       <c r="E24" t="s">
         <v>72</v>
@@ -4098,7 +4158,7 @@
       </c>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="65"/>
       <c r="E25" t="s">
         <v>30</v>
@@ -4108,7 +4168,7 @@
       </c>
       <c r="G25" s="20"/>
     </row>
-    <row r="26" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D26" s="65"/>
       <c r="E26" t="s">
         <v>91</v>
@@ -4118,7 +4178,7 @@
       </c>
       <c r="G26" s="20"/>
     </row>
-    <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D27" s="65"/>
       <c r="E27" s="1" t="s">
         <v>6</v>
@@ -4129,7 +4189,7 @@
       </c>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="65"/>
       <c r="E28" t="s">
         <v>32</v>
@@ -4141,7 +4201,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="65"/>
       <c r="E29" t="s">
         <v>34</v>
@@ -4153,7 +4213,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" s="65"/>
       <c r="E30" t="s">
         <v>33</v>
@@ -4165,7 +4225,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="65"/>
       <c r="E31" t="s">
         <v>35</v>
@@ -4177,7 +4237,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="65"/>
       <c r="E32" t="s">
         <v>69</v>
@@ -4189,7 +4249,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="65"/>
       <c r="E33" t="s">
         <v>70</v>
@@ -4201,7 +4261,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="65"/>
       <c r="E34" t="s">
         <v>76</v>
@@ -4213,7 +4273,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D35" s="65"/>
       <c r="E35" t="s">
         <v>78</v>
@@ -4225,7 +4285,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D36" s="65"/>
       <c r="E36" t="s">
         <v>79</v>
@@ -4237,7 +4297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D37" s="65"/>
       <c r="E37" t="s">
         <v>98</v>
@@ -4249,7 +4309,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D38" s="65"/>
       <c r="E38" t="s">
         <v>99</v>
@@ -4261,7 +4321,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D39" s="65"/>
       <c r="E39" t="s">
         <v>100</v>
@@ -4269,7 +4329,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="20"/>
     </row>
-    <row r="40" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D40" s="66"/>
       <c r="E40" s="1" t="s">
         <v>10</v>
@@ -4298,16 +4358,16 @@
       <selection activeCell="F20" sqref="F16:F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="70.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -4321,7 +4381,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="64" t="s">
         <v>16</v>
       </c>
@@ -4333,7 +4393,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="65"/>
       <c r="E10" s="11" t="s">
         <v>19</v>
@@ -4343,7 +4403,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>18</v>
@@ -4353,7 +4413,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>44</v>
@@ -4363,7 +4423,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>110</v>
@@ -4373,7 +4433,7 @@
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>20</v>
@@ -4383,7 +4443,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D15" s="65"/>
       <c r="E15" s="13" t="s">
         <v>6</v>
@@ -4394,7 +4454,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>32</v>
@@ -4406,7 +4466,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D17" s="65"/>
       <c r="E17" s="11" t="s">
         <v>34</v>
@@ -4418,7 +4478,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="65"/>
       <c r="E18" s="11" t="s">
         <v>33</v>
@@ -4430,7 +4490,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="65"/>
       <c r="E19" s="11" t="s">
         <v>35</v>
@@ -4442,7 +4502,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="65"/>
       <c r="E20" s="11" t="s">
         <v>69</v>
@@ -4454,7 +4514,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D21" s="65"/>
       <c r="E21" s="11" t="s">
         <v>70</v>
@@ -4462,7 +4522,7 @@
       <c r="F21" s="43"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D22" s="66"/>
       <c r="E22" s="13" t="s">
         <v>13</v>
@@ -4489,16 +4549,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -4512,7 +4572,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="64" t="s">
         <v>111</v>
       </c>
@@ -4524,7 +4584,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" ht="30" x14ac:dyDescent="0.25">
       <c r="D10" s="65"/>
       <c r="E10" s="31" t="s">
         <v>43</v>
@@ -4534,7 +4594,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>28</v>
@@ -4542,7 +4602,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" s="13" t="s">
         <v>6</v>
@@ -4553,7 +4613,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>32</v>
@@ -4565,7 +4625,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>34</v>
@@ -4577,7 +4637,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
         <v>33</v>
@@ -4589,7 +4649,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>35</v>
@@ -4601,7 +4661,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="66"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
@@ -4624,20 +4684,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
   <dimension ref="D7:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F27" activeCellId="2" sqref="F32 F31 F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.21875" customWidth="1"/>
-    <col min="5" max="5" width="45.44140625" customWidth="1"/>
-    <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="5" max="5" width="45.42578125" customWidth="1"/>
+    <col min="6" max="6" width="32.85546875" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="4:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -4651,7 +4711,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D9" s="67" t="s">
         <v>21</v>
       </c>
@@ -4663,7 +4723,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D10" s="68"/>
       <c r="E10" s="19" t="s">
         <v>112</v>
@@ -4673,7 +4733,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D11" s="68"/>
       <c r="E11" s="19" t="s">
         <v>94</v>
@@ -4683,7 +4743,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D12" s="68"/>
       <c r="E12" s="19" t="s">
         <v>22</v>
@@ -4693,7 +4753,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D13" s="68"/>
       <c r="E13" s="19" t="s">
         <v>95</v>
@@ -4701,7 +4761,7 @@
       <c r="F13" s="12"/>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D14" s="68"/>
       <c r="E14" s="19" t="s">
         <v>96</v>
@@ -4709,7 +4769,7 @@
       <c r="F14" s="12"/>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D15" s="68"/>
       <c r="E15" s="19" t="s">
         <v>23</v>
@@ -4719,7 +4779,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D16" s="68"/>
       <c r="E16" s="19" t="s">
         <v>85</v>
@@ -4729,7 +4789,7 @@
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D17" s="68"/>
       <c r="E17" s="13" t="s">
         <v>6</v>
@@ -4740,7 +4800,7 @@
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D18" s="68"/>
       <c r="E18" s="19" t="s">
         <v>32</v>
@@ -4752,7 +4812,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D19" s="68"/>
       <c r="E19" s="19" t="s">
         <v>34</v>
@@ -4764,7 +4824,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D20" s="68"/>
       <c r="E20" s="19" t="s">
         <v>33</v>
@@ -4776,7 +4836,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D21" s="68"/>
       <c r="E21" s="19" t="s">
         <v>35</v>
@@ -4788,7 +4848,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D22" s="68"/>
       <c r="E22" s="19" t="s">
         <v>69</v>
@@ -4800,7 +4860,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D23" s="68"/>
       <c r="E23" s="19" t="s">
         <v>76</v>
@@ -4812,7 +4872,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D24" s="68"/>
       <c r="E24" s="19" t="s">
         <v>78</v>
@@ -4824,7 +4884,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D25" s="68"/>
       <c r="E25" s="19" t="s">
         <v>79</v>
@@ -4836,7 +4896,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D26" s="68"/>
       <c r="E26" s="19" t="s">
         <v>98</v>
@@ -4848,7 +4908,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D27" s="68"/>
       <c r="E27" s="19" t="s">
         <v>99</v>
@@ -4860,7 +4920,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D28" s="68"/>
       <c r="E28" s="19" t="s">
         <v>100</v>
@@ -4872,7 +4932,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D29" s="68"/>
       <c r="E29" s="19" t="s">
         <v>101</v>
@@ -4884,7 +4944,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D30" s="68"/>
       <c r="E30" s="19" t="s">
         <v>102</v>
@@ -4896,23 +4956,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D31" s="68"/>
       <c r="E31" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="F31" s="41"/>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="F31" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D32" s="68"/>
       <c r="E32" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F32" s="41"/>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="F32" s="41">
+        <v>1800</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D33" s="68"/>
       <c r="E33" s="19" t="s">
         <v>116</v>
@@ -4920,7 +4988,7 @@
       <c r="F33" s="41"/>
       <c r="G33" s="20"/>
     </row>
-    <row r="34" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D34" s="68"/>
       <c r="E34" s="19" t="s">
         <v>117</v>
@@ -4932,14 +5000,14 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D35" s="69"/>
       <c r="E35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="14">
         <f>F17-SUM(F18:F34)</f>
-        <v>158500</v>
+        <v>112375</v>
       </c>
       <c r="G35" s="21"/>
     </row>

</xml_diff>

<commit_message>
updated 18 11 2023 -2
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranen\OneDrive\Documents\Sounak\InterioWorkSounak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE82297B-F648-4E26-98EB-A6EF2D5157B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -518,7 +518,9 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-3 tubs 20kg</t>
+3 tubs 20kg
+5kg special glue
+</t>
         </r>
       </text>
     </comment>
@@ -1172,7 +1174,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="121">
   <si>
     <t>Provider</t>
   </si>
@@ -2666,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
   <dimension ref="C7:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C17" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:I10"/>
+    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2826,7 +2828,7 @@
         <v>89000</v>
       </c>
       <c r="H13">
-        <v>36300</v>
+        <v>38050</v>
       </c>
       <c r="I13">
         <f>SUM(K25:K27)</f>
@@ -2846,11 +2848,11 @@
       </c>
       <c r="F14">
         <f>Furniture!F17</f>
-        <v>535730</v>
+        <v>537480</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F18:F34)</f>
-        <v>423355</v>
+        <f>SUM(Furniture!F18:F36)</f>
+        <v>425105</v>
       </c>
       <c r="H14">
         <v>28300</v>
@@ -2925,15 +2927,15 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1642293</v>
+        <v>1644043</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1407918</v>
+        <v>1409668</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>277918</v>
+        <v>279668</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
@@ -2958,7 +2960,7 @@
       </c>
       <c r="F19" s="28">
         <f>H17</f>
-        <v>277918</v>
+        <v>279668</v>
       </c>
     </row>
     <row r="20" spans="3:16" x14ac:dyDescent="0.25">
@@ -4682,10 +4684,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:G35"/>
+  <dimension ref="D7:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F27" activeCellId="2" sqref="F32 F31 F27"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4729,7 +4731,7 @@
         <v>112</v>
       </c>
       <c r="F10" s="12">
-        <v>16450</v>
+        <v>18200</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -4796,7 +4798,7 @@
       </c>
       <c r="F17" s="14">
         <f>SUM(F9:F16)</f>
-        <v>535730</v>
+        <v>537480</v>
       </c>
       <c r="G17" s="20"/>
     </row>
@@ -4985,35 +4987,51 @@
       <c r="E33" s="19" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F33" s="41">
+        <v>1750</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
       <c r="D34" s="68"/>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="19"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="D35" s="68"/>
+      <c r="E35" s="19"/>
+      <c r="F35" s="41"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D36" s="68"/>
+      <c r="E36" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F34" s="12">
+      <c r="F36" s="12">
         <v>0</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D35" s="69"/>
-      <c r="E35" s="1" t="s">
+    <row r="37" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="69"/>
+      <c r="E37" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F35" s="14">
-        <f>F17-SUM(F18:F34)</f>
+      <c r="F37" s="14">
+        <f>F17-SUM(F18:F36)</f>
         <v>112375</v>
       </c>
-      <c r="G35" s="21"/>
+      <c r="G37" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D35"/>
+    <mergeCell ref="D9:D37"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated as of 25-11-2023
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranen\OneDrive\Documents\Sounak\InterioWorkSounak\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DFA8812-754A-418D-ADF0-839C1A1E88F0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Furniture" sheetId="6" r:id="rId9"/>
     <sheet name="Bathroom &amp; Kitchen" sheetId="7" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -574,7 +574,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{87678B8C-756B-4A16-A0B1-A3C2A9059184}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{87678B8C-756B-4A16-A0B1-A3C2A9059184}">
       <text>
         <r>
           <rPr>
@@ -599,7 +599,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
       <text>
         <r>
           <rPr>
@@ -623,7 +623,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
       <text>
         <r>
           <rPr>
@@ -647,7 +647,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
       <text>
         <r>
           <rPr>
@@ -672,7 +672,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
       <text>
         <r>
           <rPr>
@@ -697,7 +697,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
       <text>
         <r>
           <rPr>
@@ -722,7 +722,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
       <text>
         <r>
           <rPr>
@@ -748,7 +748,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
       <text>
         <r>
           <rPr>
@@ -772,7 +772,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
       <text>
         <r>
           <rPr>
@@ -796,7 +796,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
       <text>
         <r>
           <rPr>
@@ -820,7 +820,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
       <text>
         <r>
           <rPr>
@@ -844,7 +844,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
       <text>
         <r>
           <rPr>
@@ -868,7 +868,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+    <comment ref="F30" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
           <rPr>
@@ -892,7 +892,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
       <text>
         <r>
           <rPr>
@@ -913,6 +913,31 @@
           </rPr>
           <t xml:space="preserve">
 Delivery o flaminates</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Self 1600
+AIA - 5300</t>
         </r>
       </text>
     </comment>
@@ -1174,7 +1199,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="124">
   <si>
     <t>Provider</t>
   </si>
@@ -1461,12 +1486,6 @@
     <t>Raw Material - 2nd Lot - Laminates&amp;Louvers</t>
   </si>
   <si>
-    <t>Estimated Glass cost</t>
-  </si>
-  <si>
-    <t>Alumunium Cost</t>
-  </si>
-  <si>
     <t>Self Consumed</t>
   </si>
   <si>
@@ -1537,6 +1556,21 @@
   </si>
   <si>
     <t>Bank(3717) Self(1283)</t>
+  </si>
+  <si>
+    <t>Tata AIA - Sounak</t>
+  </si>
+  <si>
+    <t>Self(Self &amp; AIA)</t>
+  </si>
+  <si>
+    <t>Payment - 19</t>
+  </si>
+  <si>
+    <t>Payment - 20</t>
+  </si>
+  <si>
+    <t>Estimated Glass&amp; alumunium Frame</t>
   </si>
 </sst>
 </file>
@@ -2350,6 +2384,10 @@
 </file>
 
 <file path=xl/persons/person54.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person55.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2668,23 +2706,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
   <dimension ref="C7:P27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:I17"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5703125" customWidth="1"/>
-    <col min="15" max="15" width="9.28515625" customWidth="1"/>
-    <col min="16" max="16" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" customWidth="1"/>
+    <col min="15" max="15" width="9.33203125" customWidth="1"/>
+    <col min="16" max="16" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:10" ht="79.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:10" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="22" t="s">
         <v>25</v>
       </c>
@@ -2707,7 +2745,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D9" s="5">
         <v>1</v>
       </c>
@@ -2734,7 +2772,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D10" s="5">
         <v>2</v>
       </c>
@@ -2761,7 +2799,7 @@
         <v>24000</v>
       </c>
     </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D11" s="5">
         <v>3</v>
       </c>
@@ -2785,7 +2823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D12" s="5">
         <v>4</v>
       </c>
@@ -2812,7 +2850,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D13" s="5">
         <v>5</v>
       </c>
@@ -2839,7 +2877,7 @@
         <v>26000</v>
       </c>
     </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D14" s="5">
         <v>6</v>
       </c>
@@ -2847,15 +2885,15 @@
         <v>27</v>
       </c>
       <c r="F14">
-        <f>Furniture!F17</f>
-        <v>537480</v>
+        <f>Furniture!F16</f>
+        <v>678750</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F18:F36)</f>
-        <v>425105</v>
+        <f>SUM(Furniture!F17:F35)</f>
+        <v>446405</v>
       </c>
       <c r="H14">
-        <v>28300</v>
+        <v>49600</v>
       </c>
       <c r="I14">
         <f>SUM(L25:L27)</f>
@@ -2863,10 +2901,10 @@
       </c>
       <c r="J14" s="4">
         <f t="shared" si="0"/>
-        <v>112375</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.25">
+        <v>232345</v>
+      </c>
+    </row>
+    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D15" s="5">
         <v>7</v>
       </c>
@@ -2893,7 +2931,7 @@
         <v>67000</v>
       </c>
     </row>
-    <row r="16" spans="4:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="5">
         <v>8</v>
       </c>
@@ -2920,22 +2958,22 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="1"/>
       <c r="E17" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1644043</v>
+        <v>1785313</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1409668</v>
+        <v>1430968</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>279668</v>
+        <v>300968</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
@@ -2943,10 +2981,10 @@
       </c>
       <c r="J17" s="3">
         <f t="shared" si="0"/>
-        <v>234375</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+        <v>354345</v>
+      </c>
+    </row>
+    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E18" s="29" t="s">
         <v>36</v>
       </c>
@@ -2954,25 +2992,25 @@
         <v>1213000</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E19" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F19" s="28">
         <f>H17</f>
-        <v>279668</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+        <v>300968</v>
+      </c>
+    </row>
+    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
       <c r="E20" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>151375</v>
-      </c>
-    </row>
-    <row r="23" spans="3:16" ht="28.15" customHeight="1" x14ac:dyDescent="0.25">
+        <v>271345</v>
+      </c>
+    </row>
+    <row r="23" spans="3:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="56" t="s">
         <v>45</v>
       </c>
@@ -2990,7 +3028,7 @@
       <c r="O23" s="56"/>
       <c r="P23" s="56"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C24" s="33" t="s">
         <v>46</v>
       </c>
@@ -3013,7 +3051,7 @@
         <v>50</v>
       </c>
       <c r="J24" s="37" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K24" s="37" t="s">
         <v>17</v>
@@ -3034,7 +3072,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C25" s="28">
         <v>1</v>
       </c>
@@ -3074,7 +3112,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C26" s="28">
         <v>2</v>
       </c>
@@ -3119,7 +3157,7 @@
         <v>61190</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C27" s="28">
         <v>3</v>
       </c>
@@ -3179,16 +3217,16 @@
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -3202,7 +3240,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
         <v>62</v>
       </c>
@@ -3214,7 +3252,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" s="11" t="s">
         <v>24</v>
@@ -3224,7 +3262,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>67</v>
@@ -3234,7 +3272,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>80</v>
@@ -3244,7 +3282,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>81</v>
@@ -3254,7 +3292,7 @@
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>84</v>
@@ -3264,7 +3302,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
         <v>83</v>
@@ -3274,7 +3312,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>20</v>
@@ -3284,7 +3322,7 @@
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="65"/>
       <c r="E17" s="13" t="s">
         <v>6</v>
@@ -3295,7 +3333,7 @@
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" s="65"/>
       <c r="E18" s="11" t="s">
         <v>32</v>
@@ -3307,7 +3345,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="65"/>
       <c r="E19" s="11" t="s">
         <v>34</v>
@@ -3319,7 +3357,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="65"/>
       <c r="E20" s="11" t="s">
         <v>33</v>
@@ -3331,7 +3369,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D21" s="65"/>
       <c r="E21" s="11" t="s">
         <v>35</v>
@@ -3343,7 +3381,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D22" s="65"/>
       <c r="E22" s="11" t="s">
         <v>69</v>
@@ -3355,7 +3393,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D23" s="65"/>
       <c r="E23" s="11" t="s">
         <v>70</v>
@@ -3367,7 +3405,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="65"/>
       <c r="E24" s="11" t="s">
         <v>76</v>
@@ -3379,7 +3417,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D25" s="65"/>
       <c r="E25" s="11" t="s">
         <v>78</v>
@@ -3391,7 +3429,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D26" s="65"/>
       <c r="E26" s="11" t="s">
         <v>79</v>
@@ -3403,31 +3441,31 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D27" s="65"/>
       <c r="E27" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F27" s="41"/>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D28" s="65"/>
       <c r="E28" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F28" s="41"/>
       <c r="G28" s="20"/>
     </row>
-    <row r="29" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D29" s="65"/>
       <c r="E29" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F29" s="12"/>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D30" s="66"/>
       <c r="E30" s="13" t="s">
         <v>13</v>
@@ -3450,20 +3488,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:G23"/>
+  <dimension ref="D6:G33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19:G23"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="4" max="5" width="24.77734375" customWidth="1"/>
+    <col min="6" max="6" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D7" s="61" t="s">
         <v>54</v>
       </c>
@@ -3471,7 +3509,7 @@
       <c r="F7" s="62"/>
       <c r="G7" s="63"/>
     </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D8" s="57" t="s">
         <v>55</v>
       </c>
@@ -3485,7 +3523,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="58"/>
       <c r="E9" s="60"/>
       <c r="F9" s="28" t="s">
@@ -3495,7 +3533,7 @@
         <v>12300</v>
       </c>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="58"/>
       <c r="E10" s="60"/>
       <c r="F10" s="47" t="s">
@@ -3505,7 +3543,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="51"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
@@ -3515,7 +3553,7 @@
         <v>16345</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="51"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28" t="s">
@@ -3525,17 +3563,17 @@
         <v>5500</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="51"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G13" s="50">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="52"/>
       <c r="E14" s="53"/>
       <c r="F14" s="53" t="s">
@@ -3546,8 +3584,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="55" t="s">
         <v>66</v>
       </c>
@@ -3561,7 +3599,7 @@
         <v>23500</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="51"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
@@ -3571,19 +3609,19 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D21" s="51"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="50"/>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D22" s="51"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="52"/>
       <c r="E23" s="53"/>
       <c r="F23" s="53" t="s">
@@ -3592,6 +3630,26 @@
       <c r="G23" s="54">
         <f>E19-SUM(G19:G22)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D26" t="s">
+        <v>119</v>
+      </c>
+      <c r="E26">
+        <v>313193</v>
+      </c>
+      <c r="F26" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26">
+        <v>5300</v>
+      </c>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f>E26-(SUM(G26:G32))</f>
+        <v>307893</v>
       </c>
     </row>
   </sheetData>
@@ -3612,17 +3670,17 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="23.109375" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="60.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -3636,7 +3694,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
         <v>2</v>
       </c>
@@ -3648,7 +3706,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="65"/>
       <c r="E10" t="s">
         <v>4</v>
@@ -3658,7 +3716,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="65"/>
       <c r="E11" s="1" t="s">
         <v>6</v>
@@ -3669,7 +3727,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" t="s">
         <v>7</v>
@@ -3681,7 +3739,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" t="s">
         <v>8</v>
@@ -3693,7 +3751,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="65"/>
       <c r="E14" t="s">
         <v>9</v>
@@ -3705,7 +3763,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="66"/>
       <c r="E15" s="1" t="s">
         <v>10</v>
@@ -3733,16 +3791,16 @@
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="27.28515625" customWidth="1"/>
-    <col min="6" max="6" width="31.5703125" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" customWidth="1"/>
+    <col min="6" max="6" width="31.5546875" customWidth="1"/>
+    <col min="7" max="7" width="32.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="58.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="58.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -3756,7 +3814,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="64" t="s">
         <v>11</v>
       </c>
@@ -3768,7 +3826,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="65"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
@@ -3779,7 +3837,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>32</v>
@@ -3791,7 +3849,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>31</v>
@@ -3803,10 +3861,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F13" s="41">
         <v>15000</v>
@@ -3815,22 +3873,22 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F14" s="41">
         <v>5000</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F15" s="12">
         <v>0</v>
@@ -3839,7 +3897,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="66"/>
       <c r="E16" s="13" t="s">
         <v>13</v>
@@ -3868,16 +3926,16 @@
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="79.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="79.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -3891,7 +3949,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D9" s="64" t="s">
         <v>15</v>
       </c>
@@ -3903,7 +3961,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D10" s="65"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
@@ -3914,7 +3972,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>32</v>
@@ -3926,7 +3984,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>34</v>
@@ -3938,7 +3996,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>33</v>
@@ -3950,7 +4008,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="66"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
@@ -3977,16 +4035,16 @@
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="49.28515625" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="49.33203125" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="16.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="64.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="64.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -4000,7 +4058,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
         <v>61</v>
       </c>
@@ -4012,17 +4070,17 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F10" s="12">
         <v>720</v>
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" t="s">
         <v>74</v>
@@ -4032,27 +4090,27 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F12" s="4">
         <v>6580</v>
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F13" s="4">
         <v>900</v>
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="65"/>
       <c r="E14" t="s">
         <v>75</v>
@@ -4062,7 +4120,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="65"/>
       <c r="E15" t="s">
         <v>87</v>
@@ -4072,7 +4130,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D16" s="65"/>
       <c r="E16" t="s">
         <v>86</v>
@@ -4082,7 +4140,7 @@
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="65"/>
       <c r="E17" t="s">
         <v>88</v>
@@ -4092,17 +4150,17 @@
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" s="65"/>
       <c r="E18" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F18" s="4">
         <v>1620</v>
       </c>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="65"/>
       <c r="E19" t="s">
         <v>92</v>
@@ -4110,7 +4168,7 @@
       <c r="F19" s="4"/>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="65"/>
       <c r="E20" t="s">
         <v>90</v>
@@ -4120,7 +4178,7 @@
       </c>
       <c r="G20" s="20"/>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D21" s="65"/>
       <c r="E21" t="s">
         <v>89</v>
@@ -4130,17 +4188,17 @@
       </c>
       <c r="G21" s="20"/>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D22" s="65"/>
       <c r="E22" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F22" s="4">
         <v>600</v>
       </c>
       <c r="G22" s="20"/>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D23" s="65"/>
       <c r="E23" t="s">
         <v>71</v>
@@ -4150,7 +4208,7 @@
       </c>
       <c r="G23" s="20"/>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="65"/>
       <c r="E24" t="s">
         <v>72</v>
@@ -4160,7 +4218,7 @@
       </c>
       <c r="G24" s="20"/>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D25" s="65"/>
       <c r="E25" t="s">
         <v>30</v>
@@ -4170,7 +4228,7 @@
       </c>
       <c r="G25" s="20"/>
     </row>
-    <row r="26" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D26" s="65"/>
       <c r="E26" t="s">
         <v>91</v>
@@ -4180,7 +4238,7 @@
       </c>
       <c r="G26" s="20"/>
     </row>
-    <row r="27" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D27" s="65"/>
       <c r="E27" s="1" t="s">
         <v>6</v>
@@ -4191,7 +4249,7 @@
       </c>
       <c r="G27" s="20"/>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D28" s="65"/>
       <c r="E28" t="s">
         <v>32</v>
@@ -4203,7 +4261,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D29" s="65"/>
       <c r="E29" t="s">
         <v>34</v>
@@ -4215,7 +4273,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D30" s="65"/>
       <c r="E30" t="s">
         <v>33</v>
@@ -4227,7 +4285,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D31" s="65"/>
       <c r="E31" t="s">
         <v>35</v>
@@ -4239,7 +4297,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D32" s="65"/>
       <c r="E32" t="s">
         <v>69</v>
@@ -4251,7 +4309,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D33" s="65"/>
       <c r="E33" t="s">
         <v>70</v>
@@ -4263,7 +4321,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D34" s="65"/>
       <c r="E34" t="s">
         <v>76</v>
@@ -4275,7 +4333,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D35" s="65"/>
       <c r="E35" t="s">
         <v>78</v>
@@ -4287,7 +4345,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D36" s="65"/>
       <c r="E36" t="s">
         <v>79</v>
@@ -4299,10 +4357,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D37" s="65"/>
       <c r="E37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F37" s="41">
         <v>2859</v>
@@ -4311,10 +4369,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D38" s="65"/>
       <c r="E38" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F38" s="41">
         <v>2000</v>
@@ -4323,15 +4381,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D39" s="65"/>
       <c r="E39" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F39" s="4"/>
       <c r="G39" s="20"/>
     </row>
-    <row r="40" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D40" s="66"/>
       <c r="E40" s="1" t="s">
         <v>10</v>
@@ -4357,19 +4415,19 @@
   <dimension ref="D7:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F16:F20"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="70.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="70.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -4383,7 +4441,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
         <v>16</v>
       </c>
@@ -4395,7 +4453,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" s="11" t="s">
         <v>19</v>
@@ -4405,7 +4463,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>18</v>
@@ -4415,7 +4473,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="65"/>
       <c r="E12" s="11" t="s">
         <v>44</v>
@@ -4425,17 +4483,17 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F13" s="12">
         <v>15000</v>
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>20</v>
@@ -4445,7 +4503,7 @@
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="65"/>
       <c r="E15" s="13" t="s">
         <v>6</v>
@@ -4456,7 +4514,7 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>32</v>
@@ -4468,7 +4526,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="65"/>
       <c r="E17" s="11" t="s">
         <v>34</v>
@@ -4480,7 +4538,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" s="65"/>
       <c r="E18" s="11" t="s">
         <v>33</v>
@@ -4492,7 +4550,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="65"/>
       <c r="E19" s="11" t="s">
         <v>35</v>
@@ -4504,7 +4562,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="65"/>
       <c r="E20" s="11" t="s">
         <v>69</v>
@@ -4516,7 +4574,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="65"/>
       <c r="E21" s="11" t="s">
         <v>70</v>
@@ -4524,7 +4582,7 @@
       <c r="F21" s="43"/>
       <c r="G21" s="4"/>
     </row>
-    <row r="22" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D22" s="66"/>
       <c r="E22" s="13" t="s">
         <v>13</v>
@@ -4551,16 +4609,16 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="31.5703125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5546875" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="17" t="s">
         <v>0</v>
       </c>
@@ -4574,9 +4632,9 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="64" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>40</v>
@@ -4586,7 +4644,7 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="D10" s="65"/>
       <c r="E10" s="31" t="s">
         <v>43</v>
@@ -4596,7 +4654,7 @@
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D11" s="65"/>
       <c r="E11" s="11" t="s">
         <v>28</v>
@@ -4604,7 +4662,7 @@
       <c r="F11" s="12"/>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D12" s="65"/>
       <c r="E12" s="13" t="s">
         <v>6</v>
@@ -4615,7 +4673,7 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="65"/>
       <c r="E13" s="11" t="s">
         <v>32</v>
@@ -4627,7 +4685,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="65"/>
       <c r="E14" s="11" t="s">
         <v>34</v>
@@ -4639,7 +4697,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
         <v>33</v>
@@ -4651,7 +4709,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="65"/>
       <c r="E16" s="11" t="s">
         <v>35</v>
@@ -4663,7 +4721,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="66"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
@@ -4684,22 +4742,22 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:G37"/>
+  <dimension ref="D7:G36"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
-    <col min="5" max="5" width="45.42578125" customWidth="1"/>
-    <col min="6" max="6" width="32.85546875" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" customWidth="1"/>
+    <col min="5" max="5" width="45.44140625" customWidth="1"/>
+    <col min="6" max="6" width="32.88671875" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="4:7" ht="73.150000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:7" ht="73.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="6" t="s">
         <v>0</v>
       </c>
@@ -4713,7 +4771,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D9" s="67" t="s">
         <v>21</v>
       </c>
@@ -4725,17 +4783,17 @@
       </c>
       <c r="G9" s="20"/>
     </row>
-    <row r="10" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D10" s="68"/>
       <c r="E10" s="19" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F10" s="12">
         <v>18200</v>
       </c>
       <c r="G10" s="20"/>
     </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D11" s="68"/>
       <c r="E11" s="19" t="s">
         <v>94</v>
@@ -4745,7 +4803,7 @@
       </c>
       <c r="G11" s="20"/>
     </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D12" s="68"/>
       <c r="E12" s="19" t="s">
         <v>22</v>
@@ -4755,283 +4813,285 @@
       </c>
       <c r="G12" s="20"/>
     </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="68"/>
       <c r="E13" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F13" s="12"/>
+        <v>123</v>
+      </c>
+      <c r="F13" s="12">
+        <v>20000</v>
+      </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="68"/>
       <c r="E14" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="12"/>
+        <v>23</v>
+      </c>
+      <c r="F14" s="12">
+        <v>300000</v>
+      </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D15" s="68"/>
       <c r="E15" s="19" t="s">
-        <v>23</v>
+        <v>85</v>
       </c>
       <c r="F15" s="12">
-        <v>200000</v>
+        <v>54100</v>
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="68"/>
-      <c r="E16" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="12">
-        <v>32830</v>
+      <c r="E16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" s="14">
+        <f>SUM(F9:F15)</f>
+        <v>678750</v>
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="68"/>
-      <c r="E17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="14">
-        <f>SUM(F9:F16)</f>
-        <v>537480</v>
-      </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="41">
+        <v>80000</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D18" s="68"/>
       <c r="E18" s="19" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F18" s="41">
-        <v>80000</v>
+        <v>26500</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D19" s="68"/>
       <c r="E19" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F19" s="41">
-        <v>26500</v>
+        <v>50000</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D20" s="68"/>
       <c r="E20" s="19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F20" s="41">
-        <v>50000</v>
+        <v>14000</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D21" s="68"/>
       <c r="E21" s="19" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="F21" s="41">
-        <v>14000</v>
+        <v>5000</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D22" s="68"/>
       <c r="E22" s="19" t="s">
-        <v>69</v>
+        <v>76</v>
       </c>
       <c r="F22" s="41">
-        <v>5000</v>
+        <v>27000</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D23" s="68"/>
       <c r="E23" s="19" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F23" s="41">
-        <v>27000</v>
+        <v>50000</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D24" s="68"/>
       <c r="E24" s="19" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F24" s="41">
-        <v>50000</v>
+        <v>11270</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D25" s="68"/>
       <c r="E25" s="19" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="F25" s="41">
-        <v>11270</v>
+        <v>21725</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D26" s="68"/>
       <c r="E26" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F26" s="41">
-        <v>21725</v>
+        <v>44325</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D27" s="68"/>
       <c r="E27" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F27" s="41">
-        <v>44325</v>
+        <v>21560</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D28" s="68"/>
       <c r="E28" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F28" s="41">
-        <v>21560</v>
+        <v>7250</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D29" s="68"/>
       <c r="E29" s="19" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F29" s="41">
-        <v>7250</v>
+        <v>18600</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D30" s="68"/>
       <c r="E30" s="19" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="F30" s="41">
-        <v>18600</v>
+        <v>44325</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D31" s="68"/>
       <c r="E31" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F31" s="41">
-        <v>44325</v>
+        <v>1800</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D32" s="68"/>
       <c r="E32" s="19" t="s">
         <v>114</v>
       </c>
       <c r="F32" s="41">
-        <v>1800</v>
+        <v>1750</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D33" s="68"/>
       <c r="E33" s="19" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F33" s="41">
-        <v>1750</v>
+        <v>21300</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D34" s="68"/>
-      <c r="E34" s="19"/>
+      <c r="E34" s="19" t="s">
+        <v>121</v>
+      </c>
       <c r="F34" s="41"/>
       <c r="G34" s="20"/>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D35" s="68"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D36" s="68"/>
-      <c r="E36" s="19" t="s">
-        <v>117</v>
-      </c>
-      <c r="F36" s="12">
+      <c r="E35" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" s="12">
         <v>0</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D37" s="69"/>
-      <c r="E37" s="1" t="s">
+    <row r="36" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D36" s="69"/>
+      <c r="E36" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F37" s="14">
-        <f>F17-SUM(F18:F36)</f>
-        <v>112375</v>
-      </c>
-      <c r="G37" s="21"/>
+      <c r="F36" s="14">
+        <f>F16-SUM(F17:F35)</f>
+        <v>232345</v>
+      </c>
+      <c r="G36" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D37"/>
+    <mergeCell ref="D9:D36"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated as of 25-11-2023 part2
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DFA8812-754A-418D-ADF0-839C1A1E88F0}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048F7A35-1B26-488F-A3FE-FFDFFDDE8C39}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="M26" authorId="0" shapeId="0" xr:uid="{05599553-7662-4E42-93A4-2E2ED5534801}">
+    <comment ref="N26" authorId="0" shapeId="0" xr:uid="{05599553-7662-4E42-93A4-2E2ED5534801}">
       <text>
         <r>
           <rPr>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J27" authorId="0" shapeId="0" xr:uid="{C6A08A85-8275-4C88-95E8-4526C8E02D7C}">
+    <comment ref="K27" authorId="0" shapeId="0" xr:uid="{C6A08A85-8275-4C88-95E8-4526C8E02D7C}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L27" authorId="0" shapeId="0" xr:uid="{134DA49D-E84E-4882-A21A-C0FA2F9A36E6}">
+    <comment ref="M27" authorId="0" shapeId="0" xr:uid="{134DA49D-E84E-4882-A21A-C0FA2F9A36E6}">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M27" authorId="0" shapeId="0" xr:uid="{F8374CFC-2A6A-41D3-A4EE-2F8672A0B170}">
+    <comment ref="N27" authorId="0" shapeId="0" xr:uid="{F8374CFC-2A6A-41D3-A4EE-2F8672A0B170}">
       <text>
         <r>
           <rPr>
@@ -519,8 +519,9 @@
           </rPr>
           <t xml:space="preserve">
 3 tubs 20kg
-5kg special glue
-</t>
+5kg  - 16500
+Extra glue for PU and Acrylic - 1750
+5th Tub Glue and Extra glue - 5590</t>
         </r>
       </text>
     </comment>
@@ -570,7 +571,8 @@
           </rPr>
           <t xml:space="preserve">
 Tentative
-Till now exepnded - 14000+21725+1750 = 37475+3600 = 41075</t>
+Till now exepnded - 14000+21725+1750 = 37475+3600 (Locks)
+= 41075+4700(Edge Binding) = 45775</t>
         </r>
       </text>
     </comment>
@@ -868,6 +870,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="H29" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+15000</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F30" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
@@ -916,6 +942,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Glue
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F33" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
       <text>
         <r>
@@ -936,8 +987,106 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Self 1600
-AIA - 5300</t>
+Self 16000
+AIA - 5300
+Extra ply
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Edge Binding</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Glue and screw</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I36" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da till now</t>
         </r>
       </text>
     </comment>
@@ -1199,7 +1348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="132">
   <si>
     <t>Provider</t>
   </si>
@@ -1571,6 +1720,30 @@
   </si>
   <si>
     <t>Estimated Glass&amp; alumunium Frame</t>
+  </si>
+  <si>
+    <t>Payment - 21</t>
+  </si>
+  <si>
+    <t>Payment - 22</t>
+  </si>
+  <si>
+    <t>AIA</t>
+  </si>
+  <si>
+    <t>Edge Binding (Furninture)</t>
+  </si>
+  <si>
+    <t>Payment -6</t>
+  </si>
+  <si>
+    <t>Payment -7</t>
+  </si>
+  <si>
+    <t>Bikas Da</t>
+  </si>
+  <si>
+    <t>Glue Extra</t>
   </si>
 </sst>
 </file>
@@ -2388,6 +2561,18 @@
 </file>
 
 <file path=xl/persons/person55.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person56.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person57.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person58.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2704,10 +2889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
-  <dimension ref="C7:P27"/>
+  <dimension ref="C7:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2715,14 +2900,14 @@
     <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="51" customWidth="1"/>
     <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.5546875" customWidth="1"/>
-    <col min="15" max="15" width="9.33203125" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" customWidth="1"/>
+    <col min="10" max="10" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.5546875" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="17" max="17" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="8" spans="4:10" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="4:11" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="22" t="s">
         <v>25</v>
       </c>
@@ -2739,13 +2924,16 @@
         <v>63</v>
       </c>
       <c r="I8" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="J8" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="K8" s="26" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D9" s="5">
         <v>1</v>
       </c>
@@ -2763,16 +2951,16 @@
       <c r="H9">
         <v>40140</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <f>SUM(G25:G27)</f>
         <v>294139</v>
       </c>
-      <c r="J9" s="4">
-        <f t="shared" ref="J9:J17" si="0">F9-G9</f>
+      <c r="K9" s="4">
+        <f t="shared" ref="K9:K17" si="0">F9-G9</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D10" s="5">
         <v>2</v>
       </c>
@@ -2784,22 +2972,22 @@
         <v>65000</v>
       </c>
       <c r="G10">
-        <f>SUM(Paint!F11:F15)</f>
-        <v>41000</v>
+        <f>SUM(Paint!F11:F17)</f>
+        <v>42500</v>
       </c>
       <c r="H10">
-        <v>7283</v>
-      </c>
-      <c r="I10">
+        <v>8783</v>
+      </c>
+      <c r="J10">
         <f>SUM(H25:H27)</f>
         <v>33717</v>
       </c>
-      <c r="J10" s="4">
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>24000</v>
-      </c>
-    </row>
-    <row r="11" spans="4:10" x14ac:dyDescent="0.3">
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D11" s="5">
         <v>3</v>
       </c>
@@ -2814,16 +3002,16 @@
         <f>SUM('False Ceiling'!F11:F13)</f>
         <v>120000</v>
       </c>
-      <c r="I11">
-        <f>SUM(I25:I27)</f>
+      <c r="J11">
+        <f>SUM(J25:J27)</f>
         <v>120000</v>
       </c>
-      <c r="J11" s="4">
+      <c r="K11" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D12" s="5">
         <v>4</v>
       </c>
@@ -2841,16 +3029,16 @@
       <c r="H12">
         <v>31695</v>
       </c>
-      <c r="I12">
-        <f>SUM(J25:J27)</f>
+      <c r="J12">
+        <f>SUM(K25:K27)</f>
         <v>109189</v>
       </c>
-      <c r="J12" s="4">
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
         <v>5000</v>
       </c>
     </row>
-    <row r="13" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D13" s="5">
         <v>5</v>
       </c>
@@ -2866,18 +3054,18 @@
         <v>89000</v>
       </c>
       <c r="H13">
-        <v>38050</v>
-      </c>
-      <c r="I13">
-        <f>SUM(K25:K27)</f>
+        <v>36300</v>
+      </c>
+      <c r="J13">
+        <f>SUM(L25:L27)</f>
         <v>52700</v>
       </c>
-      <c r="J13" s="4">
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
         <v>26000</v>
       </c>
     </row>
-    <row r="14" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D14" s="5">
         <v>6</v>
       </c>
@@ -2886,25 +3074,28 @@
       </c>
       <c r="F14">
         <f>Furniture!F16</f>
-        <v>678750</v>
+        <v>694390</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F17:F35)</f>
-        <v>446405</v>
+        <f>SUM(Furniture!F17:F41)</f>
+        <v>486695</v>
       </c>
       <c r="H14">
-        <v>49600</v>
+        <v>46050</v>
       </c>
       <c r="I14">
-        <f>SUM(L25:L27)</f>
+        <v>45590</v>
+      </c>
+      <c r="J14">
+        <f>SUM(M25:M27)</f>
         <v>395055</v>
       </c>
-      <c r="J14" s="4">
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>232345</v>
-      </c>
-    </row>
-    <row r="15" spans="4:10" x14ac:dyDescent="0.3">
+        <v>207695</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.3">
       <c r="D15" s="5">
         <v>7</v>
       </c>
@@ -2922,16 +3113,16 @@
       <c r="H15">
         <v>129000</v>
       </c>
-      <c r="I15">
-        <f>SUM(M25:M27)</f>
+      <c r="J15">
+        <f>SUM(N25:N27)</f>
         <v>99900</v>
       </c>
-      <c r="J15" s="4">
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
         <v>67000</v>
       </c>
     </row>
-    <row r="16" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="5">
         <v>8</v>
       </c>
@@ -2949,42 +3140,46 @@
       <c r="H16">
         <v>5200</v>
       </c>
-      <c r="I16">
-        <f>SUM(N25:N27)</f>
+      <c r="J16">
+        <f>SUM(O25:O27)</f>
         <v>25300</v>
       </c>
-      <c r="J16" s="4">
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="1"/>
       <c r="E17" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1785313</v>
+        <v>1800953</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1430968</v>
+        <v>1472758</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>300968</v>
+        <v>297168</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
+        <v>45590</v>
+      </c>
+      <c r="J17" s="2">
+        <f>SUM(J9:J16)</f>
         <v>1130000</v>
       </c>
-      <c r="J17" s="3">
+      <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>354345</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.3">
+        <v>328195</v>
+      </c>
+    </row>
+    <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E18" s="29" t="s">
         <v>36</v>
       </c>
@@ -2992,25 +3187,25 @@
         <v>1213000</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E19" s="28" t="s">
         <v>53</v>
       </c>
       <c r="F19" s="28">
-        <f>H17</f>
-        <v>300968</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+        <f>SUM(H17,I17)</f>
+        <v>342758</v>
+      </c>
+    </row>
+    <row r="20" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E20" s="28" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>271345</v>
-      </c>
-    </row>
-    <row r="23" spans="3:16" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+        <v>245195</v>
+      </c>
+    </row>
+    <row r="23" spans="3:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="56" t="s">
         <v>45</v>
       </c>
@@ -3027,8 +3222,9 @@
       <c r="N23" s="56"/>
       <c r="O23" s="56"/>
       <c r="P23" s="56"/>
-    </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
+      <c r="Q23" s="56"/>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" s="33" t="s">
         <v>46</v>
       </c>
@@ -3047,32 +3243,33 @@
       <c r="H24" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="37" t="s">
+      <c r="I24" s="37"/>
+      <c r="J24" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="J24" s="37" t="s">
+      <c r="K24" s="37" t="s">
         <v>116</v>
       </c>
-      <c r="K24" s="37" t="s">
+      <c r="L24" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="L24" s="37" t="s">
+      <c r="M24" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="M24" s="37" t="s">
+      <c r="N24" s="37" t="s">
         <v>28</v>
       </c>
-      <c r="N24" s="37" t="s">
+      <c r="O24" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="O24" s="38" t="s">
+      <c r="P24" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="P24" s="38" t="s">
+      <c r="Q24" s="38" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="25" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C25" s="28">
         <v>1</v>
       </c>
@@ -3089,35 +3286,36 @@
         <v>127000</v>
       </c>
       <c r="H25" s="28"/>
-      <c r="I25" s="40">
+      <c r="I25" s="28"/>
+      <c r="J25" s="40">
         <v>50000</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="40">
+      <c r="K25" s="28"/>
+      <c r="L25" s="40">
         <v>17700</v>
       </c>
-      <c r="L25" s="40">
+      <c r="M25" s="40">
         <v>80000</v>
       </c>
-      <c r="M25" s="28"/>
-      <c r="N25" s="40">
+      <c r="N25" s="28"/>
+      <c r="O25" s="40">
         <v>25300</v>
       </c>
-      <c r="O25" s="28">
-        <f>SUM(G25:N25)</f>
+      <c r="P25" s="28">
+        <f>SUM(G25:O25)</f>
         <v>300000</v>
       </c>
-      <c r="P25" s="28">
-        <f>SUM(E25,D25)-O25</f>
+      <c r="Q25" s="28">
+        <f>SUM(E25,D25)-P25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="26" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C26" s="28">
         <v>2</v>
       </c>
       <c r="D26" s="28">
-        <f>D25+P25</f>
+        <f>D25+Q25</f>
         <v>0</v>
       </c>
       <c r="E26" s="28">
@@ -3132,37 +3330,38 @@
       <c r="H26" s="40">
         <v>15000</v>
       </c>
-      <c r="I26" s="40">
+      <c r="I26" s="40"/>
+      <c r="J26" s="40">
         <v>40000</v>
       </c>
-      <c r="J26" s="40">
+      <c r="K26" s="40">
         <v>58371</v>
       </c>
-      <c r="K26" s="40">
+      <c r="L26" s="40">
         <v>20000</v>
       </c>
-      <c r="L26" s="40">
+      <c r="M26" s="40">
         <v>96000</v>
       </c>
-      <c r="M26" s="40">
+      <c r="N26" s="40">
         <v>42300</v>
       </c>
-      <c r="N26" s="28"/>
-      <c r="O26" s="28">
-        <f>SUM(G26:N26)</f>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28">
+        <f>SUM(G26:O26)</f>
         <v>438810</v>
       </c>
-      <c r="P26" s="28">
-        <f t="shared" ref="P26:P27" si="1">SUM(E26,D26)-O26</f>
+      <c r="Q26" s="28">
+        <f t="shared" ref="Q26:Q27" si="1">SUM(E26,D26)-P26</f>
         <v>61190</v>
       </c>
     </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C27" s="28">
         <v>3</v>
       </c>
       <c r="D27" s="28">
-        <f>D26+P26</f>
+        <f>D26+Q26</f>
         <v>61190</v>
       </c>
       <c r="E27" s="28">
@@ -3175,34 +3374,35 @@
       <c r="H27" s="40">
         <v>18717</v>
       </c>
-      <c r="I27" s="40">
+      <c r="I27" s="40"/>
+      <c r="J27" s="40">
         <v>30000</v>
       </c>
-      <c r="J27" s="40">
+      <c r="K27" s="40">
         <v>50818</v>
       </c>
-      <c r="K27" s="40">
+      <c r="L27" s="40">
         <v>15000</v>
       </c>
-      <c r="L27" s="40">
+      <c r="M27" s="40">
         <v>219055</v>
       </c>
-      <c r="M27" s="40">
+      <c r="N27" s="40">
         <v>57600</v>
       </c>
-      <c r="N27" s="28"/>
-      <c r="O27" s="28">
-        <f>SUM(G27:N27)</f>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28">
+        <f>SUM(G27:O27)</f>
         <v>391190</v>
       </c>
-      <c r="P27" s="28">
+      <c r="Q27" s="28">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C23:P23"/>
+    <mergeCell ref="C23:Q23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -3488,10 +3688,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:G33"/>
+  <dimension ref="D6:G37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G29" sqref="G26:G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3633,23 +3833,47 @@
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" t="s">
+      <c r="D26" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="28">
         <v>313193</v>
       </c>
-      <c r="F26" t="s">
+      <c r="F26" s="28" t="s">
         <v>85</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="28">
         <v>5300</v>
       </c>
     </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G33">
-        <f>E26-(SUM(G26:G32))</f>
-        <v>307893</v>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="F27" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="28">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="F28" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="G28" s="28">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="F29" s="28" t="s">
+        <v>131</v>
+      </c>
+      <c r="G29" s="28">
+        <v>5590</v>
+      </c>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <f>E26-(SUM(G26:G36))</f>
+        <v>267603</v>
       </c>
     </row>
   </sheetData>
@@ -3785,10 +4009,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5512692-EDEE-4A22-9F00-43BA354170EF}">
-  <dimension ref="D7:G16"/>
+  <dimension ref="D7:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3885,32 +4109,52 @@
         <v>118</v>
       </c>
     </row>
-    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="65"/>
       <c r="E15" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="41">
+        <v>1500</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="65"/>
+      <c r="E16" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="F16" s="41"/>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="65"/>
+      <c r="E17" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F17" s="12">
         <v>0</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="66"/>
-      <c r="E16" s="13" t="s">
+    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="66"/>
+      <c r="E18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="14">
-        <f>F10-SUM(F11:F15)</f>
-        <v>24000</v>
-      </c>
-      <c r="G16" s="21"/>
+      <c r="F18" s="14">
+        <f>F10-SUM(F11:F17)</f>
+        <v>22500</v>
+      </c>
+      <c r="G18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D16"/>
+    <mergeCell ref="D9:D18"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4415,7 +4659,7 @@
   <dimension ref="D7:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+      <selection activeCell="F20" sqref="F16:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4742,10 +4986,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:G36"/>
+  <dimension ref="D7:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4789,7 +5033,7 @@
         <v>110</v>
       </c>
       <c r="F10" s="12">
-        <v>18200</v>
+        <v>23840</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -4819,7 +5063,7 @@
         <v>123</v>
       </c>
       <c r="F13" s="12">
-        <v>20000</v>
+        <v>30000</v>
       </c>
       <c r="G13" s="20"/>
     </row>
@@ -4850,11 +5094,11 @@
       </c>
       <c r="F16" s="14">
         <f>SUM(F9:F15)</f>
-        <v>678750</v>
+        <v>694390</v>
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D17" s="68"/>
       <c r="E17" s="19" t="s">
         <v>32</v>
@@ -4866,7 +5110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" s="68"/>
       <c r="E18" s="19" t="s">
         <v>34</v>
@@ -4877,8 +5121,11 @@
       <c r="G18" s="20" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" s="68"/>
       <c r="E19" s="19" t="s">
         <v>33</v>
@@ -4890,7 +5137,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" s="68"/>
       <c r="E20" s="19" t="s">
         <v>35</v>
@@ -4902,7 +5149,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" s="68"/>
       <c r="E21" s="19" t="s">
         <v>69</v>
@@ -4913,8 +5160,11 @@
       <c r="G21" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D22" s="68"/>
       <c r="E22" s="19" t="s">
         <v>76</v>
@@ -4926,7 +5176,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D23" s="68"/>
       <c r="E23" s="19" t="s">
         <v>78</v>
@@ -4937,8 +5187,11 @@
       <c r="G23" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D24" s="68"/>
       <c r="E24" s="19" t="s">
         <v>79</v>
@@ -4950,7 +5203,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D25" s="68"/>
       <c r="E25" s="19" t="s">
         <v>96</v>
@@ -4962,7 +5215,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D26" s="68"/>
       <c r="E26" s="19" t="s">
         <v>97</v>
@@ -4974,7 +5227,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D27" s="68"/>
       <c r="E27" s="19" t="s">
         <v>98</v>
@@ -4986,7 +5239,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D28" s="68"/>
       <c r="E28" s="19" t="s">
         <v>99</v>
@@ -4998,7 +5251,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D29" s="68"/>
       <c r="E29" s="19" t="s">
         <v>100</v>
@@ -5009,8 +5262,11 @@
       <c r="G29" s="20" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D30" s="68"/>
       <c r="E30" s="19" t="s">
         <v>111</v>
@@ -5022,7 +5278,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D31" s="68"/>
       <c r="E31" s="19" t="s">
         <v>112</v>
@@ -5034,7 +5290,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D32" s="68"/>
       <c r="E32" s="19" t="s">
         <v>114</v>
@@ -5046,7 +5302,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="68"/>
       <c r="E33" s="19" t="s">
         <v>115</v>
@@ -5058,40 +5314,98 @@
         <v>120</v>
       </c>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="68"/>
       <c r="E34" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F34" s="41"/>
-      <c r="G34" s="20"/>
-    </row>
-    <row r="35" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F34" s="41">
+        <v>4700</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="68"/>
       <c r="E35" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="F35" s="12">
+      <c r="F35" s="41">
+        <v>5590</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D36" s="68"/>
+      <c r="E36" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="41">
+        <v>30000</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H36" t="s">
+        <v>130</v>
+      </c>
+      <c r="I36">
+        <v>126500</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D37" s="68"/>
+      <c r="E37" s="19"/>
+      <c r="F37" s="41"/>
+      <c r="G37" s="20"/>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D38" s="68"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" s="68"/>
+      <c r="E39" s="19"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="68"/>
+      <c r="E40" s="19"/>
+      <c r="F40" s="41"/>
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="68"/>
+      <c r="E41" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F41" s="12">
         <v>0</v>
       </c>
-      <c r="G35" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="36" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D36" s="69"/>
-      <c r="E36" s="1" t="s">
+    <row r="42" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="69"/>
+      <c r="E42" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F36" s="14">
-        <f>F16-SUM(F17:F35)</f>
-        <v>232345</v>
-      </c>
-      <c r="G36" s="21"/>
+      <c r="F42" s="14">
+        <f>F16-SUM(F17:F41)</f>
+        <v>207695</v>
+      </c>
+      <c r="G42" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D36"/>
+    <mergeCell ref="D9:D42"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added updates till 01-12-2023
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{048F7A35-1B26-488F-A3FE-FFDFFDDE8C39}"/>
+  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386A01BA-2394-490C-9677-6381AF66F7F7}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="8" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -521,7 +521,8 @@
 3 tubs 20kg
 5kg  - 16500
 Extra glue for PU and Acrylic - 1750
-5th Tub Glue and Extra glue - 5590</t>
+5th Tub Glue and Extra glue - 5590
+6th Louvre Glue and normal glue - 2000</t>
         </r>
       </text>
     </comment>
@@ -572,11 +573,12 @@
           <t xml:space="preserve">
 Tentative
 Till now exepnded - 14000+21725+1750 = 37475+3600 (Locks)
-= 41075+4700(Edge Binding) = 45775</t>
+= 41075+4700(Edge Binding) = 45775
+ for the section of Louve Glue, rest material - 1730, total till now: 47505</t>
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{87678B8C-756B-4A16-A0B1-A3C2A9059184}">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{87678B8C-756B-4A16-A0B1-A3C2A9059184}">
       <text>
         <r>
           <rPr>
@@ -601,7 +603,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
       <text>
         <r>
           <rPr>
@@ -625,7 +627,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
       <text>
         <r>
           <rPr>
@@ -649,7 +651,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
       <text>
         <r>
           <rPr>
@@ -674,7 +676,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
       <text>
         <r>
           <rPr>
@@ -699,7 +701,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
       <text>
         <r>
           <rPr>
@@ -724,7 +726,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
       <text>
         <r>
           <rPr>
@@ -750,7 +752,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
       <text>
         <r>
           <rPr>
@@ -774,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
       <text>
         <r>
           <rPr>
@@ -798,7 +800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
       <text>
         <r>
           <rPr>
@@ -822,7 +824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
       <text>
         <r>
           <rPr>
@@ -846,7 +848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
       <text>
         <r>
           <rPr>
@@ -870,7 +872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H29" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
+    <comment ref="H30" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
       <text>
         <r>
           <rPr>
@@ -894,7 +896,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
           <rPr>
@@ -918,7 +920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
       <text>
         <r>
           <rPr>
@@ -942,7 +944,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
       <text>
         <r>
           <rPr>
@@ -967,7 +969,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
       <text>
         <r>
           <rPr>
@@ -994,7 +996,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
       <text>
         <r>
           <rPr>
@@ -1018,7 +1020,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
       <text>
         <r>
           <rPr>
@@ -1042,7 +1044,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
       <text>
         <r>
           <rPr>
@@ -1066,7 +1068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I36" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
+    <comment ref="I37" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
       <text>
         <r>
           <rPr>
@@ -1087,6 +1089,30 @@
           </rPr>
           <t xml:space="preserve">
 Bikas da till now</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Louvre Glue, muskin tapes, heatex and normal glue</t>
         </r>
       </text>
     </comment>
@@ -1348,7 +1374,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="135">
   <si>
     <t>Provider</t>
   </si>
@@ -1744,6 +1770,15 @@
   </si>
   <si>
     <t>Glue Extra</t>
+  </si>
+  <si>
+    <t>Raw Material - 4th Lot Extra laminates</t>
+  </si>
+  <si>
+    <t>Louvre Glue and muskin tape</t>
+  </si>
+  <si>
+    <t>Sections</t>
   </si>
 </sst>
 </file>
@@ -1883,7 +1918,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -2184,11 +2219,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2335,6 +2383,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2576,7 +2626,15 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person59.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/persons/person6.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person60.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2891,8 +2949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
   <dimension ref="C7:Q27"/>
   <sheetViews>
-    <sheetView topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2973,10 +3031,13 @@
       </c>
       <c r="G10">
         <f>SUM(Paint!F11:F17)</f>
-        <v>42500</v>
+        <v>52500</v>
       </c>
       <c r="H10">
         <v>8783</v>
+      </c>
+      <c r="I10">
+        <v>10000</v>
       </c>
       <c r="J10">
         <f>SUM(H25:H27)</f>
@@ -2984,7 +3045,7 @@
       </c>
       <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>22500</v>
+        <v>12500</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.3">
@@ -3073,18 +3134,18 @@
         <v>27</v>
       </c>
       <c r="F14">
-        <f>Furniture!F16</f>
-        <v>694390</v>
+        <f>Furniture!F17</f>
+        <v>706910</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F17:F41)</f>
-        <v>486695</v>
+        <f>SUM(Furniture!F18:F42)</f>
+        <v>490425</v>
       </c>
       <c r="H14">
         <v>46050</v>
       </c>
       <c r="I14">
-        <v>45590</v>
+        <v>49320</v>
       </c>
       <c r="J14">
         <f>SUM(M25:M27)</f>
@@ -3092,7 +3153,7 @@
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>207695</v>
+        <v>216485</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
@@ -3156,11 +3217,11 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1800953</v>
+        <v>1813473</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1472758</v>
+        <v>1486488</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
@@ -3168,7 +3229,7 @@
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>45590</v>
+        <v>59320</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(J9:J16)</f>
@@ -3176,7 +3237,7 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>328195</v>
+        <v>326985</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
@@ -3193,7 +3254,7 @@
       </c>
       <c r="F19" s="28">
         <f>SUM(H17,I17)</f>
-        <v>342758</v>
+        <v>356488</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
@@ -3202,7 +3263,7 @@
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>245195</v>
+        <v>243985</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
@@ -3688,16 +3749,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:G37"/>
+  <dimension ref="D6:H40"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="G29" sqref="G26:G29"/>
+      <selection activeCell="L31" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="5" width="24.77734375" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.77734375" customWidth="1"/>
+    <col min="8" max="8" width="16.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -3784,8 +3846,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" s="55" t="s">
         <v>66</v>
       </c>
@@ -3799,7 +3861,7 @@
         <v>23500</v>
       </c>
     </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" s="51"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
@@ -3809,19 +3871,19 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" s="51"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="50"/>
     </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D22" s="51"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="52"/>
       <c r="E23" s="53"/>
       <c r="F23" s="53" t="s">
@@ -3832,48 +3894,94 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D26" s="28" t="s">
         <v>119</v>
       </c>
       <c r="E26" s="28">
         <v>313193</v>
       </c>
-      <c r="F26" s="28" t="s">
+      <c r="F26" s="70" t="s">
         <v>85</v>
       </c>
-      <c r="G26" s="28">
+      <c r="G26" s="70">
         <v>5300</v>
       </c>
-    </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F27" s="28" t="s">
+      <c r="H26" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F27" s="71" t="s">
         <v>127</v>
       </c>
-      <c r="G27" s="28">
+      <c r="G27" s="71">
         <v>4700</v>
       </c>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F28" s="28" t="s">
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F28" s="71" t="s">
         <v>130</v>
       </c>
-      <c r="G28" s="28">
+      <c r="G28" s="71">
         <v>30000</v>
       </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="F29" s="28" t="s">
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F29" s="71" t="s">
         <v>131</v>
       </c>
-      <c r="G29" s="28">
+      <c r="G29" s="71">
         <v>5590</v>
       </c>
-    </row>
-    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G37">
-        <f>E26-(SUM(G26:G36))</f>
-        <v>267603</v>
+      <c r="H29" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F30" s="71" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="71">
+        <v>10000</v>
+      </c>
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F31" s="71" t="s">
+        <v>133</v>
+      </c>
+      <c r="G31" s="71">
+        <v>3730</v>
+      </c>
+      <c r="H31" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="F32" s="71"/>
+      <c r="G32" s="71"/>
+    </row>
+    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F33" s="71"/>
+      <c r="G33" s="71"/>
+    </row>
+    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F34" s="71"/>
+      <c r="G34" s="71"/>
+    </row>
+    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>E26-(SUM(G26:G39))</f>
+        <v>253873</v>
       </c>
     </row>
   </sheetData>
@@ -4012,7 +4120,7 @@
   <dimension ref="D7:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4126,8 +4234,12 @@
       <c r="E16" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="20"/>
+      <c r="F16" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D17" s="65"/>
@@ -4148,7 +4260,7 @@
       </c>
       <c r="F18" s="14">
         <f>F10-SUM(F11:F17)</f>
-        <v>22500</v>
+        <v>12500</v>
       </c>
       <c r="G18" s="21"/>
     </row>
@@ -4986,10 +5098,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:I42"/>
+  <dimension ref="D7:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5033,7 +5145,7 @@
         <v>110</v>
       </c>
       <c r="F10" s="12">
-        <v>23840</v>
+        <v>25840</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -5060,156 +5172,154 @@
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="68"/>
       <c r="E13" s="19" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="F13" s="12">
-        <v>30000</v>
+        <v>10520</v>
       </c>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D14" s="68"/>
       <c r="E14" s="19" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="F14" s="12">
-        <v>300000</v>
+        <v>30000</v>
       </c>
       <c r="G14" s="20"/>
     </row>
-    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D15" s="68"/>
       <c r="E15" s="19" t="s">
-        <v>85</v>
+        <v>23</v>
       </c>
       <c r="F15" s="12">
-        <v>54100</v>
+        <v>300000</v>
       </c>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D16" s="68"/>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="12">
+        <v>54100</v>
+      </c>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="68"/>
+      <c r="E17" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F16" s="14">
-        <f>SUM(F9:F15)</f>
-        <v>694390</v>
-      </c>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="68"/>
-      <c r="E17" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="41">
-        <v>80000</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>36</v>
-      </c>
+      <c r="F17" s="14">
+        <f>SUM(F9:F16)</f>
+        <v>706910</v>
+      </c>
+      <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D18" s="68"/>
       <c r="E18" s="19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="41">
-        <v>26500</v>
+        <v>80000</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H18" t="s">
-        <v>130</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D19" s="68"/>
       <c r="E19" s="19" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F19" s="41">
-        <v>50000</v>
+        <v>26500</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
+      </c>
+      <c r="H19" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D20" s="68"/>
       <c r="E20" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" s="41">
-        <v>14000</v>
+        <v>50000</v>
       </c>
       <c r="G20" s="20" t="s">
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D21" s="68"/>
       <c r="E21" s="19" t="s">
-        <v>69</v>
+        <v>35</v>
       </c>
       <c r="F21" s="41">
-        <v>5000</v>
+        <v>14000</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" t="s">
-        <v>130</v>
+        <v>77</v>
       </c>
     </row>
     <row r="22" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D22" s="68"/>
       <c r="E22" s="19" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="F22" s="41">
-        <v>27000</v>
+        <v>5000</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>36</v>
+      </c>
+      <c r="H22" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D23" s="68"/>
       <c r="E23" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F23" s="41">
-        <v>50000</v>
+        <v>27000</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="H23" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D24" s="68"/>
       <c r="E24" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F24" s="41">
-        <v>11270</v>
+        <v>50000</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>36</v>
+      </c>
+      <c r="H24" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D25" s="68"/>
       <c r="E25" s="19" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="F25" s="41">
-        <v>21725</v>
+        <v>11270</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>36</v>
@@ -5218,10 +5328,10 @@
     <row r="26" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D26" s="68"/>
       <c r="E26" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F26" s="41">
-        <v>44325</v>
+        <v>21725</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>36</v>
@@ -5230,10 +5340,10 @@
     <row r="27" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D27" s="68"/>
       <c r="E27" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F27" s="41">
-        <v>21560</v>
+        <v>44325</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>36</v>
@@ -5242,10 +5352,10 @@
     <row r="28" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D28" s="68"/>
       <c r="E28" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F28" s="41">
-        <v>7250</v>
+        <v>21560</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>36</v>
@@ -5254,85 +5364,85 @@
     <row r="29" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D29" s="68"/>
       <c r="E29" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F29" s="41">
-        <v>18600</v>
+        <v>7250</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>36</v>
-      </c>
-      <c r="H29" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D30" s="68"/>
       <c r="E30" s="19" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F30" s="41">
-        <v>44325</v>
+        <v>18600</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>36</v>
+      </c>
+      <c r="H30" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D31" s="68"/>
       <c r="E31" s="19" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F31" s="41">
-        <v>1800</v>
+        <v>44325</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>117</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.3">
       <c r="D32" s="68"/>
       <c r="E32" s="19" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F32" s="41">
-        <v>1750</v>
+        <v>1800</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>38</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="68"/>
       <c r="E33" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F33" s="41">
-        <v>21300</v>
+        <v>1750</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>120</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="68"/>
       <c r="E34" s="19" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="F34" s="41">
-        <v>4700</v>
+        <v>21300</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="68"/>
       <c r="E35" s="19" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F35" s="41">
-        <v>5590</v>
+        <v>4700</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>126</v>
@@ -5341,32 +5451,44 @@
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D36" s="68"/>
       <c r="E36" s="19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F36" s="41">
-        <v>30000</v>
+        <v>5590</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>126</v>
       </c>
-      <c r="H36" t="s">
-        <v>130</v>
-      </c>
-      <c r="I36">
-        <v>126500</v>
-      </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37" s="68"/>
-      <c r="E37" s="19"/>
-      <c r="F37" s="41"/>
-      <c r="G37" s="20"/>
+      <c r="E37" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F37" s="41">
+        <v>30000</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H37" t="s">
+        <v>130</v>
+      </c>
+      <c r="I37">
+        <v>126500</v>
+      </c>
     </row>
     <row r="38" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D38" s="68"/>
-      <c r="E38" s="19"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="20"/>
+      <c r="E38" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="41">
+        <v>3730</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="39" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D39" s="68"/>
@@ -5380,32 +5502,38 @@
       <c r="F40" s="41"/>
       <c r="G40" s="20"/>
     </row>
-    <row r="41" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D41" s="68"/>
-      <c r="E41" s="19" t="s">
+      <c r="E41" s="19"/>
+      <c r="F41" s="41"/>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="68"/>
+      <c r="E42" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="F41" s="12">
+      <c r="F42" s="12">
         <v>0</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="42" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="69"/>
-      <c r="E42" s="1" t="s">
+    <row r="43" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="69"/>
+      <c r="E43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F42" s="14">
-        <f>F16-SUM(F17:F41)</f>
-        <v>207695</v>
-      </c>
-      <c r="G42" s="21"/>
+      <c r="F43" s="14">
+        <f>F17-SUM(F18:F42)</f>
+        <v>216485</v>
+      </c>
+      <c r="G43" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D42"/>
+    <mergeCell ref="D9:D43"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added changes as of 12-12-2023
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{386A01BA-2394-490C-9677-6381AF66F7F7}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1835D893-4067-49CD-BD2E-AF7F4B55422C}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -22,7 +22,7 @@
     <sheet name="Grill" sheetId="5" r:id="rId7"/>
     <sheet name="Civil" sheetId="9" r:id="rId8"/>
     <sheet name="Furniture" sheetId="6" r:id="rId9"/>
-    <sheet name="Bathroom &amp; Kitchen" sheetId="7" r:id="rId10"/>
+    <sheet name="Bathroom-Kitchen-Barandah" sheetId="7" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -197,7 +197,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
       <text>
         <r>
           <rPr>
@@ -247,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
       <text>
         <r>
           <rPr>
@@ -271,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
       <text>
         <r>
           <rPr>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
       <text>
         <r>
           <rPr>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
       <text>
         <r>
           <rPr>
@@ -391,7 +391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
       <text>
         <r>
           <rPr>
@@ -415,7 +415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
       <text>
         <r>
           <rPr>
@@ -439,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
       <text>
         <r>
           <rPr>
@@ -574,11 +574,12 @@
 Tentative
 Till now exepnded - 14000+21725+1750 = 37475+3600 (Locks)
 = 41075+4700(Edge Binding) = 45775
- for the section of Louve Glue, rest material - 1730, total till now: 47505</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{87678B8C-756B-4A16-A0B1-A3C2A9059184}">
+ for the section of Louve Glue, rest material - 1730, total till now: 47505
+EdgeBinding Kabja together = 4200, till now 51705</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{8C08C4BE-5E2B-415E-A79C-0CC9A4B263EE}">
       <text>
         <r>
           <rPr>
@@ -598,12 +599,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-tentatively 30000 extra 
-150000+30000</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+10520 (previous)+ estimated 4 louvres,2 laminates, 1 acrylic+9400</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{E3B0DB5E-EFB2-4183-B2C1-99AD1E10DC45}">
       <text>
         <r>
           <rPr>
@@ -623,11 +623,35 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
+Glass works</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
 Bikas Da</t>
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
       <text>
         <r>
           <rPr>
@@ -651,7 +675,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
       <text>
         <r>
           <rPr>
@@ -676,7 +700,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
       <text>
         <r>
           <rPr>
@@ -701,7 +725,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
       <text>
         <r>
           <rPr>
@@ -726,7 +750,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
       <text>
         <r>
           <rPr>
@@ -752,7 +776,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
       <text>
         <r>
           <rPr>
@@ -776,7 +800,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
       <text>
         <r>
           <rPr>
@@ -800,7 +824,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
       <text>
         <r>
           <rPr>
@@ -824,7 +848,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
       <text>
         <r>
           <rPr>
@@ -848,7 +872,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
       <text>
         <r>
           <rPr>
@@ -872,7 +896,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H30" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
+    <comment ref="H31" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
       <text>
         <r>
           <rPr>
@@ -896,7 +920,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
           <rPr>
@@ -920,7 +944,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+    <comment ref="F33" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
       <text>
         <r>
           <rPr>
@@ -944,7 +968,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
       <text>
         <r>
           <rPr>
@@ -969,7 +993,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
       <text>
         <r>
           <rPr>
@@ -996,7 +1020,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
       <text>
         <r>
           <rPr>
@@ -1020,7 +1044,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
       <text>
         <r>
           <rPr>
@@ -1044,7 +1068,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
       <text>
         <r>
           <rPr>
@@ -1068,7 +1092,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I37" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
+    <comment ref="I38" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
       <text>
         <r>
           <rPr>
@@ -1092,7 +1116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
       <text>
         <r>
           <rPr>
@@ -1113,6 +1137,102 @@
           </rPr>
           <t xml:space="preserve">
 Louvre Glue, muskin tapes, heatex and normal glue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas Da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I40" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da till date - 04-12-2023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Edge Binding Kabja</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Anam - 35k advanced</t>
         </r>
       </text>
     </comment>
@@ -1141,7 +1261,151 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{16786DDB-AC57-453B-99D7-248BBA1E2047}">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{9B98C3D4-1986-4726-9F41-505270A064CA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+48k paid till no -01-12-2023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{D6CF9A0F-81C3-4D85-84A2-6CDCDC2723E7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+15k paid out of this - 01-12-2023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{7508B8C7-8A23-4CE9-A886-982714ED9558}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+paid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{53983B98-F7F8-4D5D-8CE9-7EE2559BD2DB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+3200+500 delivery</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{99689982-6292-4165-AD26-14539A18A3BA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+2 types of tiles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{AF35FB86-ED8F-4A26-B190-DD67EF15CFCE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+10k paid till - 01-12-2023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{16786DDB-AC57-453B-99D7-248BBA1E2047}">
       <text>
         <r>
           <rPr>
@@ -1166,7 +1430,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{C647BD32-4C90-4257-AF43-75E2E0686478}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{C647BD32-4C90-4257-AF43-75E2E0686478}">
       <text>
         <r>
           <rPr>
@@ -1192,7 +1456,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{E57FE724-2CA6-4078-A874-BDF0213C3E12}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{E57FE724-2CA6-4078-A874-BDF0213C3E12}">
       <text>
         <r>
           <rPr>
@@ -1216,7 +1480,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{199A5F92-BA83-4DB3-A502-ACEE8B96E2D5}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{199A5F92-BA83-4DB3-A502-ACEE8B96E2D5}">
       <text>
         <r>
           <rPr>
@@ -1242,7 +1506,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{F03B2F0A-2345-4635-B9FB-69E038D76831}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{F03B2F0A-2345-4635-B9FB-69E038D76831}">
       <text>
         <r>
           <rPr>
@@ -1266,7 +1530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{E95C9AF8-5C84-47C1-8E8A-538A8936C269}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{E95C9AF8-5C84-47C1-8E8A-538A8936C269}">
       <text>
         <r>
           <rPr>
@@ -1290,7 +1554,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{A183F4EA-FB59-4730-B241-1696B70A5F95}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{A183F4EA-FB59-4730-B241-1696B70A5F95}">
       <text>
         <r>
           <rPr>
@@ -1317,7 +1581,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{795FE048-63B4-4A28-BEA6-9ED2DFB591E9}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{795FE048-63B4-4A28-BEA6-9ED2DFB591E9}">
       <text>
         <r>
           <rPr>
@@ -1345,7 +1609,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{BFEC1F17-8CE3-44A8-84E4-53A5FE57EDFC}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{BFEC1F17-8CE3-44A8-84E4-53A5FE57EDFC}">
       <text>
         <r>
           <rPr>
@@ -1366,6 +1630,56 @@
           </rPr>
           <t xml:space="preserve">
 kitchen renovation smoothing granites and leveling </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{7D69A899-3C94-4DFE-BDDC-B4CC0BC7AF9E}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+granite First
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{0FC6798B-65E5-4F18-A209-2B4DB72F3A08}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Advance
+for tiles to chinarpark shop</t>
         </r>
       </text>
     </comment>
@@ -1374,7 +1688,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="158">
   <si>
     <t>Provider</t>
   </si>
@@ -1688,18 +2002,9 @@
     <t>Payment -5</t>
   </si>
   <si>
-    <t>5w light - 3 - 240</t>
-  </si>
-  <si>
     <t>3w light - 47 - 140</t>
   </si>
   <si>
-    <t>2w light - 9 -100</t>
-  </si>
-  <si>
-    <t>Driver - 5 - 120 (2 ampere smps)</t>
-  </si>
-  <si>
     <t>Sliding for parents room</t>
   </si>
   <si>
@@ -1715,9 +2020,6 @@
     <t>Payment - 16</t>
   </si>
   <si>
-    <t xml:space="preserve">Profiles - 14 mm - 9 - 180 each </t>
-  </si>
-  <si>
     <t>Payment - 17</t>
   </si>
   <si>
@@ -1779,6 +2081,87 @@
   </si>
   <si>
     <t>Sections</t>
+  </si>
+  <si>
+    <t>Sahid- Granite 1</t>
+  </si>
+  <si>
+    <t>Bikas da</t>
+  </si>
+  <si>
+    <t>Payment - 23</t>
+  </si>
+  <si>
+    <t>Payment - 24</t>
+  </si>
+  <si>
+    <t>Edge Binding (Furninture)&amp;kabja</t>
+  </si>
+  <si>
+    <t>Big Tiles</t>
+  </si>
+  <si>
+    <t>Raw material Handles</t>
+  </si>
+  <si>
+    <t>Majuri for barandah</t>
+  </si>
+  <si>
+    <t>Tiles for verandah</t>
+  </si>
+  <si>
+    <t>Erfan &amp; Anam (toughened)</t>
+  </si>
+  <si>
+    <t>Payment - 25</t>
+  </si>
+  <si>
+    <t>Anam Toughned Glass Advanced</t>
+  </si>
+  <si>
+    <t>Spent</t>
+  </si>
+  <si>
+    <t>5w light - 6 - 240</t>
+  </si>
+  <si>
+    <t>2w light - 30 -100</t>
+  </si>
+  <si>
+    <t>Led Strip Lights Profile -250(240 bulbs)- 8 piece - Warm</t>
+  </si>
+  <si>
+    <t>Led Strip Lights Profile -250(240 bulbs)- 2 piece - White</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Profiles - 14 mm - 11 - 180 each </t>
+  </si>
+  <si>
+    <t>Drivers - 13- 430 -(10 ampere smps)</t>
+  </si>
+  <si>
+    <t>Driver - 8 - 120 (2 ampere smps)</t>
+  </si>
+  <si>
+    <t>Santras for Room and barandah</t>
+  </si>
+  <si>
+    <t>Tiles Advance</t>
+  </si>
+  <si>
+    <t>Bathroom-Kitchen-Baranah</t>
+  </si>
+  <si>
+    <t>Remaining Self to Pay</t>
+  </si>
+  <si>
+    <t>Remaining Total to Pay</t>
+  </si>
+  <si>
+    <t>Remainig Bank to Pay</t>
+  </si>
+  <si>
+    <t>Bank To Pay in Total</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +2301,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -2220,15 +2603,58 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -2236,7 +2662,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2341,6 +2767,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2383,8 +2814,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2635,6 +3066,30 @@
 </file>
 
 <file path=xl/persons/person60.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person61.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person62.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person63.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person64.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person65.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person66.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -2949,8 +3404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
   <dimension ref="C7:Q27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2982,7 +3437,7 @@
         <v>63</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="J8" s="45" t="s">
         <v>64</v>
@@ -3080,11 +3535,11 @@
         <v>29</v>
       </c>
       <c r="F12">
-        <f>'Electric &amp; Lights'!F27</f>
-        <v>145884</v>
+        <f>'Electric &amp; Lights'!F30</f>
+        <v>152354</v>
       </c>
       <c r="G12">
-        <f>SUM('Electric &amp; Lights'!F28:F39)</f>
+        <f>SUM('Electric &amp; Lights'!F31:F42)</f>
         <v>140884</v>
       </c>
       <c r="H12">
@@ -3096,7 +3551,7 @@
       </c>
       <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>11470</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.3">
@@ -3108,7 +3563,7 @@
       </c>
       <c r="F13">
         <f>Grill!F15</f>
-        <v>115000</v>
+        <v>114000</v>
       </c>
       <c r="G13">
         <f>SUM(Grill!F16:F21)</f>
@@ -3123,7 +3578,7 @@
       </c>
       <c r="K13" s="4">
         <f t="shared" si="0"/>
-        <v>26000</v>
+        <v>25000</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.3">
@@ -3134,18 +3589,18 @@
         <v>27</v>
       </c>
       <c r="F14">
-        <f>Furniture!F17</f>
-        <v>706910</v>
+        <f>Furniture!F18</f>
+        <v>739095</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F18:F42)</f>
-        <v>490425</v>
+        <f>SUM(Furniture!F19:F45)</f>
+        <v>539625</v>
       </c>
       <c r="H14">
         <v>46050</v>
       </c>
       <c r="I14">
-        <v>49320</v>
+        <v>98520</v>
       </c>
       <c r="J14">
         <f>SUM(M25:M27)</f>
@@ -3153,7 +3608,7 @@
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>216485</v>
+        <v>199470</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
@@ -3164,15 +3619,18 @@
         <v>82</v>
       </c>
       <c r="F15">
-        <f>'Bathroom &amp; Kitchen'!F17</f>
-        <v>295900</v>
+        <f>'Bathroom-Kitchen-Barandah'!F21</f>
+        <v>312950</v>
       </c>
       <c r="G15">
-        <f>SUM('Bathroom &amp; Kitchen'!F18:F29)</f>
-        <v>228900</v>
+        <f>SUM('Bathroom-Kitchen-Barandah'!F22:F33)</f>
+        <v>247900</v>
       </c>
       <c r="H15">
         <v>129000</v>
+      </c>
+      <c r="I15">
+        <v>19000</v>
       </c>
       <c r="J15">
         <f>SUM(N25:N27)</f>
@@ -3180,7 +3638,7 @@
       </c>
       <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>67000</v>
+        <v>65050</v>
       </c>
     </row>
     <row r="16" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3217,11 +3675,11 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1813473</v>
+        <v>1868178</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1486488</v>
+        <v>1554688</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
@@ -3229,7 +3687,7 @@
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>59320</v>
+        <v>127520</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(J9:J16)</f>
@@ -3237,12 +3695,12 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>326985</v>
+        <v>313490</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E18" s="29" t="s">
-        <v>36</v>
+        <v>157</v>
       </c>
       <c r="F18" s="29">
         <v>1213000</v>
@@ -3254,36 +3712,54 @@
       </c>
       <c r="F19" s="28">
         <f>SUM(H17,I17)</f>
-        <v>356488</v>
+        <v>424688</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E20" s="28" t="s">
-        <v>10</v>
+        <v>154</v>
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>243985</v>
+        <v>230490</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="E21" s="74" t="s">
+        <v>155</v>
+      </c>
+      <c r="F21" s="28">
+        <f>K17</f>
+        <v>313490</v>
+      </c>
+    </row>
+    <row r="22" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="E22" s="74" t="s">
+        <v>156</v>
+      </c>
+      <c r="F22" s="28">
+        <f>F21-F20</f>
+        <v>83000</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="56" t="s">
+      <c r="C23" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="56"/>
-      <c r="E23" s="56"/>
-      <c r="F23" s="56"/>
-      <c r="G23" s="56"/>
-      <c r="H23" s="56"/>
-      <c r="I23" s="56"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="56"/>
-      <c r="P23" s="56"/>
-      <c r="Q23" s="56"/>
+      <c r="D23" s="59"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+      <c r="L23" s="59"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="59"/>
+      <c r="P23" s="59"/>
+      <c r="Q23" s="59"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" s="33" t="s">
@@ -3309,7 +3785,7 @@
         <v>50</v>
       </c>
       <c r="K24" s="37" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="L24" s="37" t="s">
         <v>17</v>
@@ -3472,10 +3948,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD019853-AAD7-4C4A-AE9D-387A8C77D1D3}">
-  <dimension ref="D7:G30"/>
+  <dimension ref="D7:G34"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3502,7 +3978,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="67" t="s">
         <v>62</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -3514,7 +3990,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="11" t="s">
         <v>24</v>
       </c>
@@ -3524,7 +4000,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="11" t="s">
         <v>67</v>
       </c>
@@ -3534,7 +4010,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="11" t="s">
         <v>80</v>
       </c>
@@ -3544,7 +4020,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="11" t="s">
         <v>81</v>
       </c>
@@ -3554,7 +4030,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="65"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="11" t="s">
         <v>84</v>
       </c>
@@ -3564,7 +4040,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="65"/>
+      <c r="D15" s="68"/>
       <c r="E15" s="11" t="s">
         <v>83</v>
       </c>
@@ -3573,173 +4049,221 @@
       </c>
       <c r="G15" s="20"/>
     </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="65"/>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="68"/>
       <c r="E16" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="F16" s="32">
+        <v>3700</v>
+      </c>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="68"/>
+      <c r="E17" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F17" s="32">
+        <v>6500</v>
+      </c>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="68"/>
+      <c r="E18" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="F18" s="32">
+        <v>2000</v>
+      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="68"/>
+      <c r="E19" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="F19" s="32">
+        <v>4850</v>
+      </c>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="68"/>
+      <c r="E20" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F20" s="12">
         <v>15000</v>
       </c>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="65"/>
-      <c r="E17" s="13" t="s">
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="68"/>
+      <c r="E21" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="14">
-        <f>SUM(F9:F16)</f>
-        <v>295900</v>
-      </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="65"/>
-      <c r="E18" s="11" t="s">
+      <c r="F21" s="14">
+        <f>SUM(F9:F20)</f>
+        <v>312950</v>
+      </c>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="68"/>
+      <c r="E22" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="41">
+      <c r="F22" s="41">
         <v>50000</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G22" s="20" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="65"/>
-      <c r="E19" s="11" t="s">
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="68"/>
+      <c r="E23" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="41">
+      <c r="F23" s="41">
         <v>23500</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="65"/>
-      <c r="E20" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="41">
-        <v>50000</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="65"/>
-      <c r="E21" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="F21" s="41">
-        <v>40000</v>
-      </c>
-      <c r="G21" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="65"/>
-      <c r="E22" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="41">
-        <v>2300</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="65"/>
-      <c r="E23" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F23" s="41">
-        <v>5500</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="65"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="11" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
       <c r="F24" s="41">
         <v>50000</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="65"/>
+      <c r="D25" s="68"/>
       <c r="E25" s="11" t="s">
-        <v>78</v>
+        <v>35</v>
       </c>
       <c r="F25" s="41">
-        <v>6000</v>
+        <v>40000</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="65"/>
+      <c r="D26" s="68"/>
       <c r="E26" s="11" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F26" s="41">
-        <v>1600</v>
+        <v>2300</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="65"/>
+      <c r="D27" s="68"/>
       <c r="E27" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="F27" s="41">
+        <v>5500</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="68"/>
+      <c r="E28" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="41">
+        <v>50000</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D29" s="68"/>
+      <c r="E29" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="F29" s="41">
+        <v>6000</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D30" s="68"/>
+      <c r="E30" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="F30" s="41">
+        <v>1600</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="68"/>
+      <c r="E31" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="F27" s="41"/>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="65"/>
-      <c r="E28" s="11" t="s">
+      <c r="F31" s="41">
+        <v>15000</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="68"/>
+      <c r="E32" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="F28" s="41"/>
-      <c r="G28" s="20"/>
-    </row>
-    <row r="29" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D29" s="65"/>
-      <c r="E29" s="11" t="s">
+      <c r="F32" s="41">
+        <v>4000</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="68"/>
+      <c r="E33" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F29" s="12"/>
-      <c r="G29" s="20"/>
-    </row>
-    <row r="30" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D30" s="66"/>
-      <c r="E30" s="13" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="69"/>
+      <c r="E34" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F30" s="14">
-        <f>F17-SUM(F18:F29)</f>
-        <v>67000</v>
-      </c>
-      <c r="G30" s="21"/>
+      <c r="F34" s="14">
+        <f>F21-SUM(F22:F33)</f>
+        <v>65050</v>
+      </c>
+      <c r="G34" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D30"/>
+    <mergeCell ref="D9:D34"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3749,33 +4273,33 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:H40"/>
+  <dimension ref="D6:I42"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="4" max="5" width="24.77734375" customWidth="1"/>
     <col min="6" max="6" width="26.77734375" customWidth="1"/>
-    <col min="8" max="8" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="24.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
-      <c r="G7" s="63"/>
+      <c r="E7" s="65"/>
+      <c r="F7" s="65"/>
+      <c r="G7" s="66"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="59">
+      <c r="E8" s="62">
         <v>45000</v>
       </c>
       <c r="F8" s="48" t="s">
@@ -3786,8 +4310,8 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="58"/>
-      <c r="E9" s="60"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="63"/>
       <c r="F9" s="28" t="s">
         <v>16</v>
       </c>
@@ -3796,8 +4320,8 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="58"/>
-      <c r="E10" s="60"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="63"/>
       <c r="F10" s="47" t="s">
         <v>56</v>
       </c>
@@ -3846,8 +4370,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D19" s="55" t="s">
         <v>66</v>
       </c>
@@ -3861,7 +4385,7 @@
         <v>23500</v>
       </c>
     </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D20" s="51"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
@@ -3871,19 +4395,19 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D21" s="51"/>
       <c r="E21" s="28"/>
       <c r="F21" s="28"/>
       <c r="G21" s="50"/>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D22" s="51"/>
       <c r="E22" s="28"/>
       <c r="F22" s="28"/>
       <c r="G22" s="50"/>
     </row>
-    <row r="23" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D23" s="52"/>
       <c r="E23" s="53"/>
       <c r="F23" s="53" t="s">
@@ -3894,94 +4418,152 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="E26" s="28">
+    <row r="24" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="25" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D25" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" s="57">
         <v>313193</v>
       </c>
-      <c r="F26" s="70" t="s">
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57" t="s">
+        <v>130</v>
+      </c>
+      <c r="I25" s="58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F26" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G26" s="70">
+      <c r="G26" s="29">
         <v>5300</v>
       </c>
-      <c r="H26" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F27" s="71" t="s">
+      <c r="H26" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="I26">
+        <f>SUM(G26:G41)</f>
+        <v>127520</v>
+      </c>
+    </row>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F27" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="G27" s="28">
+        <v>4700</v>
+      </c>
+      <c r="H27" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F28" s="28" t="s">
+        <v>126</v>
+      </c>
+      <c r="G28" s="28">
+        <v>30000</v>
+      </c>
+      <c r="H28" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F29" s="28" t="s">
         <v>127</v>
       </c>
-      <c r="G27" s="71">
-        <v>4700</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="G29" s="28">
+        <v>5590</v>
+      </c>
+      <c r="H29" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F28" s="71" t="s">
-        <v>130</v>
-      </c>
-      <c r="G28" s="71">
-        <v>30000</v>
-      </c>
-      <c r="H28" t="s">
+    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F30" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="G30" s="28">
+        <v>10000</v>
+      </c>
+      <c r="H30" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F31" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="G31" s="28">
+        <v>3730</v>
+      </c>
+      <c r="H31" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F29" s="71" t="s">
+    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F32" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="G29" s="71">
-        <v>5590</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="G32" s="28">
+        <v>15000</v>
+      </c>
+      <c r="H32" s="73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F33" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="G33" s="28">
+        <v>10000</v>
+      </c>
+      <c r="H33" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F30" s="71" t="s">
-        <v>12</v>
-      </c>
-      <c r="G30" s="71">
-        <v>10000</v>
-      </c>
-      <c r="H30" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F31" s="71" t="s">
-        <v>133</v>
-      </c>
-      <c r="G31" s="71">
-        <v>3730</v>
-      </c>
-      <c r="H31" t="s">
+    <row r="34" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F34" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="G34" s="28">
+        <v>4200</v>
+      </c>
+      <c r="H34" s="28" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="F32" s="71"/>
-      <c r="G32" s="71"/>
-    </row>
-    <row r="33" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F33" s="71"/>
-      <c r="G33" s="71"/>
-    </row>
-    <row r="34" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="F34" s="71"/>
-      <c r="G34" s="71"/>
-    </row>
-    <row r="40" spans="6:7" x14ac:dyDescent="0.3">
-      <c r="G40">
-        <f>E26-(SUM(G26:G39))</f>
-        <v>253873</v>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F35" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="G35" s="28">
+        <v>35000</v>
+      </c>
+      <c r="H35" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F36" s="73" t="s">
+        <v>152</v>
+      </c>
+      <c r="G36" s="73">
+        <v>4000</v>
+      </c>
+      <c r="H36" s="73" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="G42">
+        <f>E25-(SUM(G26:G41))</f>
+        <v>185673</v>
       </c>
     </row>
   </sheetData>
@@ -4027,7 +4609,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="67" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -4039,7 +4621,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" t="s">
         <v>4</v>
       </c>
@@ -4049,7 +4631,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
@@ -4060,7 +4642,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" t="s">
         <v>7</v>
       </c>
@@ -4072,7 +4654,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" t="s">
         <v>8</v>
       </c>
@@ -4084,7 +4666,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="65"/>
+      <c r="D14" s="68"/>
       <c r="E14" t="s">
         <v>9</v>
       </c>
@@ -4096,7 +4678,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="66"/>
+      <c r="D15" s="69"/>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
@@ -4147,7 +4729,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="67" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -4159,7 +4741,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
@@ -4170,7 +4752,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
@@ -4182,7 +4764,7 @@
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="11" t="s">
         <v>31</v>
       </c>
@@ -4194,7 +4776,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="11" t="s">
         <v>101</v>
       </c>
@@ -4206,7 +4788,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="65"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="11" t="s">
         <v>102</v>
       </c>
@@ -4214,11 +4796,11 @@
         <v>5000</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="65"/>
+      <c r="D15" s="68"/>
       <c r="E15" s="11" t="s">
         <v>103</v>
       </c>
@@ -4230,21 +4812,21 @@
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="65"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="11" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F16" s="41">
         <v>10000</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="65"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="11" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="F17" s="12">
         <v>0</v>
@@ -4254,7 +4836,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="66"/>
+      <c r="D18" s="69"/>
       <c r="E18" s="13" t="s">
         <v>13</v>
       </c>
@@ -4306,7 +4888,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="67" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -4318,7 +4900,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
@@ -4329,7 +4911,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="11" t="s">
         <v>32</v>
       </c>
@@ -4341,7 +4923,7 @@
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="11" t="s">
         <v>34</v>
       </c>
@@ -4353,7 +4935,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="11" t="s">
         <v>33</v>
       </c>
@@ -4365,7 +4947,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="66"/>
+      <c r="D14" s="69"/>
       <c r="E14" s="13" t="s">
         <v>13</v>
       </c>
@@ -4385,10 +4967,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1544B4-216C-4DA0-B248-9403EAEF3872}">
-  <dimension ref="D7:G40"/>
+  <dimension ref="D7:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4415,7 +4997,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="64" t="s">
+      <c r="D9" s="67" t="s">
         <v>61</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -4427,17 +5009,17 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="11" t="s">
-        <v>104</v>
+        <v>144</v>
       </c>
       <c r="F10" s="12">
-        <v>720</v>
+        <v>1440</v>
       </c>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" t="s">
         <v>74</v>
       </c>
@@ -4447,9 +5029,9 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" s="4">
         <v>6580</v>
@@ -4457,17 +5039,17 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>145</v>
       </c>
       <c r="F13" s="4">
-        <v>900</v>
+        <v>3000</v>
       </c>
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="65"/>
+      <c r="D14" s="68"/>
       <c r="E14" t="s">
         <v>75</v>
       </c>
@@ -4477,7 +5059,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="65"/>
+      <c r="D15" s="68"/>
       <c r="E15" t="s">
         <v>87</v>
       </c>
@@ -4487,7 +5069,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="65"/>
+      <c r="D16" s="68"/>
       <c r="E16" t="s">
         <v>86</v>
       </c>
@@ -4497,268 +5079,298 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="65"/>
+      <c r="D17" s="68"/>
       <c r="E17" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2000</v>
+      </c>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="68"/>
+      <c r="E18" t="s">
+        <v>147</v>
+      </c>
+      <c r="F18" s="4">
+        <v>500</v>
+      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="68"/>
+      <c r="E19" t="s">
         <v>88</v>
       </c>
-      <c r="F17" s="4">
+      <c r="F19" s="4">
         <v>2040</v>
       </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="65"/>
-      <c r="E18" t="s">
-        <v>113</v>
-      </c>
-      <c r="F18" s="4">
-        <v>1620</v>
-      </c>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="65"/>
-      <c r="E19" t="s">
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="68"/>
+      <c r="E20" t="s">
+        <v>148</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1980</v>
+      </c>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="68"/>
+      <c r="E21" t="s">
         <v>92</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="65"/>
-      <c r="E20" t="s">
+      <c r="F21" s="4"/>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D22" s="68"/>
+      <c r="E22" t="s">
         <v>90</v>
       </c>
-      <c r="F20" s="4">
+      <c r="F22" s="4">
         <v>2940</v>
       </c>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="65"/>
-      <c r="E21" t="s">
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D23" s="68"/>
+      <c r="E23" t="s">
         <v>89</v>
       </c>
-      <c r="F21" s="4">
+      <c r="F23" s="4">
         <v>5720</v>
       </c>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="65"/>
-      <c r="E22" t="s">
-        <v>107</v>
-      </c>
-      <c r="F22" s="4">
-        <v>600</v>
-      </c>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="65"/>
-      <c r="E23" t="s">
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D24" s="68"/>
+      <c r="E24" t="s">
+        <v>149</v>
+      </c>
+      <c r="F24" s="4">
+        <v>430</v>
+      </c>
+      <c r="G24" s="20"/>
+    </row>
+    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D25" s="68"/>
+      <c r="E25" t="s">
+        <v>150</v>
+      </c>
+      <c r="F25" s="4">
+        <v>960</v>
+      </c>
+      <c r="G25" s="20"/>
+    </row>
+    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D26" s="68"/>
+      <c r="E26" t="s">
         <v>71</v>
       </c>
-      <c r="F23" s="4">
+      <c r="F26" s="4">
         <v>26960</v>
       </c>
-      <c r="G23" s="20"/>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="65"/>
-      <c r="E24" t="s">
+      <c r="G26" s="20"/>
+    </row>
+    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D27" s="68"/>
+      <c r="E27" t="s">
         <v>72</v>
       </c>
-      <c r="F24" s="4">
+      <c r="F27" s="4">
         <v>31754</v>
       </c>
-      <c r="G24" s="20"/>
-    </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="65"/>
-      <c r="E25" t="s">
+      <c r="G27" s="20"/>
+    </row>
+    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D28" s="68"/>
+      <c r="E28" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="4">
+      <c r="F28" s="4">
         <v>27000</v>
       </c>
-      <c r="G25" s="20"/>
-    </row>
-    <row r="26" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D26" s="65"/>
-      <c r="E26" t="s">
+      <c r="G28" s="20"/>
+    </row>
+    <row r="29" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D29" s="68"/>
+      <c r="E29" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="4">
+      <c r="F29" s="4">
         <v>15350</v>
       </c>
-      <c r="G26" s="20"/>
-    </row>
-    <row r="27" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D27" s="65"/>
-      <c r="E27" s="1" t="s">
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D30" s="68"/>
+      <c r="E30" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="3">
-        <f>SUM(F9:F26)</f>
-        <v>145884</v>
-      </c>
-      <c r="G27" s="20"/>
-    </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="65"/>
-      <c r="E28" t="s">
+      <c r="F30" s="3">
+        <f>SUM(F9:F29)</f>
+        <v>152354</v>
+      </c>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="68"/>
+      <c r="E31" t="s">
         <v>32</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F31" s="41">
         <v>16345</v>
       </c>
-      <c r="G28" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="65"/>
-      <c r="E29" t="s">
+    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="68"/>
+      <c r="E32" t="s">
         <v>34</v>
       </c>
-      <c r="F29" s="41">
+      <c r="F32" s="41">
         <v>11088</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="65"/>
-      <c r="E30" t="s">
-        <v>33</v>
-      </c>
-      <c r="F30" s="41">
-        <v>4100</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="65"/>
-      <c r="E31" t="s">
-        <v>35</v>
-      </c>
-      <c r="F31" s="41">
-        <v>6903</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="65"/>
-      <c r="E32" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="41">
-        <v>36280</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D33" s="65"/>
+      <c r="D33" s="68"/>
       <c r="E33" t="s">
-        <v>70</v>
+        <v>33</v>
       </c>
       <c r="F33" s="41">
-        <v>8805</v>
+        <v>4100</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D34" s="65"/>
+      <c r="D34" s="68"/>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
       <c r="F34" s="41">
-        <v>31700</v>
+        <v>6903</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="65"/>
+      <c r="D35" s="68"/>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F35" s="41">
-        <v>15350</v>
+        <v>36280</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="65"/>
+      <c r="D36" s="68"/>
       <c r="E36" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F36" s="41">
-        <v>5454</v>
+        <v>8805</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="65"/>
+      <c r="D37" s="68"/>
       <c r="E37" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="F37" s="41">
-        <v>2859</v>
+        <v>31700</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="65"/>
+      <c r="D38" s="68"/>
       <c r="E38" t="s">
+        <v>78</v>
+      </c>
+      <c r="F38" s="41">
+        <v>15350</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="68"/>
+      <c r="E39" t="s">
+        <v>79</v>
+      </c>
+      <c r="F39" s="41">
+        <v>5454</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="68"/>
+      <c r="E40" t="s">
+        <v>96</v>
+      </c>
+      <c r="F40" s="41">
+        <v>2859</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D41" s="68"/>
+      <c r="E41" t="s">
         <v>97</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F41" s="41">
         <v>2000</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G41" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="39" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="65"/>
-      <c r="E39" t="s">
+    <row r="42" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="68"/>
+      <c r="E42" t="s">
         <v>98</v>
       </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D40" s="66"/>
-      <c r="E40" s="1" t="s">
+      <c r="F42" s="4"/>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="69"/>
+      <c r="E43" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F40" s="3">
-        <f>F27-SUM(F28:F39)</f>
-        <v>5000</v>
-      </c>
-      <c r="G40" s="21"/>
+      <c r="F43" s="3">
+        <f>F30-SUM(F31:F42)</f>
+        <v>11470</v>
+      </c>
+      <c r="G43" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D40"/>
+    <mergeCell ref="D9:D43"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4771,7 +5383,7 @@
   <dimension ref="D7:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F16:F20"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4798,8 +5410,8 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="64" t="s">
-        <v>16</v>
+      <c r="D9" s="67" t="s">
+        <v>140</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>17</v>
@@ -4810,17 +5422,17 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="12">
-        <v>20000</v>
+        <v>19000</v>
       </c>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="11" t="s">
         <v>18</v>
       </c>
@@ -4830,7 +5442,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="11" t="s">
         <v>44</v>
       </c>
@@ -4840,9 +5452,9 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="F13" s="12">
         <v>15000</v>
@@ -4850,7 +5462,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="65"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="11" t="s">
         <v>20</v>
       </c>
@@ -4860,18 +5472,18 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="65"/>
+      <c r="D15" s="68"/>
       <c r="E15" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="14">
         <f>SUM(F9:F14)</f>
-        <v>115000</v>
+        <v>114000</v>
       </c>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="65"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="11" t="s">
         <v>32</v>
       </c>
@@ -4883,7 +5495,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="65"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="11" t="s">
         <v>34</v>
       </c>
@@ -4895,7 +5507,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="65"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="11" t="s">
         <v>33</v>
       </c>
@@ -4907,7 +5519,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="65"/>
+      <c r="D19" s="68"/>
       <c r="E19" s="11" t="s">
         <v>35</v>
       </c>
@@ -4919,7 +5531,7 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="65"/>
+      <c r="D20" s="68"/>
       <c r="E20" s="11" t="s">
         <v>69</v>
       </c>
@@ -4931,7 +5543,7 @@
       </c>
     </row>
     <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="65"/>
+      <c r="D21" s="68"/>
       <c r="E21" s="11" t="s">
         <v>70</v>
       </c>
@@ -4939,13 +5551,13 @@
       <c r="G21" s="4"/>
     </row>
     <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="66"/>
+      <c r="D22" s="69"/>
       <c r="E22" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F22" s="44">
         <f>F15-SUM(F16:F21)</f>
-        <v>26000</v>
+        <v>25000</v>
       </c>
       <c r="G22" s="21"/>
     </row>
@@ -4989,8 +5601,8 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="64" t="s">
-        <v>109</v>
+      <c r="D9" s="67" t="s">
+        <v>106</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>40</v>
@@ -5001,7 +5613,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="65"/>
+      <c r="D10" s="68"/>
       <c r="E10" s="31" t="s">
         <v>43</v>
       </c>
@@ -5011,7 +5623,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="65"/>
+      <c r="D11" s="68"/>
       <c r="E11" s="11" t="s">
         <v>28</v>
       </c>
@@ -5019,7 +5631,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="65"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
@@ -5030,7 +5642,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="65"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="11" t="s">
         <v>32</v>
       </c>
@@ -5042,7 +5654,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="65"/>
+      <c r="D14" s="68"/>
       <c r="E14" s="11" t="s">
         <v>34</v>
       </c>
@@ -5054,7 +5666,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="65"/>
+      <c r="D15" s="68"/>
       <c r="E15" s="11" t="s">
         <v>33</v>
       </c>
@@ -5066,7 +5678,7 @@
       </c>
     </row>
     <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="65"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="11" t="s">
         <v>35</v>
       </c>
@@ -5078,7 +5690,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="66"/>
+      <c r="D17" s="69"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
       </c>
@@ -5098,10 +5710,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:I43"/>
+  <dimension ref="D7:J46"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M37" sqref="M37"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5128,7 +5740,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="70" t="s">
         <v>21</v>
       </c>
       <c r="E9" s="18" t="s">
@@ -5140,9 +5752,9 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="68"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="19" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="F10" s="12">
         <v>25840</v>
@@ -5150,7 +5762,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="68"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="19" t="s">
         <v>94</v>
       </c>
@@ -5160,380 +5772,428 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="68"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F12" s="12">
+        <v>51705</v>
+      </c>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="71"/>
+      <c r="E13" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="F13" s="12">
+        <v>16000</v>
+      </c>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="71"/>
+      <c r="E14" s="19" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="71"/>
+      <c r="E15" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="F15" s="12">
+        <v>55000</v>
+      </c>
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="71"/>
+      <c r="E16" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="F16" s="12">
+        <v>300000</v>
+      </c>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="71"/>
+      <c r="E17" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="12">
+        <v>54100</v>
+      </c>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="71"/>
+      <c r="E18" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="14">
+        <f>SUM(F9:F17)</f>
+        <v>739095</v>
+      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="71"/>
+      <c r="E19" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" s="41">
+        <v>80000</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="71"/>
+      <c r="E20" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F20" s="41">
+        <v>26500</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="H20" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="71"/>
+      <c r="E21" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="41">
         <v>50000</v>
       </c>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="68"/>
-      <c r="E13" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F13" s="12">
-        <v>10520</v>
-      </c>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="68"/>
-      <c r="E14" s="19" t="s">
-        <v>123</v>
-      </c>
-      <c r="F14" s="12">
-        <v>30000</v>
-      </c>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="68"/>
-      <c r="E15" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F15" s="12">
-        <v>300000</v>
-      </c>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="68"/>
-      <c r="E16" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F16" s="12">
-        <v>54100</v>
-      </c>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="68"/>
-      <c r="E17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" s="14">
-        <f>SUM(F9:F16)</f>
-        <v>706910</v>
-      </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="68"/>
-      <c r="E18" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F18" s="41">
-        <v>80000</v>
-      </c>
-      <c r="G18" s="20" t="s">
+      <c r="G21" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="68"/>
-      <c r="E19" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F19" s="41">
-        <v>26500</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D20" s="68"/>
-      <c r="E20" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F20" s="41">
-        <v>50000</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D21" s="68"/>
-      <c r="E21" s="19" t="s">
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="71"/>
+      <c r="E22" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="41">
+      <c r="F22" s="41">
         <v>14000</v>
       </c>
-      <c r="G21" s="20" t="s">
+      <c r="G22" s="20" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D22" s="68"/>
-      <c r="E22" s="19" t="s">
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="71"/>
+      <c r="E23" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="F22" s="41">
+      <c r="F23" s="41">
         <v>5000</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="68"/>
-      <c r="E23" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="F23" s="41">
-        <v>27000</v>
       </c>
       <c r="G23" s="20" t="s">
         <v>36</v>
       </c>
+      <c r="H23" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="24" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D24" s="68"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F24" s="41">
-        <v>50000</v>
+        <v>27000</v>
       </c>
       <c r="G24" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H24" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="25" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D25" s="68"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25" s="41">
-        <v>11270</v>
+        <v>50000</v>
       </c>
       <c r="G25" s="20" t="s">
         <v>36</v>
       </c>
+      <c r="H25" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="26" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="68"/>
+      <c r="D26" s="71"/>
       <c r="E26" s="19" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="F26" s="41">
-        <v>21725</v>
+        <v>11270</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="27" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="68"/>
+      <c r="D27" s="71"/>
       <c r="E27" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F27" s="41">
-        <v>44325</v>
+        <v>21725</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D28" s="68"/>
+      <c r="D28" s="71"/>
       <c r="E28" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F28" s="41">
-        <v>21560</v>
+        <v>44325</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="68"/>
+      <c r="D29" s="71"/>
       <c r="E29" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F29" s="41">
-        <v>7250</v>
+        <v>21560</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D30" s="68"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="19" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F30" s="41">
-        <v>18600</v>
+        <v>7250</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="H30" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D31" s="68"/>
+      <c r="D31" s="71"/>
       <c r="E31" s="19" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="F31" s="41">
-        <v>44325</v>
+        <v>18600</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>36</v>
       </c>
+      <c r="H31" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D32" s="68"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="19" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F32" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D33" s="71"/>
+      <c r="E33" s="19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F33" s="41">
         <v>1800</v>
       </c>
-      <c r="G32" s="20" t="s">
+      <c r="G33" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D34" s="71"/>
+      <c r="E34" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="41">
+        <v>1750</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D35" s="71"/>
+      <c r="E35" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="F35" s="41">
+        <v>21300</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D36" s="71"/>
+      <c r="E36" s="19" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D33" s="68"/>
-      <c r="E33" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="F33" s="41">
-        <v>1750</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="68"/>
-      <c r="E34" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" s="41">
-        <v>21300</v>
-      </c>
-      <c r="G34" s="20" t="s">
+      <c r="F36" s="41">
+        <v>4700</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D37" s="71"/>
+      <c r="E37" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="41">
+        <v>5590</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D38" s="71"/>
+      <c r="E38" s="19" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D35" s="68"/>
-      <c r="E35" s="19" t="s">
+      <c r="F38" s="41">
+        <v>30000</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H38" t="s">
+        <v>126</v>
+      </c>
+      <c r="I38">
+        <v>126500</v>
+      </c>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D39" s="71"/>
+      <c r="E39" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="F35" s="41">
-        <v>4700</v>
-      </c>
-      <c r="G35" s="20" t="s">
+      <c r="F39" s="41">
+        <v>3730</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D40" s="71"/>
+      <c r="E40" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="F40" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="H40" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="68"/>
-      <c r="E36" s="19" t="s">
+      <c r="I40">
+        <v>136500</v>
+      </c>
+      <c r="J40">
+        <f>F16-I40</f>
+        <v>163500</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D41" s="71"/>
+      <c r="E41" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F41" s="41">
+        <v>4200</v>
+      </c>
+      <c r="G41" s="20" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="41">
-        <v>5590</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D37" s="68"/>
-      <c r="E37" s="19" t="s">
-        <v>124</v>
-      </c>
-      <c r="F37" s="41">
-        <v>30000</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>126</v>
-      </c>
-      <c r="H37" t="s">
-        <v>130</v>
-      </c>
-      <c r="I37">
-        <v>126500</v>
-      </c>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D38" s="68"/>
-      <c r="E38" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F38" s="41">
-        <v>3730</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D39" s="68"/>
-      <c r="E39" s="19"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D40" s="68"/>
-      <c r="E40" s="19"/>
-      <c r="F40" s="41"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D41" s="68"/>
-      <c r="E41" s="19"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="68"/>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D42" s="71"/>
       <c r="E42" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="F42" s="12">
+        <v>141</v>
+      </c>
+      <c r="F42" s="41">
+        <v>35000</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D43" s="71"/>
+      <c r="E43" s="19"/>
+      <c r="F43" s="41"/>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D44" s="71"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="41"/>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="45" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D45" s="71"/>
+      <c r="E45" s="19" t="s">
+        <v>121</v>
+      </c>
+      <c r="F45" s="12">
         <v>0</v>
       </c>
-      <c r="G42" s="20" t="s">
+      <c r="G45" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D43" s="69"/>
-      <c r="E43" s="1" t="s">
+    <row r="46" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D46" s="72"/>
+      <c r="E46" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F43" s="14">
-        <f>F17-SUM(F18:F42)</f>
-        <v>216485</v>
-      </c>
-      <c r="G43" s="21"/>
+      <c r="F46" s="14">
+        <f>F18-SUM(F19:F45)</f>
+        <v>199470</v>
+      </c>
+      <c r="G46" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D43"/>
+    <mergeCell ref="D9:D46"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated as of 30-12-20203
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="267" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{91433706-920A-4295-A378-D6CB078E6392}"/>
+  <xr:revisionPtr revIDLastSave="340" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CADB46A7-79DE-4449-B91C-D9087C942A95}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -187,6 +187,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{AE7B9833-D9E4-4D9F-8A3E-8F144D340007}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Ronty paid t to Gaur Da cash</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -197,7 +221,41 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+barandah Ceiling</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>sounak nandi</author>
+  </authors>
+  <commentList>
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
       <text>
         <r>
           <rPr>
@@ -222,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
       <text>
         <r>
           <rPr>
@@ -247,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
       <text>
         <r>
           <rPr>
@@ -271,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
       <text>
         <r>
           <rPr>
@@ -295,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
       <text>
         <r>
           <rPr>
@@ -319,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
       <text>
         <r>
           <rPr>
@@ -343,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
       <text>
         <r>
           <rPr>
@@ -367,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
       <text>
         <r>
           <rPr>
@@ -391,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
       <text>
         <r>
           <rPr>
@@ -415,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
       <text>
         <r>
           <rPr>
@@ -439,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
       <text>
         <r>
           <rPr>
@@ -463,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{1E3E7512-5BB0-42F9-BC92-CBABBA91DF39}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{1E3E7512-5BB0-42F9-BC92-CBABBA91DF39}">
       <text>
         <r>
           <rPr>
@@ -492,7 +550,7 @@
 </comments>
 </file>
 
-<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>sounak nandi</author>
@@ -1285,11 +1343,83 @@
         </r>
       </text>
     </comment>
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I44" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Till today 18-12-2023</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Handles</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
-<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments6.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>sounak nandi</author>
@@ -1780,12 +1910,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{4798DD2C-9DA1-41D4-8E38-190E059D9E0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+sahid da</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="171">
   <si>
     <t>Provider</t>
   </si>
@@ -2286,6 +2440,18 @@
   </si>
   <si>
     <t>Bathroom, Kitchen and Barandah</t>
+  </si>
+  <si>
+    <t>Payment - 29</t>
+  </si>
+  <si>
+    <t>Payment - 30</t>
+  </si>
+  <si>
+    <t>Handles</t>
+  </si>
+  <si>
+    <t>False ceiling</t>
   </si>
 </sst>
 </file>
@@ -2786,7 +2952,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -2949,6 +3115,8 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3234,7 +3402,31 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person69.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/persons/person7.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person70.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person71.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person72.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person73.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person74.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -3546,7 +3738,7 @@
   <dimension ref="C7:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+      <selection activeCell="I17" activeCellId="1" sqref="H17 I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3623,14 +3815,14 @@
       </c>
       <c r="F10">
         <f>Paint!F10</f>
-        <v>65000</v>
+        <v>70000</v>
       </c>
       <c r="G10">
-        <f>SUM(Paint!F11:F17)</f>
-        <v>52500</v>
+        <f>SUM(Paint!F11:F19)</f>
+        <v>53000</v>
       </c>
       <c r="H10">
-        <v>8783</v>
+        <v>9283</v>
       </c>
       <c r="I10">
         <v>10000</v>
@@ -3641,7 +3833,7 @@
       </c>
       <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>12500</v>
+        <v>17000</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.3">
@@ -3653,11 +3845,14 @@
       </c>
       <c r="F11">
         <f>'False Ceiling'!F10</f>
-        <v>120000</v>
+        <v>124750</v>
       </c>
       <c r="G11">
-        <f>SUM('False Ceiling'!F11:F13)</f>
-        <v>120000</v>
+        <f>SUM('False Ceiling'!F11:F14)</f>
+        <v>124750</v>
+      </c>
+      <c r="I11">
+        <v>4750</v>
       </c>
       <c r="J11">
         <f>SUM(J25:J27)</f>
@@ -3676,11 +3871,11 @@
         <v>29</v>
       </c>
       <c r="F12">
-        <f>'Electric &amp; Lights'!F31</f>
-        <v>154914</v>
+        <f>'Electric &amp; Lights'!F32</f>
+        <v>157914</v>
       </c>
       <c r="G12">
-        <f>SUM('Electric &amp; Lights'!F32:F45)</f>
+        <f>SUM('Electric &amp; Lights'!F33:F46)</f>
         <v>149914</v>
       </c>
       <c r="H12">
@@ -3695,7 +3890,7 @@
       </c>
       <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.3">
@@ -3734,17 +3929,17 @@
       </c>
       <c r="F14">
         <f>Furniture!F18</f>
-        <v>746095</v>
+        <v>750445</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F19:F45)</f>
-        <v>555625</v>
+        <f>SUM(Furniture!F19:F47)</f>
+        <v>630475</v>
       </c>
       <c r="H14">
         <v>46050</v>
       </c>
       <c r="I14">
-        <v>114520</v>
+        <v>189370</v>
       </c>
       <c r="J14">
         <f>SUM(M25:M27)</f>
@@ -3752,7 +3947,7 @@
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>190470</v>
+        <v>119970</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
@@ -3767,14 +3962,14 @@
         <v>312950</v>
       </c>
       <c r="G15">
-        <f>SUM('Bathroom-Kitchen-Barandah'!F22:F35)</f>
-        <v>259450</v>
+        <f>SUM('Bathroom-Kitchen-Barandah'!F22:F38)</f>
+        <v>264450</v>
       </c>
       <c r="H15">
         <v>129000</v>
       </c>
       <c r="I15">
-        <v>30550</v>
+        <v>35550</v>
       </c>
       <c r="J15">
         <f>SUM(N25:N27)</f>
@@ -3782,7 +3977,7 @@
       </c>
       <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>53500</v>
+        <v>48500</v>
       </c>
     </row>
     <row r="16" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3819,19 +4014,19 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1877738</v>
+        <v>1894838</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1591268</v>
+        <v>1676368</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>297168</v>
+        <v>297668</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>164100</v>
+        <v>248700</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(J9:J16)</f>
@@ -3839,7 +4034,7 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>286470</v>
+        <v>218470</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
@@ -3856,7 +4051,7 @@
       </c>
       <c r="F19" s="28">
         <f>SUM(H17,I17)</f>
-        <v>461268</v>
+        <v>546368</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
@@ -3865,7 +4060,7 @@
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>203470</v>
+        <v>135470</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.3">
@@ -3874,7 +4069,7 @@
       </c>
       <c r="F21" s="28">
         <f>K17</f>
-        <v>286470</v>
+        <v>218470</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.3">
@@ -4092,10 +4287,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD019853-AAD7-4C4A-AE9D-387A8C77D1D3}">
-  <dimension ref="D7:G36"/>
+  <dimension ref="D7:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34:G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4410,28 +4605,56 @@
         <v>120</v>
       </c>
     </row>
-    <row r="35" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D35" s="69"/>
       <c r="E35" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="F35" s="12"/>
-      <c r="G35" s="20"/>
-    </row>
-    <row r="36" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D36" s="70"/>
-      <c r="E36" s="13" t="s">
+      <c r="F35" s="41">
+        <v>5000</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="69"/>
+      <c r="E36" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" s="41"/>
+      <c r="G36" s="20"/>
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D37" s="69"/>
+      <c r="E37" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="41"/>
+      <c r="G37" s="20"/>
+    </row>
+    <row r="38" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D38" s="69"/>
+      <c r="E38" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="12"/>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D39" s="70"/>
+      <c r="E39" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F36" s="14">
-        <f>F21-SUM(F22:F35)</f>
-        <v>53500</v>
-      </c>
-      <c r="G36" s="21"/>
+      <c r="F39" s="14">
+        <f>F21-SUM(F22:F38)</f>
+        <v>48500</v>
+      </c>
+      <c r="G39" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D36"/>
+    <mergeCell ref="D9:D39"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4441,10 +4664,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:I42"/>
+  <dimension ref="D6:I49"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A46" sqref="A46:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4614,8 +4837,8 @@
         <v>27</v>
       </c>
       <c r="I26">
-        <f>SUM(G26:G41)</f>
-        <v>164100</v>
+        <f>SUM(G26:G48)</f>
+        <v>248700</v>
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.3">
@@ -4751,10 +4974,10 @@
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F39" s="77" t="s">
+      <c r="F39" s="59" t="s">
         <v>164</v>
       </c>
-      <c r="G39" s="77">
+      <c r="G39" s="59">
         <v>4550</v>
       </c>
       <c r="H39" s="59" t="s">
@@ -4762,20 +4985,79 @@
       </c>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F40" s="77" t="s">
+      <c r="F40" s="59" t="s">
         <v>165</v>
       </c>
-      <c r="G40" s="77">
+      <c r="G40" s="59">
         <v>7000</v>
       </c>
       <c r="H40" s="59" t="s">
         <v>151</v>
       </c>
     </row>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F41" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="G41" s="59">
+        <v>63500</v>
+      </c>
+      <c r="H41" s="28" t="s">
+        <v>27</v>
+      </c>
+    </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="G42">
-        <f>E25-(SUM(G26:G41))</f>
-        <v>149093</v>
+      <c r="F42" s="59" t="s">
+        <v>169</v>
+      </c>
+      <c r="G42" s="59">
+        <v>11350</v>
+      </c>
+      <c r="H42" s="59" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F43" s="77" t="s">
+        <v>165</v>
+      </c>
+      <c r="G43" s="77">
+        <v>5000</v>
+      </c>
+      <c r="H43" s="59" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F44" s="77" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="77">
+        <v>4750</v>
+      </c>
+      <c r="H44" s="77" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F45" s="78"/>
+      <c r="G45" s="78"/>
+      <c r="H45" s="79"/>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F46" s="78"/>
+      <c r="G46" s="78"/>
+      <c r="H46" s="79"/>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F47" s="78"/>
+      <c r="G47" s="78"/>
+      <c r="H47" s="79"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="G49">
+        <f>E25-(SUM(G26:G48))</f>
+        <v>64493</v>
       </c>
     </row>
   </sheetData>
@@ -4793,7 +5075,7 @@
   <dimension ref="D7:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4911,10 +5193,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5512692-EDEE-4A22-9F00-43BA354170EF}">
-  <dimension ref="D7:G18"/>
+  <dimension ref="D7:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4948,7 +5230,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="10">
-        <v>65000</v>
+        <v>70000</v>
       </c>
       <c r="G9" s="20"/>
     </row>
@@ -4959,7 +5241,7 @@
       </c>
       <c r="F10" s="14">
         <f>F9</f>
-        <v>65000</v>
+        <v>70000</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -5035,32 +5317,50 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D17" s="69"/>
       <c r="E17" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="41">
+        <v>500</v>
+      </c>
+      <c r="G17" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="69"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="41"/>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="69"/>
+      <c r="E19" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="F19" s="12">
         <v>0</v>
       </c>
-      <c r="G17" s="20" t="s">
+      <c r="G19" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="70"/>
-      <c r="E18" s="13" t="s">
+    <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="70"/>
+      <c r="E20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="14">
-        <f>F10-SUM(F11:F17)</f>
-        <v>12500</v>
-      </c>
-      <c r="G18" s="21"/>
+      <c r="F20" s="14">
+        <f>F10-SUM(F11:F19)</f>
+        <v>17000</v>
+      </c>
+      <c r="G20" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="D9:D20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5069,11 +5369,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB69F67B-3322-470C-8A9C-70E95A023898}">
-  <dimension ref="D7:G14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB69F67B-3322-470C-8A9C-70E95A023898}">
+  <dimension ref="D7:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5107,7 +5407,7 @@
         <v>14</v>
       </c>
       <c r="F9" s="10">
-        <v>120000</v>
+        <v>124750</v>
       </c>
       <c r="G9" s="20"/>
     </row>
@@ -5118,7 +5418,7 @@
       </c>
       <c r="F10" s="14">
         <f>F9</f>
-        <v>120000</v>
+        <v>124750</v>
       </c>
       <c r="G10" s="20"/>
     </row>
@@ -5146,7 +5446,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D13" s="69"/>
       <c r="E13" s="11" t="s">
         <v>33</v>
@@ -5159,30 +5459,43 @@
       </c>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="70"/>
-      <c r="E14" s="13" t="s">
+      <c r="D14" s="69"/>
+      <c r="E14" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="42">
+        <v>4750</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D15" s="70"/>
+      <c r="E15" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="14">
-        <f>F10-SUM(F11:F13)</f>
+      <c r="F15" s="14">
+        <f>F10-SUM(F11:F14)</f>
         <v>0</v>
       </c>
-      <c r="G14" s="21"/>
+      <c r="G15" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D14"/>
+    <mergeCell ref="D9:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1544B4-216C-4DA0-B248-9403EAEF3872}">
-  <dimension ref="D7:G46"/>
+  <dimension ref="D7:G47"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D46"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5414,62 +5727,55 @@
         <v>30</v>
       </c>
       <c r="F29" s="4">
-        <v>27000</v>
+        <v>30000</v>
       </c>
       <c r="G29" s="20"/>
     </row>
-    <row r="30" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D30" s="72"/>
-      <c r="E30" t="s">
-        <v>89</v>
-      </c>
-      <c r="F30" s="4">
-        <v>15350</v>
-      </c>
+      <c r="F30" s="4"/>
       <c r="G30" s="20"/>
     </row>
     <row r="31" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D31" s="72"/>
-      <c r="E31" s="1" t="s">
+      <c r="E31" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31" s="4">
+        <v>15350</v>
+      </c>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="72"/>
+      <c r="E32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="3">
-        <f>SUM(F9:F30)</f>
-        <v>154914</v>
-      </c>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="72"/>
-      <c r="E32" t="s">
-        <v>32</v>
-      </c>
-      <c r="F32" s="41">
-        <v>16345</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>38</v>
-      </c>
+      <c r="F32" s="3">
+        <f>SUM(F9:F31)</f>
+        <v>157914</v>
+      </c>
+      <c r="G32" s="20"/>
     </row>
     <row r="33" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D33" s="72"/>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F33" s="41">
-        <v>11088</v>
+        <v>16345</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D34" s="72"/>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F34" s="41">
-        <v>4100</v>
+        <v>11088</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>36</v>
@@ -5478,10 +5784,10 @@
     <row r="35" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D35" s="72"/>
       <c r="E35" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F35" s="41">
-        <v>6903</v>
+        <v>4100</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>36</v>
@@ -5490,10 +5796,10 @@
     <row r="36" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D36" s="72"/>
       <c r="E36" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="F36" s="41">
-        <v>36280</v>
+        <v>6903</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>36</v>
@@ -5502,10 +5808,10 @@
     <row r="37" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D37" s="72"/>
       <c r="E37" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F37" s="41">
-        <v>8805</v>
+        <v>36280</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>36</v>
@@ -5514,10 +5820,10 @@
     <row r="38" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D38" s="72"/>
       <c r="E38" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="F38" s="41">
-        <v>31700</v>
+        <v>8805</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>36</v>
@@ -5526,34 +5832,34 @@
     <row r="39" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D39" s="72"/>
       <c r="E39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F39" s="41">
-        <v>15350</v>
+        <v>31700</v>
       </c>
       <c r="G39" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D40" s="72"/>
       <c r="E40" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F40" s="41">
-        <v>5454</v>
+        <v>15350</v>
       </c>
       <c r="G40" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D41" s="72"/>
       <c r="E41" t="s">
-        <v>94</v>
+        <v>78</v>
       </c>
       <c r="F41" s="41">
-        <v>2859</v>
+        <v>5454</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>36</v>
@@ -5562,10 +5868,10 @@
     <row r="42" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D42" s="72"/>
       <c r="E42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F42" s="41">
-        <v>2000</v>
+        <v>2859</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>36</v>
@@ -5574,45 +5880,57 @@
     <row r="43" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D43" s="72"/>
       <c r="E43" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F43" s="41">
-        <v>9030</v>
+        <v>2000</v>
       </c>
       <c r="G43" s="20" t="s">
-        <v>120</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D44" s="72"/>
       <c r="E44" t="s">
-        <v>97</v>
-      </c>
-      <c r="F44" s="41"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="45" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>96</v>
+      </c>
+      <c r="F44" s="41">
+        <v>9030</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.3">
       <c r="D45" s="72"/>
       <c r="E45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F45" s="41"/>
+      <c r="G45" s="20"/>
+    </row>
+    <row r="46" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D46" s="72"/>
+      <c r="E46" t="s">
         <v>98</v>
       </c>
-      <c r="F45" s="4"/>
-      <c r="G45" s="20"/>
-    </row>
-    <row r="46" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="73"/>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="4"/>
+      <c r="G46" s="20"/>
+    </row>
+    <row r="47" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D47" s="73"/>
+      <c r="E47" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="3">
-        <f>F31-SUM(F32:F45)</f>
-        <v>5000</v>
-      </c>
-      <c r="G46" s="21"/>
+      <c r="F47" s="3">
+        <f>F32-SUM(F33:F46)</f>
+        <v>8000</v>
+      </c>
+      <c r="G47" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D46"/>
+    <mergeCell ref="D9:D47"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5952,10 +6270,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:J46"/>
+  <dimension ref="D7:I48"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView topLeftCell="C23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6039,7 +6357,7 @@
         <v>135</v>
       </c>
       <c r="F14" s="12">
-        <v>7000</v>
+        <v>11350</v>
       </c>
       <c r="G14" s="20"/>
     </row>
@@ -6080,7 +6398,7 @@
       </c>
       <c r="F18" s="14">
         <f>SUM(F9:F17)</f>
-        <v>746095</v>
+        <v>750445</v>
       </c>
       <c r="G18" s="20"/>
     </row>
@@ -6264,7 +6582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D33" s="75"/>
       <c r="E33" s="19" t="s">
         <v>107</v>
@@ -6276,7 +6594,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="34" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D34" s="75"/>
       <c r="E34" s="19" t="s">
         <v>108</v>
@@ -6288,7 +6606,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D35" s="75"/>
       <c r="E35" s="19" t="s">
         <v>109</v>
@@ -6300,7 +6618,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="36" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D36" s="75"/>
       <c r="E36" s="19" t="s">
         <v>115</v>
@@ -6312,7 +6630,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D37" s="75"/>
       <c r="E37" s="19" t="s">
         <v>116</v>
@@ -6324,7 +6642,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D38" s="75"/>
       <c r="E38" s="19" t="s">
         <v>118</v>
@@ -6342,7 +6660,7 @@
         <v>126500</v>
       </c>
     </row>
-    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D39" s="75"/>
       <c r="E39" s="19" t="s">
         <v>119</v>
@@ -6354,7 +6672,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D40" s="75"/>
       <c r="E40" s="19" t="s">
         <v>131</v>
@@ -6371,12 +6689,8 @@
       <c r="I40">
         <v>136500</v>
       </c>
-      <c r="J40">
-        <f>F16-I40</f>
-        <v>163500</v>
-      </c>
-    </row>
-    <row r="41" spans="4:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D41" s="75"/>
       <c r="E41" s="19" t="s">
         <v>132</v>
@@ -6388,7 +6702,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D42" s="75"/>
       <c r="E42" s="19" t="s">
         <v>139</v>
@@ -6400,7 +6714,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D43" s="75"/>
       <c r="E43" s="19" t="s">
         <v>161</v>
@@ -6412,40 +6726,70 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D44" s="75"/>
       <c r="E44" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="F44" s="41"/>
-      <c r="G44" s="20"/>
-    </row>
-    <row r="45" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="F44" s="41">
+        <v>63500</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="H44" t="s">
+        <v>124</v>
+      </c>
+      <c r="I44">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D45" s="75"/>
       <c r="E45" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="F45" s="12">
+      <c r="F45" s="41">
+        <v>11350</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D46" s="75"/>
+      <c r="E46" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F46" s="41"/>
+      <c r="G46" s="20"/>
+    </row>
+    <row r="47" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D47" s="75"/>
+      <c r="E47" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="F47" s="12">
         <v>0</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="G47" s="20" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="46" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="76"/>
-      <c r="E46" s="1" t="s">
+    <row r="48" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D48" s="76"/>
+      <c r="E48" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F46" s="14">
-        <f>F18-SUM(F19:F45)</f>
-        <v>190470</v>
-      </c>
-      <c r="G46" s="21"/>
+      <c r="F48" s="14">
+        <f>F18-SUM(F19:F47)</f>
+        <v>119970</v>
+      </c>
+      <c r="G48" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D46"/>
+    <mergeCell ref="D9:D48"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added updates till 23-01-2024
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="340" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CADB46A7-79DE-4449-B91C-D9087C942A95}"/>
+  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8442F2E7-BFE7-4A02-9598-AADFF1CADFB0}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -221,7 +221,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
       <text>
         <r>
           <rPr>
@@ -255,7 +255,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
       <text>
         <r>
           <rPr>
@@ -280,7 +280,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
       <text>
         <r>
           <rPr>
@@ -305,7 +305,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
       <text>
         <r>
           <rPr>
@@ -329,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
       <text>
         <r>
           <rPr>
@@ -353,7 +353,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
       <text>
         <r>
           <rPr>
@@ -377,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
       <text>
         <r>
           <rPr>
@@ -401,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
       <text>
         <r>
           <rPr>
@@ -425,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
       <text>
         <r>
           <rPr>
@@ -449,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
       <text>
         <r>
           <rPr>
@@ -473,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
       <text>
         <r>
           <rPr>
@@ -497,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
       <text>
         <r>
           <rPr>
@@ -521,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{1E3E7512-5BB0-42F9-BC92-CBABBA91DF39}">
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{1E3E7512-5BB0-42F9-BC92-CBABBA91DF39}">
       <text>
         <r>
           <rPr>
@@ -543,6 +543,30 @@
           <t xml:space="preserve">
 Strips and 2 watts
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{0AA7B1D3-E81F-4D95-8263-EB90FB490E55}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+CCTV</t>
         </r>
       </text>
     </comment>
@@ -686,7 +710,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{E3B0DB5E-EFB2-4183-B2C1-99AD1E10DC45}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{E3B0DB5E-EFB2-4183-B2C1-99AD1E10DC45}">
       <text>
         <r>
           <rPr>
@@ -710,7 +734,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
       <text>
         <r>
           <rPr>
@@ -734,7 +758,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
       <text>
         <r>
           <rPr>
@@ -758,7 +782,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
       <text>
         <r>
           <rPr>
@@ -783,7 +807,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
       <text>
         <r>
           <rPr>
@@ -808,7 +832,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
       <text>
         <r>
           <rPr>
@@ -833,7 +857,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
       <text>
         <r>
           <rPr>
@@ -859,7 +883,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
       <text>
         <r>
           <rPr>
@@ -883,7 +907,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
       <text>
         <r>
           <rPr>
@@ -907,7 +931,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
       <text>
         <r>
           <rPr>
@@ -931,7 +955,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
       <text>
         <r>
           <rPr>
@@ -955,7 +979,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
       <text>
         <r>
           <rPr>
@@ -979,7 +1003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H31" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
+    <comment ref="H34" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
       <text>
         <r>
           <rPr>
@@ -1003,7 +1027,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+    <comment ref="F35" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
           <rPr>
@@ -1027,7 +1051,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+    <comment ref="F36" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
       <text>
         <r>
           <rPr>
@@ -1051,7 +1075,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
       <text>
         <r>
           <rPr>
@@ -1076,7 +1100,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
       <text>
         <r>
           <rPr>
@@ -1103,7 +1127,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
       <text>
         <r>
           <rPr>
@@ -1127,7 +1151,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
       <text>
         <r>
           <rPr>
@@ -1151,7 +1175,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1199,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I38" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
+    <comment ref="I41" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
       <text>
         <r>
           <rPr>
@@ -1199,7 +1223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
       <text>
         <r>
           <rPr>
@@ -1223,7 +1247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
       <text>
         <r>
           <rPr>
@@ -1247,7 +1271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I40" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
+    <comment ref="I43" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
       <text>
         <r>
           <rPr>
@@ -1271,7 +1295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
       <text>
         <r>
           <rPr>
@@ -1295,7 +1319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
       <text>
         <r>
           <rPr>
@@ -1319,7 +1343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{9801DA58-C7B4-4364-9205-58707072E88C}">
+    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{9801DA58-C7B4-4364-9205-58707072E88C}">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
+    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
       <text>
         <r>
           <rPr>
@@ -1367,7 +1391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I44" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
+    <comment ref="I47" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
       <text>
         <r>
           <rPr>
@@ -1391,7 +1415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
+    <comment ref="F48" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
       <text>
         <r>
           <rPr>
@@ -1412,6 +1436,103 @@
           </rPr>
           <t xml:space="preserve">
 Handles</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F49" authorId="0" shapeId="0" xr:uid="{7209404C-B1DE-4988-B78E-695821C66020}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+lock godrej</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F50" authorId="0" shapeId="0" xr:uid="{8CD9AA95-66D8-47E8-97CA-B73A6D47FABD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+bikas da </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{1CA1BF83-085B-4EEF-9FAE-03AB18F5FC7C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Chaka and Other set</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{843F7684-8F79-464D-8D4F-0683C00C0A13}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Anam- Till now 50k
+</t>
         </r>
       </text>
     </comment>
@@ -1440,30 +1561,6 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{9B98C3D4-1986-4726-9F41-505270A064CA}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>sounak nandi:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-48k paid till no -01-12-2023</t>
-        </r>
-      </text>
-    </comment>
     <comment ref="F14" authorId="0" shapeId="0" xr:uid="{D6CF9A0F-81C3-4D85-84A2-6CDCDC2723E7}">
       <text>
         <r>
@@ -1934,12 +2031,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{3AEBB180-7950-4B14-979A-1E21632E12F6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Jacky Payment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{39308213-7A53-4286-820A-EF5EC7AD39EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Jacky</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="195">
   <si>
     <t>Provider</t>
   </si>
@@ -1998,9 +2143,6 @@
     <t>Door - Bedroom</t>
   </si>
   <si>
-    <t>Balcony Glass Rail(Running length)</t>
-  </si>
-  <si>
     <t>Majuri</t>
   </si>
   <si>
@@ -2452,13 +2594,88 @@
   </si>
   <si>
     <t>False ceiling</t>
+  </si>
+  <si>
+    <t>CCTV</t>
+  </si>
+  <si>
+    <t>Electrical lot (bill in drive with Exhaust Fan)</t>
+  </si>
+  <si>
+    <t>Electric  World</t>
+  </si>
+  <si>
+    <t>Chanchal</t>
+  </si>
+  <si>
+    <t>Payment -8</t>
+  </si>
+  <si>
+    <t>Payment -9</t>
+  </si>
+  <si>
+    <t>Paint Shop</t>
+  </si>
+  <si>
+    <t>Godrej main door lock</t>
+  </si>
+  <si>
+    <t>Sliding for Drawing room</t>
+  </si>
+  <si>
+    <t>Payment - 31</t>
+  </si>
+  <si>
+    <t>Payment - 32</t>
+  </si>
+  <si>
+    <t>Bikas DA</t>
+  </si>
+  <si>
+    <t>Balcony Grill Glass</t>
+  </si>
+  <si>
+    <t>Raw Material - 5th lot (T patti, Chaka,Magnet,Door stopper..)</t>
+  </si>
+  <si>
+    <t>Chaka And Other Set</t>
+  </si>
+  <si>
+    <t>Tata AIA - Srijiita</t>
+  </si>
+  <si>
+    <t>Jacky</t>
+  </si>
+  <si>
+    <t>Erfan da</t>
+  </si>
+  <si>
+    <t>ThakurerJali</t>
+  </si>
+  <si>
+    <t>Shortfall</t>
+  </si>
+  <si>
+    <t>Anam</t>
+  </si>
+  <si>
+    <t>Payment - 33</t>
+  </si>
+  <si>
+    <t>Payment - 34</t>
+  </si>
+  <si>
+    <t>Payment - 35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanddep da </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2488,6 +2705,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -3063,6 +3287,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3115,8 +3343,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3430,7 +3656,55 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person75.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person76.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person77.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person78.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person79.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/persons/person8.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person80.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person81.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person82.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person83.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person84.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person85.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person86.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -3738,7 +4012,7 @@
   <dimension ref="C7:Q27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="I17" activeCellId="1" sqref="H17 I17"/>
+      <selection activeCell="H17" sqref="H17:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3755,25 +4029,25 @@
     <row r="7" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="4:11" ht="79.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D8" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="23" t="s">
         <v>25</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>26</v>
       </c>
       <c r="F8" s="24" t="s">
         <v>6</v>
       </c>
       <c r="G8" s="25" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H8" s="45" t="s">
+        <v>61</v>
+      </c>
+      <c r="I8" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="J8" s="45" t="s">
         <v>62</v>
-      </c>
-      <c r="I8" s="45" t="s">
-        <v>120</v>
-      </c>
-      <c r="J8" s="45" t="s">
-        <v>63</v>
       </c>
       <c r="K8" s="26" t="s">
         <v>13</v>
@@ -3815,17 +4089,17 @@
       </c>
       <c r="F10">
         <f>Paint!F10</f>
-        <v>70000</v>
+        <v>75000</v>
       </c>
       <c r="G10">
         <f>SUM(Paint!F11:F19)</f>
-        <v>53000</v>
+        <v>63000</v>
       </c>
       <c r="H10">
         <v>9283</v>
       </c>
       <c r="I10">
-        <v>10000</v>
+        <v>20000</v>
       </c>
       <c r="J10">
         <f>SUM(H25:H27)</f>
@@ -3833,7 +4107,7 @@
       </c>
       <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>17000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.3">
@@ -3844,12 +4118,15 @@
         <v>14</v>
       </c>
       <c r="F11">
-        <f>'False Ceiling'!F10</f>
-        <v>124750</v>
+        <f>'False Ceiling'!F11</f>
+        <v>126550</v>
       </c>
       <c r="G11">
-        <f>SUM('False Ceiling'!F11:F14)</f>
-        <v>124750</v>
+        <f>SUM('False Ceiling'!F12:F17)</f>
+        <v>126550</v>
+      </c>
+      <c r="H11">
+        <v>1800</v>
       </c>
       <c r="I11">
         <v>4750</v>
@@ -3868,21 +4145,21 @@
         <v>4</v>
       </c>
       <c r="E12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F12">
-        <f>'Electric &amp; Lights'!F32</f>
-        <v>157914</v>
+        <f>'Electric &amp; Lights'!F33</f>
+        <v>167869</v>
       </c>
       <c r="G12">
-        <f>SUM('Electric &amp; Lights'!F33:F46)</f>
-        <v>149914</v>
+        <f>SUM('Electric &amp; Lights'!F34:F49)</f>
+        <v>164869</v>
       </c>
       <c r="H12">
         <v>31695</v>
       </c>
       <c r="I12">
-        <v>9030</v>
+        <v>23985</v>
       </c>
       <c r="J12">
         <f>SUM(K25:K27)</f>
@@ -3890,7 +4167,7 @@
       </c>
       <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>8000</v>
+        <v>3000</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.3">
@@ -3902,14 +4179,17 @@
       </c>
       <c r="F13">
         <f>Grill!F15</f>
-        <v>114000</v>
+        <v>109000</v>
       </c>
       <c r="G13">
-        <f>SUM(Grill!F16:F21)</f>
-        <v>89000</v>
+        <f>SUM(Grill!F16:F22)</f>
+        <v>99000</v>
       </c>
       <c r="H13">
         <v>36300</v>
+      </c>
+      <c r="I13">
+        <v>10000</v>
       </c>
       <c r="J13">
         <f>SUM(L25:L27)</f>
@@ -3917,7 +4197,7 @@
       </c>
       <c r="K13" s="4">
         <f t="shared" si="0"/>
-        <v>25000</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.3">
@@ -3925,21 +4205,21 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F14">
-        <f>Furniture!F18</f>
-        <v>750445</v>
+        <f>Furniture!F21</f>
+        <v>804695</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F19:F47)</f>
-        <v>630475</v>
+        <f>SUM(Furniture!F22:F55)</f>
+        <v>684725</v>
       </c>
       <c r="H14">
-        <v>46050</v>
+        <v>60950</v>
       </c>
       <c r="I14">
-        <v>189370</v>
+        <v>228720</v>
       </c>
       <c r="J14">
         <f>SUM(M25:M27)</f>
@@ -3955,21 +4235,21 @@
         <v>7</v>
       </c>
       <c r="E15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F15">
         <f>'Bathroom-Kitchen-Barandah'!F21</f>
-        <v>312950</v>
+        <v>343950</v>
       </c>
       <c r="G15">
-        <f>SUM('Bathroom-Kitchen-Barandah'!F22:F38)</f>
-        <v>264450</v>
+        <f>SUM('Bathroom-Kitchen-Barandah'!F22:F40)</f>
+        <v>316888</v>
       </c>
       <c r="H15">
         <v>129000</v>
       </c>
       <c r="I15">
-        <v>35550</v>
+        <v>87988</v>
       </c>
       <c r="J15">
         <f>SUM(N25:N27)</f>
@@ -3977,7 +4257,7 @@
       </c>
       <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>48500</v>
+        <v>27062</v>
       </c>
     </row>
     <row r="16" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -3985,7 +4265,7 @@
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16">
         <f>Civil!F12</f>
@@ -4014,19 +4294,19 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1894838</v>
+        <v>1991843</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1676368</v>
+        <v>1819811</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>297668</v>
+        <v>314368</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>248700</v>
+        <v>375443</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(J9:J16)</f>
@@ -4034,12 +4314,12 @@
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>218470</v>
+        <v>172032</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E18" s="29" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="F18" s="29">
         <v>1213000</v>
@@ -4047,34 +4327,41 @@
     </row>
     <row r="19" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E19" s="28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="28">
         <f>SUM(H17,I17)</f>
-        <v>546368</v>
+        <v>689811</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E20" s="28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>135470</v>
+        <v>89032</v>
+      </c>
+      <c r="G20" s="61">
+        <f>F20-SUM('Extra Source'!G68,'Extra Source'!G55)</f>
+        <v>69032</v>
+      </c>
+      <c r="H20" s="28" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="21" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E21" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F21" s="28">
         <f>K17</f>
-        <v>218470</v>
+        <v>172032</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.3">
       <c r="E22" s="28" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F22" s="28">
         <f>F21-F20</f>
@@ -4082,61 +4369,61 @@
       </c>
     </row>
     <row r="23" spans="3:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="60"/>
-      <c r="E23" s="60"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-      <c r="L23" s="60"/>
-      <c r="M23" s="60"/>
-      <c r="N23" s="60"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="60"/>
+      <c r="C23" s="62" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="62"/>
+      <c r="E23" s="62"/>
+      <c r="F23" s="62"/>
+      <c r="G23" s="62"/>
+      <c r="H23" s="62"/>
+      <c r="I23" s="62"/>
+      <c r="J23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="62"/>
+      <c r="M23" s="62"/>
+      <c r="N23" s="62"/>
+      <c r="O23" s="62"/>
+      <c r="P23" s="62"/>
+      <c r="Q23" s="62"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="E24" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="D24" s="34" t="s">
-        <v>52</v>
-      </c>
-      <c r="E24" s="35" t="s">
+      <c r="F24" s="36" t="s">
         <v>47</v>
       </c>
-      <c r="F24" s="36" t="s">
+      <c r="G24" s="37" t="s">
         <v>48</v>
-      </c>
-      <c r="G24" s="37" t="s">
-        <v>49</v>
       </c>
       <c r="H24" s="37" t="s">
         <v>12</v>
       </c>
       <c r="I24" s="37"/>
       <c r="J24" s="37" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K24" s="37" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L24" s="37" t="s">
         <v>17</v>
       </c>
       <c r="M24" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="N24" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="N24" s="37" t="s">
-        <v>28</v>
-      </c>
       <c r="O24" s="37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P24" s="38" t="s">
         <v>6</v>
@@ -4287,10 +4574,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD019853-AAD7-4C4A-AE9D-387A8C77D1D3}">
-  <dimension ref="D7:G39"/>
+  <dimension ref="D7:N41"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34:G35"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4299,6 +4586,7 @@
     <col min="5" max="5" width="31.5546875" customWidth="1"/>
     <col min="6" max="6" width="32.88671875" customWidth="1"/>
     <col min="7" max="7" width="14.109375" customWidth="1"/>
+    <col min="10" max="10" width="11.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -4313,25 +4601,25 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="68" t="s">
-        <v>61</v>
+      <c r="D9" s="70" t="s">
+        <v>60</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F9" s="10">
-        <v>90000</v>
+        <v>121000</v>
       </c>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="69"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="12">
         <v>32000</v>
@@ -4339,9 +4627,9 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="69"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F11" s="12">
         <v>27500</v>
@@ -4349,9 +4637,9 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="69"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="11" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F12" s="32">
         <v>92300</v>
@@ -4359,9 +4647,9 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="69"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F13" s="32">
         <v>13600</v>
@@ -4369,9 +4657,9 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="69"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F14" s="32">
         <v>20000</v>
@@ -4379,9 +4667,9 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="69"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" s="32">
         <v>5500</v>
@@ -4389,9 +4677,9 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="69"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="11" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F16" s="32">
         <v>3700</v>
@@ -4399,9 +4687,9 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="69"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F17" s="32">
         <v>6500</v>
@@ -4409,9 +4697,9 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="69"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="11" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F18" s="32">
         <v>2000</v>
@@ -4419,9 +4707,9 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="69"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="11" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F19" s="32">
         <v>4850</v>
@@ -4429,9 +4717,9 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="69"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F20" s="12">
         <v>15000</v>
@@ -4439,222 +4727,264 @@
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="69"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F21" s="14">
         <f>SUM(F9:F20)</f>
-        <v>312950</v>
+        <v>343950</v>
       </c>
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="69"/>
+      <c r="D22" s="71"/>
       <c r="E22" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" s="41">
         <v>50000</v>
       </c>
       <c r="G22" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="69"/>
+      <c r="D23" s="71"/>
       <c r="E23" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F23" s="41">
         <v>23500</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="69"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F24" s="41">
         <v>50000</v>
       </c>
       <c r="G24" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="69"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F25" s="41">
         <v>40000</v>
       </c>
       <c r="G25" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="69"/>
+      <c r="D26" s="71"/>
       <c r="E26" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F26" s="41">
         <v>2300</v>
       </c>
       <c r="G26" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="69"/>
+      <c r="D27" s="71"/>
       <c r="E27" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F27" s="41">
         <v>5500</v>
       </c>
       <c r="G27" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="69"/>
+      <c r="D28" s="71"/>
       <c r="E28" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F28" s="41">
         <v>50000</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="69"/>
+      <c r="D29" s="71"/>
       <c r="E29" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="41">
         <v>6000</v>
       </c>
       <c r="G29" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="69"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F30" s="41">
         <v>1600</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="69"/>
+      <c r="D31" s="71"/>
       <c r="E31" s="11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F31" s="41">
         <v>15000</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="69"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="41">
         <v>4000</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D33" s="69"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="33" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D33" s="71"/>
       <c r="E33" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" s="41">
         <v>4550</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D34" s="69"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="34" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D34" s="71"/>
       <c r="E34" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F34" s="41">
         <v>7000</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="69"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="35" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D35" s="71"/>
       <c r="E35" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F35" s="41">
         <v>5000</v>
       </c>
       <c r="G35" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="69"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="36" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D36" s="71"/>
       <c r="E36" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="41">
+        <v>40000</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="37" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D37" s="71"/>
+      <c r="E37" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="41"/>
-      <c r="G36" s="20"/>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="69"/>
-      <c r="E37" s="11" t="s">
+      <c r="F37" s="41">
+        <v>12438</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H37" t="s">
+        <v>186</v>
+      </c>
+      <c r="I37">
+        <v>100438</v>
+      </c>
+      <c r="J37" t="s">
+        <v>194</v>
+      </c>
+      <c r="K37">
+        <v>10000</v>
+      </c>
+      <c r="L37" t="s">
+        <v>190</v>
+      </c>
+      <c r="M37">
+        <v>32000</v>
+      </c>
+      <c r="N37">
+        <f>SUM(I37,K37,M37)</f>
+        <v>142438</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D38" s="71"/>
+      <c r="E38" s="11"/>
+      <c r="F38" s="41"/>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D39" s="71"/>
+      <c r="E39" s="11"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D40" s="71"/>
+      <c r="E40" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="41"/>
-      <c r="G37" s="20"/>
-    </row>
-    <row r="38" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D38" s="69"/>
-      <c r="E38" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="F38" s="12"/>
-      <c r="G38" s="20"/>
-    </row>
-    <row r="39" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D39" s="70"/>
-      <c r="E39" s="13" t="s">
+      <c r="F40" s="12"/>
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D41" s="72"/>
+      <c r="E41" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="14">
-        <f>F21-SUM(F22:F38)</f>
-        <v>48500</v>
-      </c>
-      <c r="G39" s="21"/>
+      <c r="F41" s="14">
+        <f>F21-SUM(F22:F40)</f>
+        <v>27062</v>
+      </c>
+      <c r="G41" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D39"/>
+    <mergeCell ref="D9:D41"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4664,10 +4994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:I49"/>
+  <dimension ref="D6:I80"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:XFD46"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4679,30 +5009,30 @@
   <sheetData>
     <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="65" t="s">
+      <c r="D7" s="67" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="69"/>
+    </row>
+    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D8" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="67"/>
-    </row>
-    <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="61" t="s">
-        <v>55</v>
-      </c>
-      <c r="E8" s="63">
+      <c r="E8" s="65">
         <v>45000</v>
       </c>
       <c r="F8" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G8" s="49">
         <v>4700</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="62"/>
-      <c r="E9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="66"/>
       <c r="F9" s="28" t="s">
         <v>16</v>
       </c>
@@ -4711,10 +5041,10 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="62"/>
-      <c r="E10" s="64"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="66"/>
       <c r="F10" s="47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="50">
         <v>6000</v>
@@ -4724,7 +5054,7 @@
       <c r="D11" s="51"/>
       <c r="E11" s="28"/>
       <c r="F11" s="28" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G11" s="50">
         <v>16345</v>
@@ -4734,7 +5064,7 @@
       <c r="D12" s="51"/>
       <c r="E12" s="28"/>
       <c r="F12" s="28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G12" s="50">
         <v>5500</v>
@@ -4744,7 +5074,7 @@
       <c r="D13" s="51"/>
       <c r="E13" s="28"/>
       <c r="F13" s="28" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G13" s="50">
         <v>155</v>
@@ -4764,13 +5094,13 @@
     <row r="18" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="19" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D19" s="55" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E19" s="48">
         <v>25000</v>
       </c>
       <c r="F19" s="48" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G19" s="49">
         <v>23500</v>
@@ -4780,7 +5110,7 @@
       <c r="D20" s="51"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" s="50">
         <v>1500</v>
@@ -4812,7 +5142,7 @@
     <row r="24" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="25" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D25" s="56" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E25" s="57">
         <v>313193</v>
@@ -4820,58 +5150,58 @@
       <c r="F25" s="57"/>
       <c r="G25" s="57"/>
       <c r="H25" s="57" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I25" s="58" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F26" s="29" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G26" s="29">
         <v>5300</v>
       </c>
       <c r="H26" s="29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="I26">
-        <f>SUM(G26:G48)</f>
-        <v>248700</v>
+        <f>SUM(G26:G54)</f>
+        <v>313193</v>
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F27" s="28" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G27" s="28">
         <v>4700</v>
       </c>
       <c r="H27" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F28" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G28" s="28">
         <v>30000</v>
       </c>
       <c r="H28" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F29" s="28" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G29" s="28">
         <v>5590</v>
       </c>
       <c r="H29" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.3">
@@ -4887,177 +5217,322 @@
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F31" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G31" s="28">
         <v>3730</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F32" s="28" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G32" s="28">
         <v>15000</v>
       </c>
       <c r="H32" s="59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="33" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F33" s="28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G33" s="28">
         <v>10000</v>
       </c>
       <c r="H33" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F34" s="28" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G34" s="28">
         <v>4200</v>
       </c>
       <c r="H34" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F35" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G35" s="28">
         <v>35000</v>
       </c>
       <c r="H35" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F36" s="59" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G36" s="59">
         <v>4000</v>
       </c>
       <c r="H36" s="59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="37" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F37" s="59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G37" s="59">
         <v>16000</v>
       </c>
       <c r="H37" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F38" s="59" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G38" s="59">
         <v>9030</v>
       </c>
       <c r="H38" s="59" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F39" s="59" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G39" s="59">
         <v>4550</v>
       </c>
       <c r="H39" s="59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F40" s="59" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G40" s="59">
         <v>7000</v>
       </c>
       <c r="H40" s="59" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="41" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F41" s="59" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G41" s="59">
         <v>63500</v>
       </c>
       <c r="H41" s="28" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="42" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F42" s="59" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G42" s="59">
         <v>11350</v>
       </c>
       <c r="H42" s="59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F43" s="59" t="s">
+        <v>164</v>
+      </c>
+      <c r="G43" s="59">
+        <v>5000</v>
+      </c>
+      <c r="H43" s="59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F44" s="59" t="s">
+        <v>15</v>
+      </c>
+      <c r="G44" s="59">
+        <v>4750</v>
+      </c>
+      <c r="H44" s="59" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F45" s="59" t="s">
+        <v>172</v>
+      </c>
+      <c r="G45" s="59">
+        <v>7705</v>
+      </c>
+      <c r="H45" s="59" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F46" s="59" t="s">
+        <v>173</v>
+      </c>
+      <c r="G46" s="59">
+        <v>5000</v>
+      </c>
+      <c r="H46" s="59" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F47" s="59" t="s">
+        <v>176</v>
+      </c>
+      <c r="G47" s="59">
+        <v>10000</v>
+      </c>
+      <c r="H47" s="59" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F48" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="G48" s="59">
+        <v>20000</v>
+      </c>
+      <c r="H48" s="59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F49" s="59" t="s">
+        <v>184</v>
+      </c>
+      <c r="G49" s="59">
+        <v>4350</v>
+      </c>
+      <c r="H49" s="59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F50" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="G50" s="59">
+        <v>10000</v>
+      </c>
+      <c r="H50" s="59" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F51" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="G51" s="59">
+        <v>5000</v>
+      </c>
+      <c r="H51" s="59" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F52" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="G52" s="79">
+        <v>2438</v>
+      </c>
+      <c r="H52" s="79" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>10</v>
+      </c>
+      <c r="G55">
+        <f>E25-(SUM(G26:G54))</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="61" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D61" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="57">
+        <v>80000</v>
+      </c>
+      <c r="F61" s="57"/>
+      <c r="G61" s="57"/>
+      <c r="H61" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="I61" s="58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="62" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F62" s="29" t="s">
+        <v>186</v>
+      </c>
+      <c r="G62" s="29">
+        <v>40000</v>
+      </c>
+      <c r="H62" s="29" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="43" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F43" s="77" t="s">
-        <v>165</v>
-      </c>
-      <c r="G43" s="77">
-        <v>5000</v>
-      </c>
-      <c r="H43" s="59" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="44" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F44" s="77" t="s">
-        <v>15</v>
-      </c>
-      <c r="G44" s="77">
-        <v>4750</v>
-      </c>
-      <c r="H44" s="77" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="45" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F45" s="78"/>
-      <c r="G45" s="78"/>
-      <c r="H45" s="79"/>
-    </row>
-    <row r="46" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F46" s="78"/>
-      <c r="G46" s="78"/>
-      <c r="H46" s="79"/>
-    </row>
-    <row r="47" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="F47" s="78"/>
-      <c r="G47" s="78"/>
-      <c r="H47" s="79"/>
-    </row>
-    <row r="49" spans="7:7" x14ac:dyDescent="0.3">
-      <c r="G49">
-        <f>E25-(SUM(G26:G48))</f>
-        <v>64493</v>
+      <c r="I62">
+        <f>SUM(G62:G67)</f>
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="63" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F63" s="59" t="s">
+        <v>139</v>
+      </c>
+      <c r="G63">
+        <v>10000</v>
+      </c>
+      <c r="H63" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="64" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F64" s="79" t="s">
+        <v>186</v>
+      </c>
+      <c r="G64" s="79">
+        <v>10000</v>
+      </c>
+      <c r="H64" s="79" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>10</v>
+      </c>
+      <c r="G68">
+        <f>E61-I62</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="80" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="G80">
+        <f>E61-SUM(G62:G79)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5099,11 +5574,11 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="70" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -5115,7 +5590,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="69"/>
+      <c r="D10" s="71"/>
       <c r="E10" t="s">
         <v>4</v>
       </c>
@@ -5125,7 +5600,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="69"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
@@ -5136,7 +5611,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="69"/>
+      <c r="D12" s="71"/>
       <c r="E12" t="s">
         <v>7</v>
       </c>
@@ -5144,11 +5619,11 @@
         <v>40000</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="69"/>
+      <c r="D13" s="71"/>
       <c r="E13" t="s">
         <v>8</v>
       </c>
@@ -5156,11 +5631,11 @@
         <v>127140</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="69"/>
+      <c r="D14" s="71"/>
       <c r="E14" t="s">
         <v>9</v>
       </c>
@@ -5168,11 +5643,11 @@
         <v>167139</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="70"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
@@ -5196,7 +5671,7 @@
   <dimension ref="D7:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5219,142 +5694,148 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="70" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="10">
-        <v>70000</v>
+        <v>75000</v>
       </c>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="69"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="14">
         <f>F9</f>
-        <v>70000</v>
+        <v>75000</v>
       </c>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="69"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F11" s="41">
         <v>6000</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="69"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F12" s="41">
         <v>15000</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="69"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F13" s="41">
         <v>15000</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="69"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F14" s="41">
         <v>5000</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="69"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="41">
         <v>1500</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="69"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="11" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F16" s="41">
         <v>10000</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="69"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F17" s="41">
         <v>500</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="69"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="41"/>
-      <c r="G18" s="20"/>
+      <c r="D18" s="71"/>
+      <c r="E18" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="F18" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="19" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="69"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="11" t="s">
-        <v>123</v>
+        <v>175</v>
       </c>
       <c r="F19" s="12">
         <v>0</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="70"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F20" s="14">
         <f>F10-SUM(F11:F19)</f>
-        <v>17000</v>
+        <v>12000</v>
       </c>
       <c r="G20" s="21"/>
     </row>
@@ -5370,10 +5851,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB69F67B-3322-470C-8A9C-70E95A023898}">
-  <dimension ref="D7:G15"/>
+  <dimension ref="D7:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5396,11 +5877,11 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="68" t="s">
+      <c r="D9" s="70" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -5412,79 +5893,110 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="69"/>
-      <c r="E10" s="13" t="s">
+      <c r="D10" s="71"/>
+      <c r="E10" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="F10" s="10">
+        <v>1800</v>
+      </c>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="71"/>
+      <c r="E11" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F10" s="14">
-        <f>F9</f>
-        <v>124750</v>
-      </c>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="69"/>
-      <c r="E11" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="F11" s="42">
+      <c r="F11" s="14">
+        <f>SUM(F9:F10)</f>
+        <v>126550</v>
+      </c>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D12" s="71"/>
+      <c r="E12" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="42">
         <v>50000</v>
       </c>
-      <c r="G11" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="69"/>
-      <c r="E12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="42">
-        <v>40000</v>
-      </c>
       <c r="G12" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="69"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="11" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="42">
+        <v>40000</v>
+      </c>
+      <c r="G13" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="71"/>
+      <c r="E14" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="42">
         <v>30000</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="69"/>
-      <c r="E14" s="11" t="s">
+      <c r="G14" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F14" s="42">
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="71"/>
+      <c r="E15" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="42">
         <v>4750</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="70"/>
-      <c r="E15" s="13" t="s">
+      <c r="G15" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="71"/>
+      <c r="E16" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F16" s="42">
+        <v>1800</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D17" s="71"/>
+      <c r="E17" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" s="42"/>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D18" s="72"/>
+      <c r="E18" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="14">
-        <f>F10-SUM(F11:F14)</f>
+      <c r="F18" s="14">
+        <f>F11-SUM(F12:F17)</f>
         <v>0</v>
       </c>
-      <c r="G15" s="21"/>
+      <c r="G18" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D15"/>
+    <mergeCell ref="D9:D18"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -5492,10 +6004,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1544B4-216C-4DA0-B248-9403EAEF3872}">
-  <dimension ref="D7:G47"/>
+  <dimension ref="D7:G50"/>
   <sheetViews>
     <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="F48" sqref="F47:F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5518,15 +6030,15 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="71" t="s">
-        <v>160</v>
+      <c r="D9" s="73" t="s">
+        <v>159</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F9" s="10">
         <v>10200</v>
@@ -5534,9 +6046,9 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="72"/>
+      <c r="D10" s="74"/>
       <c r="E10" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F10" s="12">
         <v>1440</v>
@@ -5544,9 +6056,9 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="72"/>
+      <c r="D11" s="74"/>
       <c r="E11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F11" s="4">
         <v>710</v>
@@ -5554,9 +6066,9 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="72"/>
+      <c r="D12" s="74"/>
       <c r="E12" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F12" s="4">
         <v>6580</v>
@@ -5564,9 +6076,9 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
+      <c r="D13" s="74"/>
       <c r="E13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F13" s="4">
         <v>3000</v>
@@ -5574,9 +6086,9 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="72"/>
+      <c r="D14" s="74"/>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F14" s="4">
         <v>870</v>
@@ -5584,9 +6096,9 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="72"/>
+      <c r="D15" s="74"/>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F15" s="4">
         <v>10240</v>
@@ -5594,9 +6106,9 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="72"/>
+      <c r="D16" s="74"/>
       <c r="E16" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F16" s="4">
         <v>1680</v>
@@ -5604,9 +6116,9 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="72"/>
+      <c r="D17" s="74"/>
       <c r="E17" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F17" s="4">
         <v>2000</v>
@@ -5614,9 +6126,9 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="72"/>
+      <c r="D18" s="74"/>
       <c r="E18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F18" s="4">
         <v>500</v>
@@ -5624,9 +6136,9 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="72"/>
+      <c r="D19" s="74"/>
       <c r="E19" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F19" s="4">
         <v>2040</v>
@@ -5634,9 +6146,9 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="72"/>
+      <c r="D20" s="74"/>
       <c r="E20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F20" s="4">
         <v>1980</v>
@@ -5644,17 +6156,17 @@
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="72"/>
+      <c r="D21" s="74"/>
       <c r="E21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F21" s="4"/>
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="72"/>
+      <c r="D22" s="74"/>
       <c r="E22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F22" s="4">
         <v>2940</v>
@@ -5662,9 +6174,9 @@
       <c r="G22" s="20"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="72"/>
+      <c r="D23" s="74"/>
       <c r="E23" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F23" s="4">
         <v>2560</v>
@@ -5672,9 +6184,9 @@
       <c r="G23" s="20"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="72"/>
+      <c r="D24" s="74"/>
       <c r="E24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F24" s="4">
         <v>5720</v>
@@ -5682,9 +6194,9 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="72"/>
+      <c r="D25" s="74"/>
       <c r="E25" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F25" s="4">
         <v>430</v>
@@ -5692,9 +6204,9 @@
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="72"/>
+      <c r="D26" s="74"/>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F26" s="4">
         <v>960</v>
@@ -5702,9 +6214,9 @@
       <c r="G26" s="20"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="72"/>
+      <c r="D27" s="74"/>
       <c r="E27" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F27" s="4">
         <v>26960</v>
@@ -5712,9 +6224,9 @@
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="72"/>
+      <c r="D28" s="74"/>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F28" s="4">
         <v>31754</v>
@@ -5722,9 +6234,9 @@
       <c r="G28" s="20"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="72"/>
+      <c r="D29" s="74"/>
       <c r="E29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="4">
         <v>30000</v>
@@ -5732,205 +6244,248 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="72"/>
-      <c r="F30" s="4"/>
+      <c r="D30" s="74"/>
+      <c r="E30" t="s">
+        <v>170</v>
+      </c>
+      <c r="F30" s="4">
+        <v>2250</v>
+      </c>
       <c r="G30" s="20"/>
     </row>
-    <row r="31" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D31" s="72"/>
+    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D31" s="74"/>
       <c r="E31" t="s">
-        <v>89</v>
+        <v>171</v>
       </c>
       <c r="F31" s="4">
+        <v>7705</v>
+      </c>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D32" s="74"/>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+      <c r="F32" s="4">
         <v>15350</v>
       </c>
-      <c r="G31" s="20"/>
-    </row>
-    <row r="32" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="72"/>
-      <c r="E32" s="1" t="s">
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="74"/>
+      <c r="E33" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="3">
-        <f>SUM(F9:F31)</f>
-        <v>157914</v>
-      </c>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D33" s="72"/>
-      <c r="E33" t="s">
-        <v>32</v>
-      </c>
-      <c r="F33" s="41">
+      <c r="F33" s="3">
+        <f>SUM(F9:F32)</f>
+        <v>167869</v>
+      </c>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D34" s="74"/>
+      <c r="E34" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="41">
         <v>16345</v>
       </c>
-      <c r="G33" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D34" s="72"/>
-      <c r="E34" t="s">
-        <v>34</v>
-      </c>
-      <c r="F34" s="41">
-        <v>11088</v>
-      </c>
       <c r="G34" s="20" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="72"/>
+      <c r="D35" s="74"/>
       <c r="E35" t="s">
         <v>33</v>
       </c>
       <c r="F35" s="41">
+        <v>11088</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="74"/>
+      <c r="E36" t="s">
+        <v>32</v>
+      </c>
+      <c r="F36" s="41">
         <v>4100</v>
       </c>
-      <c r="G35" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="72"/>
-      <c r="E36" t="s">
+      <c r="G36" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F36" s="41">
+    </row>
+    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D37" s="74"/>
+      <c r="E37" t="s">
+        <v>34</v>
+      </c>
+      <c r="F37" s="41">
         <v>6903</v>
       </c>
-      <c r="G36" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="72"/>
-      <c r="E37" t="s">
+      <c r="G37" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D38" s="74"/>
+      <c r="E38" t="s">
+        <v>67</v>
+      </c>
+      <c r="F38" s="41">
+        <v>36280</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D39" s="74"/>
+      <c r="E39" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="41">
-        <v>36280</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="72"/>
-      <c r="E38" t="s">
-        <v>69</v>
-      </c>
-      <c r="F38" s="41">
+      <c r="F39" s="41">
         <v>8805</v>
       </c>
-      <c r="G38" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D39" s="72"/>
-      <c r="E39" t="s">
-        <v>75</v>
-      </c>
-      <c r="F39" s="41">
+      <c r="G39" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D40" s="74"/>
+      <c r="E40" t="s">
+        <v>74</v>
+      </c>
+      <c r="F40" s="41">
         <v>31700</v>
       </c>
-      <c r="G39" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D40" s="72"/>
-      <c r="E40" t="s">
+      <c r="G40" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D41" s="74"/>
+      <c r="E41" t="s">
+        <v>76</v>
+      </c>
+      <c r="F41" s="41">
+        <v>15350</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="74"/>
+      <c r="E42" t="s">
         <v>77</v>
       </c>
-      <c r="F40" s="41">
-        <v>15350</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D41" s="72"/>
-      <c r="E41" t="s">
-        <v>78</v>
-      </c>
-      <c r="F41" s="41">
+      <c r="F42" s="41">
         <v>5454</v>
       </c>
-      <c r="G41" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D42" s="72"/>
-      <c r="E42" t="s">
+      <c r="G42" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="74"/>
+      <c r="E43" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="41">
+        <v>2859</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D44" s="74"/>
+      <c r="E44" t="s">
         <v>94</v>
       </c>
-      <c r="F42" s="41">
-        <v>2859</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="72"/>
-      <c r="E43" t="s">
+      <c r="F44" s="41">
+        <v>2000</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D45" s="74"/>
+      <c r="E45" t="s">
         <v>95</v>
       </c>
-      <c r="F43" s="41">
-        <v>2000</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D44" s="72"/>
-      <c r="E44" t="s">
+      <c r="F45" s="41">
+        <v>9030</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D46" s="74"/>
+      <c r="E46" t="s">
         <v>96</v>
       </c>
-      <c r="F44" s="41">
-        <v>9030</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D45" s="72"/>
-      <c r="E45" t="s">
+      <c r="F46" s="41">
+        <v>2250</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="47" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D47" s="74"/>
+      <c r="E47" t="s">
         <v>97</v>
       </c>
-      <c r="F45" s="41"/>
-      <c r="G45" s="20"/>
-    </row>
-    <row r="46" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D46" s="72"/>
-      <c r="E46" t="s">
-        <v>98</v>
-      </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="20"/>
-    </row>
-    <row r="47" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D47" s="73"/>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="41">
+        <v>7705</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D48" s="74"/>
+      <c r="E48" t="s">
+        <v>105</v>
+      </c>
+      <c r="F48" s="41">
+        <v>5000</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D49" s="74"/>
+      <c r="E49" t="s">
+        <v>106</v>
+      </c>
+      <c r="F49" s="4"/>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D50" s="75"/>
+      <c r="E50" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F47" s="3">
-        <f>F32-SUM(F33:F46)</f>
-        <v>8000</v>
-      </c>
-      <c r="G47" s="21"/>
+      <c r="F50" s="3">
+        <f>F33-SUM(F34:F49)</f>
+        <v>3000</v>
+      </c>
+      <c r="G50" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D47"/>
+    <mergeCell ref="D9:D50"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5940,10 +6495,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D61BB101-D3B6-42F4-94AF-045AE645D71D}">
-  <dimension ref="D7:G22"/>
+  <dimension ref="D7:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5966,12 +6521,12 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="68" t="s">
-        <v>138</v>
+      <c r="D9" s="70" t="s">
+        <v>137</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>17</v>
@@ -5982,49 +6537,49 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="69"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="12">
+        <v>16500</v>
+      </c>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D11" s="71"/>
+      <c r="E11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="F11" s="12">
+        <v>17500</v>
+      </c>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D12" s="71"/>
+      <c r="E12" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="12">
+        <v>15000</v>
+      </c>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="71"/>
+      <c r="E13" s="11" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="12">
+        <v>14000</v>
+      </c>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D14" s="71"/>
+      <c r="E14" s="11" t="s">
         <v>19</v>
-      </c>
-      <c r="F10" s="12">
-        <v>19000</v>
-      </c>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="69"/>
-      <c r="E11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="12">
-        <v>16500</v>
-      </c>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="69"/>
-      <c r="E12" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="F12" s="12">
-        <v>17500</v>
-      </c>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="69"/>
-      <c r="E13" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="F13" s="12">
-        <v>15000</v>
-      </c>
-      <c r="G13" s="20"/>
-    </row>
-    <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="69"/>
-      <c r="E14" s="11" t="s">
-        <v>20</v>
       </c>
       <c r="F14" s="12">
         <v>5000</v>
@@ -6032,99 +6587,112 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="69"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F15" s="14">
         <f>SUM(F9:F14)</f>
-        <v>114000</v>
+        <v>109000</v>
       </c>
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="69"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F16" s="41">
         <v>24000</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="69"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="41">
         <v>12300</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="69"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F18" s="41">
         <v>17700</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="69"/>
+      <c r="D19" s="71"/>
       <c r="E19" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" s="41">
         <v>20000</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="69"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F20" s="46">
         <v>15000</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="69"/>
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="71"/>
       <c r="E21" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="4"/>
+        <v>74</v>
+      </c>
+      <c r="F21" s="46">
+        <v>10000</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="70"/>
-      <c r="E22" s="13" t="s">
+      <c r="D22" s="71"/>
+      <c r="E22" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="43"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="72"/>
+      <c r="E23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F22" s="44">
-        <f>F15-SUM(F16:F21)</f>
-        <v>25000</v>
-      </c>
-      <c r="G22" s="21"/>
+      <c r="F23" s="44">
+        <f>F15-SUM(F16:F22)</f>
+        <v>10000</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D22"/>
+    <mergeCell ref="D9:D23"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6157,15 +6725,15 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D9" s="70" t="s">
+        <v>103</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="68" t="s">
-        <v>104</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>40</v>
       </c>
       <c r="F9" s="10">
         <v>16500</v>
@@ -6173,9 +6741,9 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="69"/>
+      <c r="D10" s="71"/>
       <c r="E10" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F10" s="12">
         <v>14000</v>
@@ -6183,15 +6751,15 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="69"/>
+      <c r="D11" s="71"/>
       <c r="E11" s="11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="12"/>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="69"/>
+      <c r="D12" s="71"/>
       <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
@@ -6202,55 +6770,55 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="69"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="41">
         <v>4700</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="69"/>
+      <c r="D14" s="71"/>
       <c r="E14" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="41">
         <v>500</v>
       </c>
       <c r="G14" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="69"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F15" s="41">
         <v>25300</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="69"/>
+      <c r="D16" s="71"/>
       <c r="E16" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="12">
         <v>0</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="70"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
       </c>
@@ -6270,10 +6838,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:I48"/>
+  <dimension ref="D7:I56"/>
   <sheetViews>
-    <sheetView topLeftCell="C23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L36" sqref="L36"/>
+    <sheetView topLeftCell="C32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6296,15 +6864,15 @@
         <v>5</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="74" t="s">
-        <v>21</v>
+      <c r="D9" s="76" t="s">
+        <v>20</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F9" s="10">
         <v>146000</v>
@@ -6312,9 +6880,9 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="75"/>
+      <c r="D10" s="77"/>
       <c r="E10" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" s="12">
         <v>25840</v>
@@ -6322,9 +6890,9 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="75"/>
+      <c r="D11" s="77"/>
       <c r="E11" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F11" s="12">
         <v>90450</v>
@@ -6332,9 +6900,9 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="75"/>
+      <c r="D12" s="77"/>
       <c r="E12" s="19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F12" s="12">
         <v>51705</v>
@@ -6342,454 +6910,552 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="75"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F13" s="12">
         <v>16000</v>
       </c>
       <c r="G13" s="20"/>
     </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="75"/>
-      <c r="E14" s="19" t="s">
-        <v>135</v>
+    <row r="14" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D14" s="77"/>
+      <c r="E14" s="60" t="s">
+        <v>183</v>
       </c>
       <c r="F14" s="12">
+        <v>4350</v>
+      </c>
+      <c r="G14" s="20"/>
+    </row>
+    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D15" s="77"/>
+      <c r="E15" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="F15" s="12">
         <v>11350</v>
       </c>
-      <c r="G14" s="20"/>
-    </row>
-    <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="75"/>
-      <c r="E15" s="19" t="s">
+      <c r="G15" s="20"/>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="77"/>
+      <c r="E16" s="19" t="s">
+        <v>182</v>
+      </c>
+      <c r="F16" s="12">
+        <v>19000</v>
+      </c>
+      <c r="G16" s="20"/>
+    </row>
+    <row r="17" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D17" s="77"/>
+      <c r="E17" s="19" t="s">
+        <v>116</v>
+      </c>
+      <c r="F17" s="12">
+        <v>71000</v>
+      </c>
+      <c r="G17" s="20"/>
+    </row>
+    <row r="18" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D18" s="77"/>
+      <c r="E18" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F18" s="12">
+        <v>300000</v>
+      </c>
+      <c r="G18" s="20"/>
+    </row>
+    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D19" s="77"/>
+      <c r="E19" s="19" t="s">
+        <v>177</v>
+      </c>
+      <c r="F19" s="12">
+        <v>14900</v>
+      </c>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="77"/>
+      <c r="E20" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="12">
+        <v>54100</v>
+      </c>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="77"/>
+      <c r="E21" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="14">
+        <f>SUM(F9:F20)</f>
+        <v>804695</v>
+      </c>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D22" s="77"/>
+      <c r="E22" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="41">
+        <v>80000</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="77"/>
+      <c r="E23" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="41">
+        <v>26500</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="77"/>
+      <c r="E24" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="41">
+        <v>50000</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="77"/>
+      <c r="E25" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="F25" s="41">
+        <v>14000</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="77"/>
+      <c r="E26" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="41">
+        <v>5000</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H26" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="77"/>
+      <c r="E27" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="41">
+        <v>27000</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D28" s="77"/>
+      <c r="E28" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="F28" s="41">
+        <v>50000</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H28" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D29" s="77"/>
+      <c r="E29" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="F29" s="41">
+        <v>11270</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D30" s="77"/>
+      <c r="E30" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="F30" s="41">
+        <v>21725</v>
+      </c>
+      <c r="G30" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D31" s="77"/>
+      <c r="E31" s="19" t="s">
+        <v>94</v>
+      </c>
+      <c r="F31" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D32" s="77"/>
+      <c r="E32" s="19" t="s">
+        <v>95</v>
+      </c>
+      <c r="F32" s="41">
+        <v>21560</v>
+      </c>
+      <c r="G32" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D33" s="77"/>
+      <c r="E33" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="F33" s="41">
+        <v>7250</v>
+      </c>
+      <c r="G33" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D34" s="77"/>
+      <c r="E34" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="F34" s="41">
+        <v>18600</v>
+      </c>
+      <c r="G34" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D35" s="77"/>
+      <c r="E35" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F35" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G35" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D36" s="77"/>
+      <c r="E36" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F36" s="41">
+        <v>1800</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D37" s="77"/>
+      <c r="E37" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F37" s="41">
+        <v>1750</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D38" s="77"/>
+      <c r="E38" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="41">
+        <v>21300</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" s="77"/>
+      <c r="E39" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="F39" s="41">
+        <v>4700</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="77"/>
+      <c r="E40" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="F40" s="41">
+        <v>5590</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="77"/>
+      <c r="E41" s="19" t="s">
         <v>117</v>
       </c>
-      <c r="F15" s="12">
-        <v>55000</v>
-      </c>
-      <c r="G15" s="20"/>
-    </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="75"/>
-      <c r="E16" s="19" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" s="12">
-        <v>300000</v>
-      </c>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="75"/>
-      <c r="E17" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="12">
-        <v>54100</v>
-      </c>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="75"/>
-      <c r="E18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" s="14">
-        <f>SUM(F9:F17)</f>
-        <v>750445</v>
-      </c>
-      <c r="G18" s="20"/>
-    </row>
-    <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="75"/>
-      <c r="E19" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="F19" s="41">
-        <v>80000</v>
-      </c>
-      <c r="G19" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D20" s="75"/>
-      <c r="E20" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="F20" s="41">
-        <v>26500</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="H20" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D21" s="75"/>
-      <c r="E21" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="F21" s="41">
+      <c r="F41" s="41">
+        <v>30000</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H41" t="s">
+        <v>123</v>
+      </c>
+      <c r="I41">
+        <v>126500</v>
+      </c>
+    </row>
+    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D42" s="77"/>
+      <c r="E42" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F42" s="41">
+        <v>3730</v>
+      </c>
+      <c r="G42" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D43" s="77"/>
+      <c r="E43" s="19" t="s">
+        <v>130</v>
+      </c>
+      <c r="F43" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G43" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H43" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43">
+        <v>136500</v>
+      </c>
+    </row>
+    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D44" s="77"/>
+      <c r="E44" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="F44" s="41">
+        <v>4200</v>
+      </c>
+      <c r="G44" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D45" s="77"/>
+      <c r="E45" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="41">
+        <v>35000</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D46" s="77"/>
+      <c r="E46" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="F46" s="41">
+        <v>16000</v>
+      </c>
+      <c r="G46" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="47" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D47" s="77"/>
+      <c r="E47" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="F47" s="41">
+        <v>63500</v>
+      </c>
+      <c r="G47" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H47" t="s">
+        <v>123</v>
+      </c>
+      <c r="I47">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="48" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D48" s="77"/>
+      <c r="E48" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F48" s="41">
+        <v>11350</v>
+      </c>
+      <c r="G48" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D49" s="77"/>
+      <c r="E49" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="F49" s="41">
+        <v>14900</v>
+      </c>
+      <c r="G49" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D50" s="77"/>
+      <c r="E50" s="19" t="s">
+        <v>167</v>
+      </c>
+      <c r="F50" s="41">
+        <v>20000</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H50" t="s">
+        <v>181</v>
+      </c>
+      <c r="I50">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D51" s="77"/>
+      <c r="E51" s="19" t="s">
+        <v>179</v>
+      </c>
+      <c r="F51" s="41">
+        <v>4350</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D52" s="77"/>
+      <c r="E52" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F52" s="41">
+        <v>15000</v>
+      </c>
+      <c r="G52" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H52" t="s">
+        <v>190</v>
+      </c>
+      <c r="I52">
         <v>50000</v>
       </c>
-      <c r="G21" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D22" s="75"/>
-      <c r="E22" s="19" t="s">
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D53" s="77"/>
+      <c r="E53" s="19" t="s">
+        <v>191</v>
+      </c>
+      <c r="F53" s="41"/>
+      <c r="G53" s="20"/>
+    </row>
+    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D54" s="77"/>
+      <c r="E54" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F54" s="41"/>
+      <c r="G54" s="20"/>
+    </row>
+    <row r="55" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D55" s="77"/>
+      <c r="E55" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F55" s="12">
+        <v>0</v>
+      </c>
+      <c r="G55" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="41">
-        <v>14000</v>
-      </c>
-      <c r="G22" s="20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="75"/>
-      <c r="E23" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="F23" s="41">
-        <v>5000</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D24" s="75"/>
-      <c r="E24" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" s="41">
-        <v>27000</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D25" s="75"/>
-      <c r="E25" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="F25" s="41">
-        <v>50000</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="75"/>
-      <c r="E26" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="F26" s="41">
-        <v>11270</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="75"/>
-      <c r="E27" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="F27" s="41">
-        <v>21725</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D28" s="75"/>
-      <c r="E28" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="F28" s="41">
-        <v>44325</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="75"/>
-      <c r="E29" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="F29" s="41">
-        <v>21560</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D30" s="75"/>
-      <c r="E30" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="F30" s="41">
-        <v>7250</v>
-      </c>
-      <c r="G30" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="31" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D31" s="75"/>
-      <c r="E31" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="F31" s="41">
-        <v>18600</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>36</v>
-      </c>
-      <c r="H31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D32" s="75"/>
-      <c r="E32" s="19" t="s">
-        <v>106</v>
-      </c>
-      <c r="F32" s="41">
-        <v>44325</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="33" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D33" s="75"/>
-      <c r="E33" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="F33" s="41">
-        <v>1800</v>
-      </c>
-      <c r="G33" s="20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="75"/>
-      <c r="E34" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="F34" s="41">
-        <v>1750</v>
-      </c>
-      <c r="G34" s="20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D35" s="75"/>
-      <c r="E35" s="19" t="s">
-        <v>109</v>
-      </c>
-      <c r="F35" s="41">
-        <v>21300</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="75"/>
-      <c r="E36" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F36" s="41">
-        <v>4700</v>
-      </c>
-      <c r="G36" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D37" s="75"/>
-      <c r="E37" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F37" s="41">
-        <v>5590</v>
-      </c>
-      <c r="G37" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D38" s="75"/>
-      <c r="E38" s="19" t="s">
-        <v>118</v>
-      </c>
-      <c r="F38" s="41">
-        <v>30000</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="H38" t="s">
-        <v>124</v>
-      </c>
-      <c r="I38">
-        <v>126500</v>
-      </c>
-    </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D39" s="75"/>
-      <c r="E39" s="19" t="s">
-        <v>119</v>
-      </c>
-      <c r="F39" s="41">
-        <v>3730</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D40" s="75"/>
-      <c r="E40" s="19" t="s">
-        <v>131</v>
-      </c>
-      <c r="F40" s="41">
-        <v>10000</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="H40" t="s">
-        <v>124</v>
-      </c>
-      <c r="I40">
-        <v>136500</v>
-      </c>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D41" s="75"/>
-      <c r="E41" s="19" t="s">
-        <v>132</v>
-      </c>
-      <c r="F41" s="41">
-        <v>4200</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="42" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D42" s="75"/>
-      <c r="E42" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="F42" s="41">
-        <v>35000</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="43" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D43" s="75"/>
-      <c r="E43" s="19" t="s">
-        <v>161</v>
-      </c>
-      <c r="F43" s="41">
-        <v>16000</v>
-      </c>
-      <c r="G43" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="44" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D44" s="75"/>
-      <c r="E44" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="F44" s="41">
-        <v>63500</v>
-      </c>
-      <c r="G44" s="20" t="s">
-        <v>120</v>
-      </c>
-      <c r="H44" t="s">
-        <v>124</v>
-      </c>
-      <c r="I44">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="45" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D45" s="75"/>
-      <c r="E45" s="19" t="s">
-        <v>163</v>
-      </c>
-      <c r="F45" s="41">
-        <v>11350</v>
-      </c>
-      <c r="G45" s="20" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D46" s="75"/>
-      <c r="E46" s="19" t="s">
-        <v>167</v>
-      </c>
-      <c r="F46" s="41"/>
-      <c r="G46" s="20"/>
-    </row>
-    <row r="47" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D47" s="75"/>
-      <c r="E47" s="19" t="s">
-        <v>168</v>
-      </c>
-      <c r="F47" s="12">
-        <v>0</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="48" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D48" s="76"/>
-      <c r="E48" s="1" t="s">
+    </row>
+    <row r="56" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D56" s="78"/>
+      <c r="E56" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F48" s="14">
-        <f>F18-SUM(F19:F47)</f>
+      <c r="F56" s="14">
+        <f>F21-SUM(F22:F55)</f>
         <v>119970</v>
       </c>
-      <c r="G48" s="21"/>
+      <c r="G56" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D48"/>
+    <mergeCell ref="D9:D56"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adde changes as of 03-02-2024
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="524" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8442F2E7-BFE7-4A02-9598-AADFF1CADFB0}"/>
+  <xr:revisionPtr revIDLastSave="632" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{797503A0-CBCD-43A8-A5C4-D36010E672DB}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -65,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K27" authorId="0" shapeId="0" xr:uid="{C6A08A85-8275-4C88-95E8-4526C8E02D7C}">
+    <comment ref="K27" authorId="0" shapeId="0" xr:uid="{0635264B-4CAD-4B16-88AB-506379F47EF7}">
       <text>
         <r>
           <rPr>
@@ -94,7 +94,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M27" authorId="0" shapeId="0" xr:uid="{134DA49D-E84E-4882-A21A-C0FA2F9A36E6}">
+    <comment ref="M27" authorId="0" shapeId="0" xr:uid="{67D78B13-317E-44A1-8CE6-488EF37CC559}">
       <text>
         <r>
           <rPr>
@@ -125,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N27" authorId="0" shapeId="0" xr:uid="{F8374CFC-2A6A-41D3-A4EE-2F8672A0B170}">
+    <comment ref="N27" authorId="0" shapeId="0" xr:uid="{5443A4C3-6A6A-4CEF-AB7E-EAD9BE7E82A0}">
       <text>
         <r>
           <rPr>
@@ -150,6 +150,78 @@
 Sandeep da - 10k
 6k - Sahid da
 1.6k sahid ktchen renovation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K28" authorId="0" shapeId="0" xr:uid="{9C9C7CF7-E494-4E99-A1DA-3545AA62EB81}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Chanchal - 3000(Last payment)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M28" authorId="0" shapeId="0" xr:uid="{8A482139-9742-4E7A-BA35-C5DC9365B6F7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1st - Anam - 20000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N28" authorId="0" shapeId="0" xr:uid="{9B158C32-2D02-4AD8-9620-9AE83B23C3B6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+1st - Sahid da - 2700</t>
         </r>
       </text>
     </comment>
@@ -221,7 +293,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
       <text>
         <r>
           <rPr>
@@ -255,7 +327,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{A259699E-5F47-47AF-BA19-632A69C8F230}">
       <text>
         <r>
           <rPr>
@@ -280,7 +352,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{D1450806-4A02-4411-820D-A285FC83FD29}">
       <text>
         <r>
           <rPr>
@@ -305,7 +377,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{0C41E90F-9375-452E-9DCF-49E0A6F60F76}">
       <text>
         <r>
           <rPr>
@@ -329,7 +401,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{AD00E99E-1BA5-4237-933D-94237C70F5BF}">
       <text>
         <r>
           <rPr>
@@ -353,7 +425,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{ED7A00FA-B24D-4B58-95AA-3AEC555D50C8}">
       <text>
         <r>
           <rPr>
@@ -377,7 +449,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{2BFB4C23-4FA1-4AF8-8E3C-B27012983E0B}">
       <text>
         <r>
           <rPr>
@@ -401,7 +473,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{77029F3E-727D-4401-8054-169CC3026B92}">
       <text>
         <r>
           <rPr>
@@ -425,7 +497,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{1BE20AFC-6ADA-4464-A7A5-C68AAFD30B3D}">
       <text>
         <r>
           <rPr>
@@ -449,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{2D1CA1B3-8C56-426C-9936-DB58E3AFF54D}">
       <text>
         <r>
           <rPr>
@@ -473,7 +545,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{6957C706-9DD7-40E5-ABCE-2D7C3683B6CC}">
       <text>
         <r>
           <rPr>
@@ -497,7 +569,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{9E9CDE10-77E9-4327-BA5C-DC626A7AF83D}">
       <text>
         <r>
           <rPr>
@@ -521,7 +593,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{1E3E7512-5BB0-42F9-BC92-CBABBA91DF39}">
+    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{1E3E7512-5BB0-42F9-BC92-CBABBA91DF39}">
       <text>
         <r>
           <rPr>
@@ -546,7 +618,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{0AA7B1D3-E81F-4D95-8263-EB90FB490E55}">
+    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{0AA7B1D3-E81F-4D95-8263-EB90FB490E55}">
       <text>
         <r>
           <rPr>
@@ -710,6 +782,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{39611792-98E1-4371-899A-334168C0C2EC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+ANAM</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F17" authorId="0" shapeId="0" xr:uid="{E3B0DB5E-EFB2-4183-B2C1-99AD1E10DC45}">
       <text>
         <r>
@@ -730,11 +826,11 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Glass works</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+Glass works - ANAM</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
       <text>
         <r>
           <rPr>
@@ -758,7 +854,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
       <text>
         <r>
           <rPr>
@@ -782,7 +878,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
       <text>
         <r>
           <rPr>
@@ -807,7 +903,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
       <text>
         <r>
           <rPr>
@@ -832,7 +928,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
       <text>
         <r>
           <rPr>
@@ -857,7 +953,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
       <text>
         <r>
           <rPr>
@@ -883,7 +979,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
       <text>
         <r>
           <rPr>
@@ -907,7 +1003,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
       <text>
         <r>
           <rPr>
@@ -931,7 +1027,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
       <text>
         <r>
           <rPr>
@@ -955,7 +1051,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
       <text>
         <r>
           <rPr>
@@ -979,7 +1075,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
       <text>
         <r>
           <rPr>
@@ -1003,7 +1099,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H34" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
+    <comment ref="H35" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
       <text>
         <r>
           <rPr>
@@ -1027,7 +1123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+    <comment ref="F36" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
           <rPr>
@@ -1051,7 +1147,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+    <comment ref="F37" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
       <text>
         <r>
           <rPr>
@@ -1075,7 +1171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
       <text>
         <r>
           <rPr>
@@ -1100,7 +1196,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
       <text>
         <r>
           <rPr>
@@ -1127,7 +1223,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
       <text>
         <r>
           <rPr>
@@ -1151,7 +1247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
       <text>
         <r>
           <rPr>
@@ -1175,7 +1271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
       <text>
         <r>
           <rPr>
@@ -1199,7 +1295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I41" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
+    <comment ref="I42" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
       <text>
         <r>
           <rPr>
@@ -1223,7 +1319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
       <text>
         <r>
           <rPr>
@@ -1247,7 +1343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
       <text>
         <r>
           <rPr>
@@ -1271,7 +1367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I43" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
+    <comment ref="I44" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
       <text>
         <r>
           <rPr>
@@ -1295,7 +1391,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
       <text>
         <r>
           <rPr>
@@ -1319,7 +1415,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
+    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{9801DA58-C7B4-4364-9205-58707072E88C}">
+    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{9801DA58-C7B4-4364-9205-58707072E88C}">
       <text>
         <r>
           <rPr>
@@ -1367,7 +1463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
+    <comment ref="F48" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
       <text>
         <r>
           <rPr>
@@ -1391,7 +1487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I47" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
+    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
       <text>
         <r>
           <rPr>
@@ -1415,7 +1511,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F48" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
+    <comment ref="F49" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
       <text>
         <r>
           <rPr>
@@ -1439,7 +1535,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F49" authorId="0" shapeId="0" xr:uid="{7209404C-B1DE-4988-B78E-695821C66020}">
+    <comment ref="F50" authorId="0" shapeId="0" xr:uid="{7209404C-B1DE-4988-B78E-695821C66020}">
       <text>
         <r>
           <rPr>
@@ -1463,7 +1559,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F50" authorId="0" shapeId="0" xr:uid="{8CD9AA95-66D8-47E8-97CA-B73A6D47FABD}">
+    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{8CD9AA95-66D8-47E8-97CA-B73A6D47FABD}">
       <text>
         <r>
           <rPr>
@@ -1487,7 +1583,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{1CA1BF83-085B-4EEF-9FAE-03AB18F5FC7C}">
+    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{1CA1BF83-085B-4EEF-9FAE-03AB18F5FC7C}">
       <text>
         <r>
           <rPr>
@@ -1511,7 +1607,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{843F7684-8F79-464D-8D4F-0683C00C0A13}">
+    <comment ref="F53" authorId="0" shapeId="0" xr:uid="{843F7684-8F79-464D-8D4F-0683C00C0A13}">
       <text>
         <r>
           <rPr>
@@ -1533,6 +1629,30 @@
           <t xml:space="preserve">
 Anam- Till now 50k
 </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{36363EF2-6EAC-4355-AEC8-861A67E5E666}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Anam</t>
         </r>
       </text>
     </comment>
@@ -1581,7 +1701,8 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-15k paid out of this - 01-12-2023</t>
+15k paid out of this - 01-12-2023
+20k completed with second 5k payment to sahid da</t>
         </r>
       </text>
     </comment>
@@ -1633,7 +1754,31 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{99689982-6292-4165-AD26-14539A18A3BA}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{B9C48C10-6527-4781-AFBF-D2945605C43A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Paid</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{99689982-6292-4165-AD26-14539A18A3BA}">
       <text>
         <r>
           <rPr>
@@ -1657,7 +1802,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{AF35FB86-ED8F-4A26-B190-DD67EF15CFCE}">
+    <comment ref="F21" authorId="0" shapeId="0" xr:uid="{AF35FB86-ED8F-4A26-B190-DD67EF15CFCE}">
       <text>
         <r>
           <rPr>
@@ -1681,7 +1826,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F22" authorId="0" shapeId="0" xr:uid="{16786DDB-AC57-453B-99D7-248BBA1E2047}">
+    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{16786DDB-AC57-453B-99D7-248BBA1E2047}">
       <text>
         <r>
           <rPr>
@@ -1706,7 +1851,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F23" authorId="0" shapeId="0" xr:uid="{C647BD32-4C90-4257-AF43-75E2E0686478}">
+    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{C647BD32-4C90-4257-AF43-75E2E0686478}">
       <text>
         <r>
           <rPr>
@@ -1732,7 +1877,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{E57FE724-2CA6-4078-A874-BDF0213C3E12}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{E57FE724-2CA6-4078-A874-BDF0213C3E12}">
       <text>
         <r>
           <rPr>
@@ -1756,7 +1901,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{199A5F92-BA83-4DB3-A502-ACEE8B96E2D5}">
+    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{199A5F92-BA83-4DB3-A502-ACEE8B96E2D5}">
       <text>
         <r>
           <rPr>
@@ -1782,7 +1927,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{F03B2F0A-2345-4635-B9FB-69E038D76831}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{F03B2F0A-2345-4635-B9FB-69E038D76831}">
       <text>
         <r>
           <rPr>
@@ -1806,7 +1951,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{E95C9AF8-5C84-47C1-8E8A-538A8936C269}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{E95C9AF8-5C84-47C1-8E8A-538A8936C269}">
       <text>
         <r>
           <rPr>
@@ -1830,7 +1975,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{A183F4EA-FB59-4730-B241-1696B70A5F95}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{A183F4EA-FB59-4730-B241-1696B70A5F95}">
       <text>
         <r>
           <rPr>
@@ -1857,7 +2002,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{795FE048-63B4-4A28-BEA6-9ED2DFB591E9}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{795FE048-63B4-4A28-BEA6-9ED2DFB591E9}">
       <text>
         <r>
           <rPr>
@@ -1885,7 +2030,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{BFEC1F17-8CE3-44A8-84E4-53A5FE57EDFC}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{BFEC1F17-8CE3-44A8-84E4-53A5FE57EDFC}">
       <text>
         <r>
           <rPr>
@@ -1909,7 +2054,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{7D69A899-3C94-4DFE-BDDC-B4CC0BC7AF9E}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{7D69A899-3C94-4DFE-BDDC-B4CC0BC7AF9E}">
       <text>
         <r>
           <rPr>
@@ -1934,7 +2079,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{0FC6798B-65E5-4F18-A209-2B4DB72F3A08}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{0FC6798B-65E5-4F18-A209-2B4DB72F3A08}">
       <text>
         <r>
           <rPr>
@@ -1959,7 +2104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{C69A89FF-54F4-4F12-A623-1A80CBA4375A}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{C69A89FF-54F4-4F12-A623-1A80CBA4375A}">
       <text>
         <r>
           <rPr>
@@ -1983,7 +2128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{9104B889-1277-41A2-B9F4-F59470ECD06C}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{9104B889-1277-41A2-B9F4-F59470ECD06C}">
       <text>
         <r>
           <rPr>
@@ -2007,7 +2152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{4798DD2C-9DA1-41D4-8E38-190E059D9E0A}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{4798DD2C-9DA1-41D4-8E38-190E059D9E0A}">
       <text>
         <r>
           <rPr>
@@ -2031,7 +2176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{3AEBB180-7950-4B14-979A-1E21632E12F6}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{3AEBB180-7950-4B14-979A-1E21632E12F6}">
       <text>
         <r>
           <rPr>
@@ -2055,7 +2200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{39308213-7A53-4286-820A-EF5EC7AD39EC}">
+    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{39308213-7A53-4286-820A-EF5EC7AD39EC}">
       <text>
         <r>
           <rPr>
@@ -2076,6 +2221,103 @@
           </rPr>
           <t xml:space="preserve">
 Jacky</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L38" authorId="0" shapeId="0" xr:uid="{8624B1FC-2A2B-4653-98BD-AD9580658BEB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Done</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{6B00E7B5-1026-45A1-9D93-59C4EFFEF3F1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sandeep da last one
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J39" authorId="0" shapeId="0" xr:uid="{2A4F910F-4EDA-4498-8CF5-05C608F88BEC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Done</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{60293CD5-B960-438A-BD76-5DE3A419A58D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sahid da</t>
         </r>
       </text>
     </comment>
@@ -2084,7 +2326,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="205">
   <si>
     <t>Provider</t>
   </si>
@@ -2668,7 +2910,37 @@
     <t>Payment - 35</t>
   </si>
   <si>
-    <t xml:space="preserve">Sanddep da </t>
+    <t>Sandeep da</t>
+  </si>
+  <si>
+    <t>Gaur da</t>
+  </si>
+  <si>
+    <t>Baranah Ceieling</t>
+  </si>
+  <si>
+    <t>Floor Re White cementing</t>
+  </si>
+  <si>
+    <t>Last lot fittings</t>
+  </si>
+  <si>
+    <t>Total Paid</t>
+  </si>
+  <si>
+    <t>Remainig</t>
+  </si>
+  <si>
+    <t>4000 Tiles</t>
+  </si>
+  <si>
+    <t>2000 Sahi Da</t>
+  </si>
+  <si>
+    <t>Santras for Ac outlet and corridor</t>
+  </si>
+  <si>
+    <t>Electrical Additional (Last buys)</t>
   </si>
 </sst>
 </file>
@@ -3291,6 +3563,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3342,7 +3615,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3708,7 +3980,31 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person87.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person88.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person89.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/persons/person9.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person90.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person91.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person92.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -4009,10 +4305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
-  <dimension ref="C7:Q27"/>
+  <dimension ref="C7:Q28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17:J17"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4072,7 +4368,7 @@
         <v>40140</v>
       </c>
       <c r="J9">
-        <f>SUM(G25:G27)</f>
+        <f>SUM(G25:G28)</f>
         <v>294139</v>
       </c>
       <c r="K9" s="4">
@@ -4092,22 +4388,22 @@
         <v>75000</v>
       </c>
       <c r="G10">
-        <f>SUM(Paint!F11:F19)</f>
-        <v>63000</v>
+        <f>SUM(Paint!F11:F20)</f>
+        <v>66930</v>
       </c>
       <c r="H10">
         <v>9283</v>
       </c>
       <c r="I10">
-        <v>20000</v>
+        <v>23930</v>
       </c>
       <c r="J10">
-        <f>SUM(H25:H27)</f>
+        <f>SUM(H25:H28)</f>
         <v>33717</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>12000</v>
+        <v>8070</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.3">
@@ -4118,26 +4414,26 @@
         <v>14</v>
       </c>
       <c r="F11">
-        <f>'False Ceiling'!F11</f>
-        <v>126550</v>
+        <f>'False Ceiling'!F12</f>
+        <v>131550</v>
       </c>
       <c r="G11">
-        <f>SUM('False Ceiling'!F12:F17)</f>
-        <v>126550</v>
+        <f>SUM('False Ceiling'!F13:F19)</f>
+        <v>128750</v>
       </c>
       <c r="H11">
-        <v>1800</v>
+        <v>4000</v>
       </c>
       <c r="I11">
         <v>4750</v>
       </c>
       <c r="J11">
-        <f>SUM(J25:J27)</f>
+        <f>SUM(J25:J28)</f>
         <v>120000</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2800</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.3">
@@ -4148,26 +4444,26 @@
         <v>28</v>
       </c>
       <c r="F12">
-        <f>'Electric &amp; Lights'!F33</f>
-        <v>167869</v>
+        <f>'Electric &amp; Lights'!F34</f>
+        <v>169869</v>
       </c>
       <c r="G12">
-        <f>SUM('Electric &amp; Lights'!F34:F49)</f>
-        <v>164869</v>
+        <f>SUM('Electric &amp; Lights'!F35:F53)</f>
+        <v>169869</v>
       </c>
       <c r="H12">
-        <v>31695</v>
+        <v>33695</v>
       </c>
       <c r="I12">
         <v>23985</v>
       </c>
       <c r="J12">
-        <f>SUM(K25:K27)</f>
-        <v>109189</v>
+        <f>SUM(K25:K28)</f>
+        <v>112189</v>
       </c>
       <c r="K12" s="4">
         <f t="shared" si="0"/>
-        <v>3000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.3">
@@ -4192,7 +4488,7 @@
         <v>10000</v>
       </c>
       <c r="J13">
-        <f>SUM(L25:L27)</f>
+        <f>SUM(L25:L28)</f>
         <v>52700</v>
       </c>
       <c r="K13" s="4">
@@ -4208,26 +4504,26 @@
         <v>26</v>
       </c>
       <c r="F14">
-        <f>Furniture!F21</f>
-        <v>804695</v>
+        <f>Furniture!F22</f>
+        <v>807585</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F22:F55)</f>
-        <v>684725</v>
+        <f>SUM(Furniture!F23:F58)</f>
+        <v>707615</v>
       </c>
       <c r="H14">
-        <v>60950</v>
+        <v>63840</v>
       </c>
       <c r="I14">
         <v>228720</v>
       </c>
       <c r="J14">
-        <f>SUM(M25:M27)</f>
-        <v>395055</v>
+        <f>SUM(M25:M28)</f>
+        <v>415055</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>119970</v>
+        <v>99970</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
@@ -4238,26 +4534,26 @@
         <v>165</v>
       </c>
       <c r="F15">
-        <f>'Bathroom-Kitchen-Barandah'!F21</f>
-        <v>343950</v>
+        <f>'Bathroom-Kitchen-Barandah'!F22</f>
+        <v>345150</v>
       </c>
       <c r="G15">
-        <f>SUM('Bathroom-Kitchen-Barandah'!F22:F40)</f>
-        <v>316888</v>
+        <f>SUM('Bathroom-Kitchen-Barandah'!F23:F42)</f>
+        <v>324588</v>
       </c>
       <c r="H15">
         <v>129000</v>
       </c>
       <c r="I15">
-        <v>87988</v>
+        <v>92988</v>
       </c>
       <c r="J15">
-        <f>SUM(N25:N27)</f>
-        <v>99900</v>
+        <f>SUM(N25:N28)</f>
+        <v>102600</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>27062</v>
+        <v>20562</v>
       </c>
     </row>
     <row r="16" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4269,17 +4565,20 @@
       </c>
       <c r="F16">
         <f>Civil!F12</f>
-        <v>30500</v>
+        <v>35500</v>
       </c>
       <c r="G16">
         <f>SUM(Civil!F13:F16)</f>
-        <v>30500</v>
+        <v>35500</v>
       </c>
       <c r="H16">
         <v>5200</v>
       </c>
+      <c r="I16">
+        <v>5000</v>
+      </c>
       <c r="J16">
-        <f>SUM(O25:O27)</f>
+        <f>SUM(O25:O28)</f>
         <v>25300</v>
       </c>
       <c r="K16" s="4">
@@ -4294,27 +4593,27 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>1991843</v>
+        <v>2007933</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1819811</v>
+        <v>1866531</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>314368</v>
+        <v>321458</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
-        <v>375443</v>
+        <v>389373</v>
       </c>
       <c r="J17" s="2">
         <f>SUM(J9:J16)</f>
-        <v>1130000</v>
+        <v>1155700</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>172032</v>
+        <v>141402</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
@@ -4331,7 +4630,7 @@
       </c>
       <c r="F19" s="28">
         <f>SUM(H17,I17)</f>
-        <v>689811</v>
+        <v>710831</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
@@ -4340,11 +4639,11 @@
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>89032</v>
+        <v>84102</v>
       </c>
       <c r="G20" s="61">
         <f>F20-SUM('Extra Source'!G68,'Extra Source'!G55)</f>
-        <v>69032</v>
+        <v>73032</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>189</v>
@@ -4356,7 +4655,7 @@
       </c>
       <c r="F21" s="28">
         <f>K17</f>
-        <v>172032</v>
+        <v>141402</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.3">
@@ -4365,27 +4664,27 @@
       </c>
       <c r="F22" s="28">
         <f>F21-F20</f>
-        <v>83000</v>
+        <v>57300</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="62" t="s">
+      <c r="C23" s="63" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
-      <c r="L23" s="62"/>
-      <c r="M23" s="62"/>
-      <c r="N23" s="62"/>
-      <c r="O23" s="62"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="62"/>
+      <c r="D23" s="63"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="63"/>
+      <c r="G23" s="63"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
+      <c r="J23" s="63"/>
+      <c r="K23" s="63"/>
+      <c r="L23" s="63"/>
+      <c r="M23" s="63"/>
+      <c r="N23" s="63"/>
+      <c r="O23" s="63"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="63"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" s="33" t="s">
@@ -4515,7 +4814,7 @@
         <v>438810</v>
       </c>
       <c r="Q26" s="28">
-        <f t="shared" ref="Q26:Q27" si="1">SUM(E26,D26)-P26</f>
+        <f t="shared" ref="Q26" si="1">SUM(E26,D26)-P26</f>
         <v>61190</v>
       </c>
     </row>
@@ -4524,7 +4823,7 @@
         <v>3</v>
       </c>
       <c r="D27" s="28">
-        <f>D26+Q26</f>
+        <f>Q26</f>
         <v>61190</v>
       </c>
       <c r="E27" s="28">
@@ -4559,8 +4858,50 @@
         <v>391190</v>
       </c>
       <c r="Q27" s="28">
-        <f t="shared" si="1"/>
+        <f>SUM(E27,D27)-P27</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="C28" s="28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="28">
+        <f>Q27</f>
+        <v>0</v>
+      </c>
+      <c r="E28" s="28">
+        <v>83000</v>
+      </c>
+      <c r="F28" s="39">
+        <v>45322</v>
+      </c>
+      <c r="G28" s="28"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40">
+        <v>0</v>
+      </c>
+      <c r="K28" s="40">
+        <v>3000</v>
+      </c>
+      <c r="L28" s="40">
+        <v>0</v>
+      </c>
+      <c r="M28" s="40">
+        <v>20000</v>
+      </c>
+      <c r="N28" s="40">
+        <v>2700</v>
+      </c>
+      <c r="O28" s="28"/>
+      <c r="P28" s="28">
+        <f>SUM(G28:O28)</f>
+        <v>25700</v>
+      </c>
+      <c r="Q28" s="28">
+        <f>SUM(E28,D28)-P28</f>
+        <v>57300</v>
       </c>
     </row>
   </sheetData>
@@ -4574,10 +4915,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD019853-AAD7-4C4A-AE9D-387A8C77D1D3}">
-  <dimension ref="D7:N41"/>
+  <dimension ref="D7:N43"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="N38" sqref="N38"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="E40" sqref="E40:E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4605,7 +4946,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -4617,7 +4958,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="11" t="s">
         <v>23</v>
       </c>
@@ -4627,7 +4968,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="71"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="11" t="s">
         <v>65</v>
       </c>
@@ -4637,7 +4978,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="11" t="s">
         <v>78</v>
       </c>
@@ -4647,7 +4988,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="11" t="s">
         <v>79</v>
       </c>
@@ -4657,7 +4998,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="11" t="s">
         <v>81</v>
       </c>
@@ -4667,7 +5008,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="11" t="s">
         <v>80</v>
       </c>
@@ -4677,7 +5018,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="71"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="11" t="s">
         <v>133</v>
       </c>
@@ -4686,18 +5027,18 @@
       </c>
       <c r="G16" s="20"/>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="71"/>
+    <row r="17" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D17" s="72"/>
       <c r="E17" s="11" t="s">
         <v>135</v>
       </c>
       <c r="F17" s="32">
-        <v>6500</v>
+        <v>7000</v>
       </c>
       <c r="G17" s="20"/>
     </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="71"/>
+    <row r="18" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D18" s="72"/>
       <c r="E18" s="11" t="s">
         <v>148</v>
       </c>
@@ -4706,285 +5047,331 @@
       </c>
       <c r="G18" s="20"/>
     </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="71"/>
+    <row r="19" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D19" s="72"/>
       <c r="E19" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="32">
+        <v>700</v>
+      </c>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D20" s="72"/>
+      <c r="E20" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="F19" s="32">
+      <c r="F20" s="32">
         <v>4850</v>
       </c>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="71"/>
-      <c r="E20" s="11" t="s">
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="72"/>
+      <c r="E21" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F21" s="12">
         <v>15000</v>
       </c>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="71"/>
-      <c r="E21" s="13" t="s">
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="72"/>
+      <c r="E22" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="14">
-        <f>SUM(F9:F20)</f>
-        <v>343950</v>
-      </c>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="71"/>
-      <c r="E22" s="11" t="s">
+      <c r="F22" s="14">
+        <f>SUM(F9:F21)</f>
+        <v>345150</v>
+      </c>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D23" s="72"/>
+      <c r="E23" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="41">
+      <c r="F23" s="41">
         <v>50000</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="71"/>
-      <c r="E23" s="11" t="s">
+    <row r="24" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D24" s="72"/>
+      <c r="E24" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="41">
+      <c r="F24" s="41">
         <v>23500</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G24" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="71"/>
-      <c r="E24" s="11" t="s">
+    <row r="25" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D25" s="72"/>
+      <c r="E25" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F25" s="41">
         <v>50000</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="71"/>
-      <c r="E25" s="11" t="s">
+    <row r="26" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D26" s="72"/>
+      <c r="E26" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F26" s="41">
         <v>40000</v>
-      </c>
-      <c r="G25" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="71"/>
-      <c r="E26" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="F26" s="41">
-        <v>2300</v>
       </c>
       <c r="G26" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="71"/>
+    <row r="27" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D27" s="72"/>
       <c r="E27" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="41">
+        <v>2300</v>
+      </c>
+      <c r="G27" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D28" s="72"/>
+      <c r="E28" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="41">
+      <c r="F28" s="41">
         <v>5500</v>
       </c>
-      <c r="G27" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="71"/>
-      <c r="E28" s="11" t="s">
+    <row r="29" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D29" s="72"/>
+      <c r="E29" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="41">
+      <c r="F29" s="41">
         <v>50000</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="71"/>
-      <c r="E29" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F29" s="41">
-        <v>6000</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="71"/>
+    <row r="30" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D30" s="72"/>
       <c r="E30" s="11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="41">
-        <v>1600</v>
+        <v>6000</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="71"/>
+      <c r="H30" t="s">
+        <v>201</v>
+      </c>
+      <c r="I30" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="31" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D31" s="72"/>
       <c r="E31" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="41">
+        <v>1600</v>
+      </c>
+      <c r="G31" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D32" s="72"/>
+      <c r="E32" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="F31" s="41">
+      <c r="F32" s="41">
         <v>15000</v>
-      </c>
-      <c r="G31" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="71"/>
-      <c r="E32" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="F32" s="41">
-        <v>4000</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="33" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D33" s="71"/>
+      <c r="D33" s="72"/>
       <c r="E33" s="11" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" s="41">
-        <v>4550</v>
+        <v>4000</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="34" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D34" s="71"/>
+      <c r="D34" s="72"/>
       <c r="E34" s="11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" s="41">
-        <v>7000</v>
+        <v>4550</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D35" s="71"/>
+      <c r="D35" s="72"/>
       <c r="E35" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F35" s="41">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="36" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D36" s="71"/>
+      <c r="D36" s="72"/>
       <c r="E36" s="11" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F36" s="41">
-        <v>40000</v>
+        <v>5000</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="37" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D37" s="71"/>
+      <c r="D37" s="72"/>
       <c r="E37" s="11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F37" s="41">
-        <v>12438</v>
+        <v>40000</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H37" t="s">
+      <c r="I37" t="s">
+        <v>199</v>
+      </c>
+      <c r="J37" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D38" s="72"/>
+      <c r="E38" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="F38" s="41">
+        <v>12438</v>
+      </c>
+      <c r="G38" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H38" t="s">
         <v>186</v>
       </c>
-      <c r="I37">
+      <c r="I38">
         <v>100438</v>
       </c>
-      <c r="J37" t="s">
+      <c r="J38">
+        <f>F9-I38</f>
+        <v>20562</v>
+      </c>
+      <c r="L38" s="62" t="s">
+        <v>190</v>
+      </c>
+      <c r="M38" s="62">
+        <v>32000</v>
+      </c>
+      <c r="N38" s="62">
+        <f>SUM(I38,K38,M38)</f>
+        <v>132438</v>
+      </c>
+    </row>
+    <row r="39" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D39" s="72"/>
+      <c r="E39" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F39" s="41">
+        <v>5000</v>
+      </c>
+      <c r="G39" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="J39" s="62" t="s">
         <v>194</v>
       </c>
-      <c r="K37">
-        <v>10000</v>
-      </c>
-      <c r="L37" t="s">
-        <v>190</v>
-      </c>
-      <c r="M37">
-        <v>32000</v>
-      </c>
-      <c r="N37">
-        <f>SUM(I37,K37,M37)</f>
-        <v>142438</v>
-      </c>
-    </row>
-    <row r="38" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D38" s="71"/>
-      <c r="E38" s="11"/>
-      <c r="F38" s="41"/>
-      <c r="G38" s="20"/>
-    </row>
-    <row r="39" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D39" s="71"/>
-      <c r="E39" s="11"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="20"/>
-    </row>
-    <row r="40" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D40" s="71"/>
+      <c r="K39" s="62">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="40" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D40" s="72"/>
       <c r="E40" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="F40" s="12"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>108</v>
+      </c>
+      <c r="F40" s="41">
+        <v>2700</v>
+      </c>
+      <c r="G40" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="41" spans="4:14" x14ac:dyDescent="0.3">
       <c r="D41" s="72"/>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="F41" s="41"/>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D42" s="72"/>
+      <c r="E42" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F42" s="12"/>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D43" s="73"/>
+      <c r="E43" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F41" s="14">
-        <f>F21-SUM(F22:F40)</f>
-        <v>27062</v>
-      </c>
-      <c r="G41" s="21"/>
+      <c r="F43" s="14">
+        <f>F22-SUM(F23:F42)</f>
+        <v>20562</v>
+      </c>
+      <c r="G43" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D41"/>
+    <mergeCell ref="D9:D43"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4997,7 +5384,7 @@
   <dimension ref="D6:I80"/>
   <sheetViews>
     <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I67" sqref="I67"/>
+      <selection activeCell="G68" sqref="G68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5009,18 +5396,18 @@
   <sheetData>
     <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="67" t="s">
+      <c r="D7" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="68"/>
-      <c r="G7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="70"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="63" t="s">
+      <c r="D8" s="64" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="65">
+      <c r="E8" s="66">
         <v>45000</v>
       </c>
       <c r="F8" s="48" t="s">
@@ -5031,8 +5418,8 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="64"/>
-      <c r="E9" s="66"/>
+      <c r="D9" s="65"/>
+      <c r="E9" s="67"/>
       <c r="F9" s="28" t="s">
         <v>16</v>
       </c>
@@ -5041,8 +5428,8 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="64"/>
-      <c r="E10" s="66"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="67"/>
       <c r="F10" s="47" t="s">
         <v>55</v>
       </c>
@@ -5447,13 +5834,13 @@
       </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F52" s="79" t="s">
+      <c r="F52" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="G52" s="79">
+      <c r="G52" s="59">
         <v>2438</v>
       </c>
-      <c r="H52" s="79" t="s">
+      <c r="H52" s="59" t="s">
         <v>150</v>
       </c>
     </row>
@@ -5495,7 +5882,7 @@
       </c>
       <c r="I62">
         <f>SUM(G62:G67)</f>
-        <v>60000</v>
+        <v>68930</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.3">
@@ -5510,26 +5897,48 @@
       </c>
     </row>
     <row r="64" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="F64" s="79" t="s">
+      <c r="F64" s="59" t="s">
         <v>186</v>
       </c>
-      <c r="G64" s="79">
+      <c r="G64" s="59">
         <v>10000</v>
       </c>
-      <c r="H64" s="79" t="s">
+      <c r="H64" s="59" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="6:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>194</v>
+      </c>
+      <c r="G65">
+        <v>5000</v>
+      </c>
+      <c r="H65" s="59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="6:8" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>195</v>
+      </c>
+      <c r="G66">
+        <v>3930</v>
+      </c>
+      <c r="H66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="68" spans="6:8" x14ac:dyDescent="0.3">
       <c r="F68" t="s">
         <v>10</v>
       </c>
       <c r="G68">
         <f>E61-I62</f>
-        <v>20000</v>
-      </c>
-    </row>
-    <row r="80" spans="6:7" x14ac:dyDescent="0.3">
+        <v>11070</v>
+      </c>
+    </row>
+    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
       <c r="G80">
         <f>E61-SUM(G62:G79)</f>
         <v>0</v>
@@ -5550,7 +5959,7 @@
   <dimension ref="D7:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5578,7 +5987,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -5590,7 +5999,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" t="s">
         <v>4</v>
       </c>
@@ -5600,7 +6009,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="71"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
@@ -5611,7 +6020,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" t="s">
         <v>7</v>
       </c>
@@ -5623,7 +6032,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" t="s">
         <v>8</v>
       </c>
@@ -5635,7 +6044,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" t="s">
         <v>9</v>
       </c>
@@ -5647,7 +6056,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
@@ -5668,10 +6077,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5512692-EDEE-4A22-9F00-43BA354170EF}">
-  <dimension ref="D7:G20"/>
+  <dimension ref="D7:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5698,7 +6107,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -5710,7 +6119,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
@@ -5721,7 +6130,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="71"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="11" t="s">
         <v>31</v>
       </c>
@@ -5733,7 +6142,7 @@
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="11" t="s">
         <v>30</v>
       </c>
@@ -5745,7 +6154,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="11" t="s">
         <v>98</v>
       </c>
@@ -5757,7 +6166,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="11" t="s">
         <v>99</v>
       </c>
@@ -5769,7 +6178,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="11" t="s">
         <v>100</v>
       </c>
@@ -5781,7 +6190,7 @@
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="71"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="11" t="s">
         <v>121</v>
       </c>
@@ -5793,7 +6202,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="71"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="11" t="s">
         <v>122</v>
       </c>
@@ -5805,7 +6214,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="71"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="11" t="s">
         <v>174</v>
       </c>
@@ -5816,32 +6225,44 @@
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="71"/>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="72"/>
       <c r="E19" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="F19" s="12">
-        <v>0</v>
+      <c r="F19" s="41">
+        <v>3930</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>35</v>
+        <v>119</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D20" s="72"/>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F20" s="12">
+        <v>0</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="73"/>
+      <c r="E21" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="14">
-        <f>F10-SUM(F11:F19)</f>
-        <v>12000</v>
-      </c>
-      <c r="G20" s="21"/>
+      <c r="F21" s="14">
+        <f>F10-SUM(F11:F20)</f>
+        <v>8070</v>
+      </c>
+      <c r="G21" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D20"/>
+    <mergeCell ref="D9:D21"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5851,10 +6272,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB69F67B-3322-470C-8A9C-70E95A023898}">
-  <dimension ref="D7:G18"/>
+  <dimension ref="D7:G20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5881,7 +6302,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -5893,108 +6314,130 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="F10" s="10">
+        <v>4800</v>
+      </c>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D11" s="72"/>
+      <c r="E11" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F10" s="10">
-        <v>1800</v>
-      </c>
-      <c r="G10" s="20"/>
-    </row>
-    <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="71"/>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="10">
+        <v>2000</v>
+      </c>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="72"/>
+      <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F11" s="14">
-        <f>SUM(F9:F10)</f>
-        <v>126550</v>
-      </c>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="71"/>
-      <c r="E12" s="11" t="s">
+      <c r="F12" s="14">
+        <f>SUM(F9:F11)</f>
+        <v>131550</v>
+      </c>
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D13" s="72"/>
+      <c r="E13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F13" s="42">
         <v>50000</v>
-      </c>
-      <c r="G12" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="71"/>
-      <c r="E13" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F13" s="42">
-        <v>40000</v>
       </c>
       <c r="G13" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F14" s="42">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F15" s="42">
+        <v>30000</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D16" s="72"/>
+      <c r="E16" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F15" s="42">
+      <c r="F16" s="42">
         <v>4750</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G16" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="71"/>
-      <c r="E16" s="11" t="s">
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="72"/>
+      <c r="E17" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F17" s="42">
         <v>1800</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="71"/>
-      <c r="E17" s="11" t="s">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="72"/>
+      <c r="E18" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="42"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D18" s="72"/>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="42">
+        <v>2200</v>
+      </c>
+      <c r="G18" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D19" s="72"/>
+      <c r="E19" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="F19" s="42"/>
+      <c r="G19" s="20"/>
+    </row>
+    <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D20" s="73"/>
+      <c r="E20" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="14">
-        <f>F11-SUM(F12:F17)</f>
-        <v>0</v>
-      </c>
-      <c r="G18" s="21"/>
+      <c r="F20" s="14">
+        <f>F12-SUM(F13:F19)</f>
+        <v>2800</v>
+      </c>
+      <c r="G20" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D18"/>
+    <mergeCell ref="D9:D20"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6004,10 +6447,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1544B4-216C-4DA0-B248-9403EAEF3872}">
-  <dimension ref="D7:G50"/>
+  <dimension ref="D7:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F48" sqref="F47:F48"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6034,7 +6477,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="73" t="s">
+      <c r="D9" s="74" t="s">
         <v>159</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -6046,7 +6489,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="74"/>
+      <c r="D10" s="75"/>
       <c r="E10" s="11" t="s">
         <v>141</v>
       </c>
@@ -6056,7 +6499,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="74"/>
+      <c r="D11" s="75"/>
       <c r="E11" t="s">
         <v>72</v>
       </c>
@@ -6066,7 +6509,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="74"/>
+      <c r="D12" s="75"/>
       <c r="E12" t="s">
         <v>101</v>
       </c>
@@ -6076,7 +6519,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="74"/>
+      <c r="D13" s="75"/>
       <c r="E13" t="s">
         <v>142</v>
       </c>
@@ -6086,7 +6529,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="74"/>
+      <c r="D14" s="75"/>
       <c r="E14" t="s">
         <v>73</v>
       </c>
@@ -6096,7 +6539,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="74"/>
+      <c r="D15" s="75"/>
       <c r="E15" t="s">
         <v>84</v>
       </c>
@@ -6106,7 +6549,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="74"/>
+      <c r="D16" s="75"/>
       <c r="E16" t="s">
         <v>83</v>
       </c>
@@ -6116,7 +6559,7 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="74"/>
+      <c r="D17" s="75"/>
       <c r="E17" t="s">
         <v>143</v>
       </c>
@@ -6126,7 +6569,7 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="74"/>
+      <c r="D18" s="75"/>
       <c r="E18" t="s">
         <v>144</v>
       </c>
@@ -6136,7 +6579,7 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="74"/>
+      <c r="D19" s="75"/>
       <c r="E19" t="s">
         <v>85</v>
       </c>
@@ -6146,7 +6589,7 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="74"/>
+      <c r="D20" s="75"/>
       <c r="E20" t="s">
         <v>145</v>
       </c>
@@ -6156,7 +6599,7 @@
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="74"/>
+      <c r="D21" s="75"/>
       <c r="E21" t="s">
         <v>89</v>
       </c>
@@ -6164,7 +6607,7 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="74"/>
+      <c r="D22" s="75"/>
       <c r="E22" t="s">
         <v>87</v>
       </c>
@@ -6174,7 +6617,7 @@
       <c r="G22" s="20"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="74"/>
+      <c r="D23" s="75"/>
       <c r="E23" t="s">
         <v>155</v>
       </c>
@@ -6184,7 +6627,7 @@
       <c r="G23" s="20"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="74"/>
+      <c r="D24" s="75"/>
       <c r="E24" t="s">
         <v>86</v>
       </c>
@@ -6194,7 +6637,7 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="74"/>
+      <c r="D25" s="75"/>
       <c r="E25" t="s">
         <v>146</v>
       </c>
@@ -6204,7 +6647,7 @@
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="74"/>
+      <c r="D26" s="75"/>
       <c r="E26" t="s">
         <v>147</v>
       </c>
@@ -6214,7 +6657,7 @@
       <c r="G26" s="20"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="74"/>
+      <c r="D27" s="75"/>
       <c r="E27" t="s">
         <v>69</v>
       </c>
@@ -6224,7 +6667,7 @@
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="74"/>
+      <c r="D28" s="75"/>
       <c r="E28" t="s">
         <v>70</v>
       </c>
@@ -6234,7 +6677,7 @@
       <c r="G28" s="20"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="74"/>
+      <c r="D29" s="75"/>
       <c r="E29" t="s">
         <v>29</v>
       </c>
@@ -6244,7 +6687,7 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="74"/>
+      <c r="D30" s="75"/>
       <c r="E30" t="s">
         <v>170</v>
       </c>
@@ -6254,7 +6697,7 @@
       <c r="G30" s="20"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="74"/>
+      <c r="D31" s="75"/>
       <c r="E31" t="s">
         <v>171</v>
       </c>
@@ -6263,229 +6706,271 @@
       </c>
       <c r="G31" s="20"/>
     </row>
-    <row r="32" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D32" s="74"/>
+    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D32" s="75"/>
       <c r="E32" t="s">
+        <v>204</v>
+      </c>
+      <c r="F32" s="4">
+        <v>2000</v>
+      </c>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D33" s="75"/>
+      <c r="E33" t="s">
         <v>88</v>
       </c>
-      <c r="F32" s="4">
+      <c r="F33" s="4">
         <v>15350</v>
       </c>
-      <c r="G32" s="20"/>
-    </row>
-    <row r="33" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="74"/>
-      <c r="E33" s="1" t="s">
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D34" s="75"/>
+      <c r="E34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="3">
-        <f>SUM(F9:F32)</f>
-        <v>167869</v>
-      </c>
-      <c r="G33" s="20"/>
-    </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D34" s="74"/>
-      <c r="E34" t="s">
+      <c r="F34" s="3">
+        <f>SUM(F9:F33)</f>
+        <v>169869</v>
+      </c>
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D35" s="75"/>
+      <c r="E35" t="s">
         <v>31</v>
       </c>
-      <c r="F34" s="41">
+      <c r="F35" s="41">
         <v>16345</v>
       </c>
-      <c r="G34" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="74"/>
-      <c r="E35" t="s">
+    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D36" s="75"/>
+      <c r="E36" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="41">
+      <c r="F36" s="41">
         <v>11088</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="74"/>
-      <c r="E36" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="41">
-        <v>4100</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="74"/>
+      <c r="D37" s="75"/>
       <c r="E37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F37" s="41">
-        <v>6903</v>
+        <v>4100</v>
       </c>
       <c r="G37" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="74"/>
+      <c r="D38" s="75"/>
       <c r="E38" t="s">
-        <v>67</v>
+        <v>34</v>
       </c>
       <c r="F38" s="41">
-        <v>36280</v>
+        <v>6903</v>
       </c>
       <c r="G38" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D39" s="74"/>
+      <c r="D39" s="75"/>
       <c r="E39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F39" s="41">
-        <v>8805</v>
+        <v>36280</v>
       </c>
       <c r="G39" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D40" s="74"/>
+      <c r="D40" s="75"/>
       <c r="E40" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="F40" s="41">
-        <v>31700</v>
+        <v>8805</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D41" s="74"/>
+      <c r="D41" s="75"/>
       <c r="E41" t="s">
+        <v>74</v>
+      </c>
+      <c r="F41" s="41">
+        <v>31700</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D42" s="75"/>
+      <c r="E42" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="41">
+      <c r="F42" s="41">
         <v>15350</v>
       </c>
-      <c r="G41" s="20" t="s">
+      <c r="G42" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D42" s="74"/>
-      <c r="E42" t="s">
+    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D43" s="75"/>
+      <c r="E43" t="s">
         <v>77</v>
       </c>
-      <c r="F42" s="41">
+      <c r="F43" s="41">
         <v>5454</v>
-      </c>
-      <c r="G42" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="74"/>
-      <c r="E43" t="s">
-        <v>93</v>
-      </c>
-      <c r="F43" s="41">
-        <v>2859</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D44" s="74"/>
+      <c r="D44" s="75"/>
       <c r="E44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F44" s="41">
-        <v>2000</v>
+        <v>2859</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D45" s="74"/>
+      <c r="D45" s="75"/>
       <c r="E45" t="s">
+        <v>94</v>
+      </c>
+      <c r="F45" s="41">
+        <v>2000</v>
+      </c>
+      <c r="G45" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="46" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D46" s="75"/>
+      <c r="E46" t="s">
         <v>95</v>
       </c>
-      <c r="F45" s="41">
+      <c r="F46" s="41">
         <v>9030</v>
       </c>
-      <c r="G45" s="20" t="s">
+      <c r="G46" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D46" s="74"/>
-      <c r="E46" t="s">
+    <row r="47" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D47" s="75"/>
+      <c r="E47" t="s">
         <v>96</v>
       </c>
-      <c r="F46" s="41">
+      <c r="F47" s="41">
         <v>2250</v>
       </c>
-      <c r="G46" s="20" t="s">
+      <c r="G47" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D47" s="74"/>
-      <c r="E47" t="s">
+    <row r="48" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D48" s="75"/>
+      <c r="E48" t="s">
         <v>97</v>
       </c>
-      <c r="F47" s="41">
+      <c r="F48" s="41">
         <v>7705</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D48" s="74"/>
-      <c r="E48" t="s">
-        <v>105</v>
-      </c>
-      <c r="F48" s="41">
-        <v>5000</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="49" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D49" s="74"/>
+    <row r="49" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D49" s="75"/>
       <c r="E49" t="s">
+        <v>105</v>
+      </c>
+      <c r="F49" s="41">
+        <v>5000</v>
+      </c>
+      <c r="G49" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D50" s="75"/>
+      <c r="E50" t="s">
         <v>106</v>
       </c>
-      <c r="F49" s="4"/>
-      <c r="G49" s="20"/>
-    </row>
-    <row r="50" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D50" s="75"/>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="41">
+        <v>3000</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="51" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D51" s="75"/>
+      <c r="E51" t="s">
+        <v>107</v>
+      </c>
+      <c r="F51" s="41">
+        <v>2000</v>
+      </c>
+      <c r="G51" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="52" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D52" s="75"/>
+      <c r="E52" t="s">
+        <v>108</v>
+      </c>
+      <c r="F52" s="41"/>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D53" s="75"/>
+      <c r="E53" t="s">
+        <v>114</v>
+      </c>
+      <c r="F53" s="4"/>
+      <c r="G53" s="20"/>
+    </row>
+    <row r="54" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D54" s="76"/>
+      <c r="E54" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="3">
-        <f>F33-SUM(F34:F49)</f>
-        <v>3000</v>
-      </c>
-      <c r="G50" s="21"/>
+      <c r="F54" s="3">
+        <f>F34-SUM(F35:F53)</f>
+        <v>0</v>
+      </c>
+      <c r="G54" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D50"/>
+    <mergeCell ref="D9:D54"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6498,7 +6983,7 @@
   <dimension ref="D7:G23"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6525,7 +7010,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>137</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -6537,7 +7022,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="11" t="s">
         <v>18</v>
       </c>
@@ -6547,7 +7032,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="71"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="11" t="s">
         <v>43</v>
       </c>
@@ -6557,7 +7042,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="11" t="s">
         <v>102</v>
       </c>
@@ -6567,7 +7052,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="11" t="s">
         <v>178</v>
       </c>
@@ -6577,7 +7062,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="11" t="s">
         <v>19</v>
       </c>
@@ -6587,7 +7072,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="13" t="s">
         <v>6</v>
       </c>
@@ -6598,7 +7083,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="71"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="11" t="s">
         <v>31</v>
       </c>
@@ -6610,7 +7095,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="71"/>
+      <c r="D17" s="72"/>
       <c r="E17" s="11" t="s">
         <v>33</v>
       </c>
@@ -6622,7 +7107,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="71"/>
+      <c r="D18" s="72"/>
       <c r="E18" s="11" t="s">
         <v>32</v>
       </c>
@@ -6634,7 +7119,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="71"/>
+      <c r="D19" s="72"/>
       <c r="E19" s="11" t="s">
         <v>34</v>
       </c>
@@ -6646,7 +7131,7 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="71"/>
+      <c r="D20" s="72"/>
       <c r="E20" s="11" t="s">
         <v>67</v>
       </c>
@@ -6658,7 +7143,7 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="71"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="11" t="s">
         <v>74</v>
       </c>
@@ -6670,7 +7155,7 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="71"/>
+      <c r="D22" s="72"/>
       <c r="E22" s="11" t="s">
         <v>76</v>
       </c>
@@ -6678,7 +7163,7 @@
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="72"/>
+      <c r="D23" s="73"/>
       <c r="E23" s="13" t="s">
         <v>13</v>
       </c>
@@ -6702,7 +7187,7 @@
   <dimension ref="D7:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6729,7 +7214,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="70" t="s">
+      <c r="D9" s="71" t="s">
         <v>103</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -6741,7 +7226,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="71"/>
+      <c r="D10" s="72"/>
       <c r="E10" s="31" t="s">
         <v>42</v>
       </c>
@@ -6751,26 +7236,28 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="71"/>
+      <c r="D11" s="72"/>
       <c r="E11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F11" s="12"/>
+        <v>197</v>
+      </c>
+      <c r="F11" s="12">
+        <v>5000</v>
+      </c>
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="71"/>
+      <c r="D12" s="72"/>
       <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F12" s="14">
         <f>SUM(F9:F11)</f>
-        <v>30500</v>
+        <v>35500</v>
       </c>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="71"/>
+      <c r="D13" s="72"/>
       <c r="E13" s="11" t="s">
         <v>31</v>
       </c>
@@ -6782,7 +7269,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="71"/>
+      <c r="D14" s="72"/>
       <c r="E14" s="11" t="s">
         <v>33</v>
       </c>
@@ -6794,7 +7281,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="71"/>
+      <c r="D15" s="72"/>
       <c r="E15" s="11" t="s">
         <v>32</v>
       </c>
@@ -6806,19 +7293,19 @@
       </c>
     </row>
     <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="71"/>
+      <c r="D16" s="72"/>
       <c r="E16" s="11" t="s">
         <v>34</v>
       </c>
       <c r="F16" s="12">
-        <v>0</v>
+        <v>5000</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="72"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
       </c>
@@ -6838,10 +7325,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:I56"/>
+  <dimension ref="D7:I59"/>
   <sheetViews>
-    <sheetView topLeftCell="C32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51:E55"/>
+    <sheetView topLeftCell="C42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C57" sqref="A57:XFD57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6868,7 +7355,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="76" t="s">
+      <c r="D9" s="77" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="18" t="s">
@@ -6880,7 +7367,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="77"/>
+      <c r="D10" s="78"/>
       <c r="E10" s="19" t="s">
         <v>104</v>
       </c>
@@ -6890,7 +7377,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="77"/>
+      <c r="D11" s="78"/>
       <c r="E11" s="19" t="s">
         <v>91</v>
       </c>
@@ -6900,7 +7387,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="77"/>
+      <c r="D12" s="78"/>
       <c r="E12" s="19" t="s">
         <v>21</v>
       </c>
@@ -6910,7 +7397,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="77"/>
+      <c r="D13" s="78"/>
       <c r="E13" s="19" t="s">
         <v>125</v>
       </c>
@@ -6920,7 +7407,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D14" s="77"/>
+      <c r="D14" s="78"/>
       <c r="E14" s="60" t="s">
         <v>183</v>
       </c>
@@ -6930,7 +7417,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="77"/>
+      <c r="D15" s="78"/>
       <c r="E15" s="19" t="s">
         <v>134</v>
       </c>
@@ -6940,7 +7427,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="77"/>
+      <c r="D16" s="78"/>
       <c r="E16" s="19" t="s">
         <v>182</v>
       </c>
@@ -6950,7 +7437,7 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="77"/>
+      <c r="D17" s="78"/>
       <c r="E17" s="19" t="s">
         <v>116</v>
       </c>
@@ -6960,7 +7447,7 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="77"/>
+      <c r="D18" s="78"/>
       <c r="E18" s="19" t="s">
         <v>22</v>
       </c>
@@ -6970,7 +7457,7 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="77"/>
+      <c r="D19" s="78"/>
       <c r="E19" s="19" t="s">
         <v>177</v>
       </c>
@@ -6979,483 +7466,519 @@
       </c>
       <c r="G19" s="20"/>
     </row>
-    <row r="20" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="77"/>
+    <row r="20" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D20" s="78"/>
       <c r="E20" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="F20" s="12">
+        <v>2890</v>
+      </c>
+      <c r="G20" s="20"/>
+    </row>
+    <row r="21" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D21" s="78"/>
+      <c r="E21" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F21" s="12">
         <v>54100</v>
       </c>
-      <c r="G20" s="20"/>
-    </row>
-    <row r="21" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="77"/>
-      <c r="E21" s="13" t="s">
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="78"/>
+      <c r="E22" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="14">
-        <f>SUM(F9:F20)</f>
-        <v>804695</v>
-      </c>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D22" s="77"/>
-      <c r="E22" s="19" t="s">
+      <c r="F22" s="14">
+        <f>SUM(F9:F21)</f>
+        <v>807585</v>
+      </c>
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D23" s="78"/>
+      <c r="E23" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F22" s="41">
+      <c r="F23" s="41">
         <v>80000</v>
       </c>
-      <c r="G22" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="77"/>
-      <c r="E23" s="19" t="s">
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="78"/>
+      <c r="E24" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F23" s="41">
+      <c r="F24" s="41">
         <v>26500</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G24" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H23" t="s">
+      <c r="H24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D24" s="77"/>
-      <c r="E24" s="19" t="s">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="78"/>
+      <c r="E25" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F25" s="41">
         <v>50000</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D25" s="77"/>
-      <c r="E25" s="19" t="s">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="78"/>
+      <c r="E26" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F26" s="41">
         <v>14000</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G26" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="77"/>
-      <c r="E26" s="19" t="s">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="78"/>
+      <c r="E27" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F27" s="41">
         <v>5000</v>
-      </c>
-      <c r="G26" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="77"/>
-      <c r="E27" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="41">
-        <v>27000</v>
       </c>
       <c r="G27" s="20" t="s">
         <v>35</v>
       </c>
+      <c r="H27" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="28" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D28" s="77"/>
+      <c r="D28" s="78"/>
       <c r="E28" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F28" s="41">
-        <v>50000</v>
+        <v>27000</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H28" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="77"/>
+      <c r="D29" s="78"/>
       <c r="E29" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F29" s="41">
-        <v>11270</v>
+        <v>50000</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>35</v>
       </c>
+      <c r="H29" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D30" s="77"/>
+      <c r="D30" s="78"/>
       <c r="E30" s="19" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F30" s="41">
-        <v>21725</v>
+        <v>11270</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D31" s="77"/>
+      <c r="D31" s="78"/>
       <c r="E31" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F31" s="41">
-        <v>44325</v>
+        <v>21725</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D32" s="77"/>
+      <c r="D32" s="78"/>
       <c r="E32" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F32" s="41">
-        <v>21560</v>
+        <v>44325</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D33" s="77"/>
+      <c r="D33" s="78"/>
       <c r="E33" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F33" s="41">
-        <v>7250</v>
+        <v>21560</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="77"/>
+      <c r="D34" s="78"/>
       <c r="E34" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F34" s="41">
-        <v>18600</v>
+        <v>7250</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H34" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D35" s="77"/>
+      <c r="D35" s="78"/>
       <c r="E35" s="19" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F35" s="41">
-        <v>44325</v>
+        <v>18600</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>35</v>
       </c>
+      <c r="H35" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="77"/>
+      <c r="D36" s="78"/>
       <c r="E36" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F36" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G36" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D37" s="78"/>
+      <c r="E37" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F36" s="41">
+      <c r="F37" s="41">
         <v>1800</v>
       </c>
-      <c r="G36" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D37" s="77"/>
-      <c r="E37" s="19" t="s">
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D38" s="78"/>
+      <c r="E38" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F37" s="41">
+      <c r="F38" s="41">
         <v>1750</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D38" s="77"/>
-      <c r="E38" s="19" t="s">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" s="78"/>
+      <c r="E39" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F39" s="41">
         <v>21300</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D39" s="77"/>
-      <c r="E39" s="19" t="s">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="78"/>
+      <c r="E40" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F39" s="41">
+      <c r="F40" s="41">
         <v>4700</v>
-      </c>
-      <c r="G39" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D40" s="77"/>
-      <c r="E40" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F40" s="41">
-        <v>5590</v>
       </c>
       <c r="G40" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="41" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D41" s="77"/>
+      <c r="D41" s="78"/>
       <c r="E41" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F41" s="41">
-        <v>30000</v>
+        <v>5590</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H41" t="s">
-        <v>123</v>
-      </c>
-      <c r="I41">
-        <v>126500</v>
-      </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D42" s="77"/>
+      <c r="D42" s="78"/>
       <c r="E42" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F42" s="41">
-        <v>3730</v>
+        <v>30000</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>119</v>
       </c>
+      <c r="H42" t="s">
+        <v>123</v>
+      </c>
+      <c r="I42">
+        <v>126500</v>
+      </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D43" s="77"/>
+      <c r="D43" s="78"/>
       <c r="E43" s="19" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F43" s="41">
-        <v>10000</v>
+        <v>3730</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H43" t="s">
-        <v>123</v>
-      </c>
-      <c r="I43">
-        <v>136500</v>
-      </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D44" s="77"/>
+      <c r="D44" s="78"/>
       <c r="E44" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F44" s="41">
-        <v>4200</v>
+        <v>10000</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>119</v>
       </c>
+      <c r="H44" t="s">
+        <v>123</v>
+      </c>
+      <c r="I44">
+        <v>136500</v>
+      </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D45" s="77"/>
+      <c r="D45" s="78"/>
       <c r="E45" s="19" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F45" s="41">
-        <v>35000</v>
+        <v>4200</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D46" s="77"/>
+      <c r="D46" s="78"/>
       <c r="E46" s="19" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="F46" s="41">
-        <v>16000</v>
+        <v>35000</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D47" s="77"/>
+      <c r="D47" s="78"/>
       <c r="E47" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F47" s="41">
-        <v>63500</v>
+        <v>16000</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H47" t="s">
-        <v>123</v>
-      </c>
-      <c r="I47">
-        <v>200000</v>
-      </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D48" s="77"/>
+      <c r="D48" s="78"/>
       <c r="E48" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F48" s="41">
-        <v>11350</v>
+        <v>63500</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>119</v>
       </c>
+      <c r="H48" t="s">
+        <v>123</v>
+      </c>
+      <c r="I48">
+        <v>200000</v>
+      </c>
     </row>
     <row r="49" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D49" s="77"/>
+      <c r="D49" s="78"/>
       <c r="E49" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F49" s="41">
+        <v>11350</v>
+      </c>
+      <c r="G49" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D50" s="78"/>
+      <c r="E50" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="F49" s="41">
+      <c r="F50" s="41">
         <v>14900</v>
       </c>
-      <c r="G49" s="20" t="s">
+      <c r="G50" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D50" s="77"/>
-      <c r="E50" s="19" t="s">
+    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D51" s="78"/>
+      <c r="E51" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="F50" s="41">
+      <c r="F51" s="41">
         <v>20000</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="H50" t="s">
-        <v>181</v>
-      </c>
-      <c r="I50">
-        <v>220000</v>
-      </c>
-    </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D51" s="77"/>
-      <c r="E51" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="F51" s="41">
-        <v>4350</v>
       </c>
       <c r="G51" s="20" t="s">
         <v>119</v>
       </c>
+      <c r="H51" t="s">
+        <v>181</v>
+      </c>
+      <c r="I51">
+        <v>220000</v>
+      </c>
     </row>
     <row r="52" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D52" s="77"/>
+      <c r="D52" s="78"/>
       <c r="E52" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F52" s="41">
-        <v>15000</v>
+        <v>4350</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H52" t="s">
+    </row>
+    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D53" s="78"/>
+      <c r="E53" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F53" s="41">
+        <v>15000</v>
+      </c>
+      <c r="G53" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H53" t="s">
         <v>190</v>
       </c>
-      <c r="I52">
+      <c r="I53">
         <v>50000</v>
       </c>
     </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D53" s="77"/>
-      <c r="E53" s="19" t="s">
+    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D54" s="78"/>
+      <c r="E54" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="F53" s="41"/>
-      <c r="G53" s="20"/>
-    </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D54" s="77"/>
-      <c r="E54" s="19" t="s">
+      <c r="F54" s="41">
+        <v>2890</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="55" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D55" s="78"/>
+      <c r="E55" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="F54" s="41"/>
-      <c r="G54" s="20"/>
-    </row>
-    <row r="55" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D55" s="77"/>
-      <c r="E55" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="F55" s="12">
-        <v>0</v>
+      <c r="F55" s="41">
+        <v>20000</v>
       </c>
       <c r="G55" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="56" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H55" t="s">
+        <v>190</v>
+      </c>
+      <c r="I55">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="56" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D56" s="78"/>
-      <c r="E56" s="1" t="s">
+      <c r="E56" s="19"/>
+      <c r="F56" s="41"/>
+      <c r="G56" s="20"/>
+    </row>
+    <row r="57" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D57" s="78"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="41"/>
+      <c r="G57" s="20"/>
+    </row>
+    <row r="58" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D58" s="78"/>
+      <c r="E58" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F58" s="12">
+        <v>0</v>
+      </c>
+      <c r="G58" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="59" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D59" s="79"/>
+      <c r="E59" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F56" s="14">
-        <f>F21-SUM(F22:F55)</f>
-        <v>119970</v>
-      </c>
-      <c r="G56" s="21"/>
+      <c r="F59" s="14">
+        <f>F22-SUM(F23:F58)</f>
+        <v>99970</v>
+      </c>
+      <c r="G59" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D56"/>
+    <mergeCell ref="D9:D59"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
15-06-2024 - final updates done
</commit_message>
<xml_diff>
--- a/Interior_Work_Excel.xlsx
+++ b/Interior_Work_Excel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/254ab4912ef77ab4/Documents/Interior Estimates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nandi\OneDrive\Documents\Interior Estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="632" documentId="13_ncr:1_{4ADAB29A-E89E-4E75-9491-0D72C9970A30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{797503A0-CBCD-43A8-A5C4-D36010E672DB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C083945-9C26-4972-848B-C488F716A5FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77DD219D-77BC-4CF5-A77A-7FB6EB665E14}"/>
   </bookViews>
@@ -153,6 +153,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{7A3359F2-1885-4595-9EC3-7C907BFD1841}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+gaur da - 3070</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="K28" authorId="0" shapeId="0" xr:uid="{9C9C7CF7-E494-4E99-A1DA-3545AA62EB81}">
       <text>
         <r>
@@ -197,7 +221,9 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-1st - Anam - 20000</t>
+1st - Anam - 20000
+2nd - 10000 Anam and 5000 Bikas Da
+3rd Anam - 13780(last payment)</t>
         </r>
       </text>
     </comment>
@@ -221,7 +247,10 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-1st - Sahid da - 2700</t>
+1st - Sahid da - 2700
+2nd - Jacky - 15000
+3rd Jacky - 5592
+</t>
         </r>
       </text>
     </comment>
@@ -293,7 +322,7 @@
     <author>sounak nandi</author>
   </authors>
   <commentList>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{4C977440-C90C-4E58-8D21-F5C20DA6AE8F}">
       <text>
         <r>
           <rPr>
@@ -830,7 +859,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F24" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{B8164F85-79D1-49E7-909E-C308FA74C92B}">
       <text>
         <r>
           <rPr>
@@ -854,7 +883,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F26" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{6873D63E-E142-46E3-886D-8F04D0808F9B}">
       <text>
         <r>
           <rPr>
@@ -878,7 +907,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{BB637B1C-9811-438F-92D3-3C9C942096C0}">
       <text>
         <r>
           <rPr>
@@ -903,7 +932,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{CC4073CA-B461-425F-8090-FB36D0CB29CF}">
       <text>
         <r>
           <rPr>
@@ -928,7 +957,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{CBE7ACC9-6A74-4824-9505-12B3442BA816}">
       <text>
         <r>
           <rPr>
@@ -953,7 +982,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{A68C8E79-FA79-4ACA-9399-E89B3AD869EC}">
       <text>
         <r>
           <rPr>
@@ -979,7 +1008,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{39947954-F308-41E6-B777-041F6238CC80}">
       <text>
         <r>
           <rPr>
@@ -1003,7 +1032,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{B0CA3A92-AB89-47A4-99E0-237B4DD818B4}">
       <text>
         <r>
           <rPr>
@@ -1027,7 +1056,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{261FBC28-851A-412F-9C4F-689AD1502034}">
       <text>
         <r>
           <rPr>
@@ -1051,7 +1080,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{EBD5186D-48B7-4D6E-B69C-93B2CE3A80DB}">
       <text>
         <r>
           <rPr>
@@ -1075,7 +1104,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{783EB1C2-146B-4AA7-AB0F-E24CF3E9CF53}">
       <text>
         <r>
           <rPr>
@@ -1099,7 +1128,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H35" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
+    <comment ref="H36" authorId="0" shapeId="0" xr:uid="{B169B1A7-7186-46C8-B3CE-5F98BB7CC85E}">
       <text>
         <r>
           <rPr>
@@ -1123,7 +1152,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
+    <comment ref="F37" authorId="1" shapeId="0" xr:uid="{EEBC63E1-B1B1-4163-BC6A-2598BEE2FDE5}">
       <text>
         <r>
           <rPr>
@@ -1147,7 +1176,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
+    <comment ref="F38" authorId="1" shapeId="0" xr:uid="{830C97D3-129A-4112-AE3F-4CE6F1407A92}">
       <text>
         <r>
           <rPr>
@@ -1171,7 +1200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
+    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{90974AF0-BD89-496C-A4AA-4C5538B8932E}">
       <text>
         <r>
           <rPr>
@@ -1196,7 +1225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F39" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{4D7215A4-3DA7-47A3-9A9A-1AEFBC6EA74F}">
       <text>
         <r>
           <rPr>
@@ -1223,7 +1252,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{326D9884-D005-4087-87B9-1C28D8A1699C}">
       <text>
         <r>
           <rPr>
@@ -1247,7 +1276,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
+    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{11A19A1E-F9B3-43ED-AD45-9773145CE4EA}">
       <text>
         <r>
           <rPr>
@@ -1271,7 +1300,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F42" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
+    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{67760B29-7AB2-4ABD-A72F-A650C1265A6A}">
       <text>
         <r>
           <rPr>
@@ -1295,7 +1324,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I42" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
+    <comment ref="I43" authorId="0" shapeId="0" xr:uid="{AFF71694-EFEC-4A6B-8CD6-6BA33938EBC2}">
       <text>
         <r>
           <rPr>
@@ -1319,7 +1348,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F43" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
+    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{EA8726D9-83FA-4872-8EFD-DD8791485B9C}">
       <text>
         <r>
           <rPr>
@@ -1343,7 +1372,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F44" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
+    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{018B0028-D9A0-4C48-B737-C43986DD3129}">
       <text>
         <r>
           <rPr>
@@ -1367,7 +1396,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I44" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
+    <comment ref="I45" authorId="0" shapeId="0" xr:uid="{938B11E1-E912-497D-B438-FEF8DD9A77AF}">
       <text>
         <r>
           <rPr>
@@ -1391,7 +1420,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F45" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
+    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{931131A1-B186-4CDA-82BD-A601849AD702}">
       <text>
         <r>
           <rPr>
@@ -1415,7 +1444,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F46" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
+    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{A251FCF5-E99D-4AEC-A49C-6C6EB8824556}">
       <text>
         <r>
           <rPr>
@@ -1439,7 +1468,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F47" authorId="0" shapeId="0" xr:uid="{9801DA58-C7B4-4364-9205-58707072E88C}">
+    <comment ref="F48" authorId="0" shapeId="0" xr:uid="{9801DA58-C7B4-4364-9205-58707072E88C}">
       <text>
         <r>
           <rPr>
@@ -1463,7 +1492,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F48" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
+    <comment ref="F49" authorId="0" shapeId="0" xr:uid="{6D32CCE3-A027-43DB-B9AA-41F63362A8AD}">
       <text>
         <r>
           <rPr>
@@ -1487,7 +1516,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I48" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
+    <comment ref="I49" authorId="0" shapeId="0" xr:uid="{0D464CDB-1659-4304-A728-55D7494D0A59}">
       <text>
         <r>
           <rPr>
@@ -1511,7 +1540,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F49" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
+    <comment ref="F50" authorId="0" shapeId="0" xr:uid="{CCBD9164-4418-4A4B-9F2C-B1F7C04FE3A7}">
       <text>
         <r>
           <rPr>
@@ -1535,7 +1564,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F50" authorId="0" shapeId="0" xr:uid="{7209404C-B1DE-4988-B78E-695821C66020}">
+    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{7209404C-B1DE-4988-B78E-695821C66020}">
       <text>
         <r>
           <rPr>
@@ -1559,7 +1588,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F51" authorId="0" shapeId="0" xr:uid="{8CD9AA95-66D8-47E8-97CA-B73A6D47FABD}">
+    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{8CD9AA95-66D8-47E8-97CA-B73A6D47FABD}">
       <text>
         <r>
           <rPr>
@@ -1583,7 +1612,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F52" authorId="0" shapeId="0" xr:uid="{1CA1BF83-085B-4EEF-9FAE-03AB18F5FC7C}">
+    <comment ref="F53" authorId="0" shapeId="0" xr:uid="{1CA1BF83-085B-4EEF-9FAE-03AB18F5FC7C}">
       <text>
         <r>
           <rPr>
@@ -1607,7 +1636,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F53" authorId="0" shapeId="0" xr:uid="{843F7684-8F79-464D-8D4F-0683C00C0A13}">
+    <comment ref="F54" authorId="0" shapeId="0" xr:uid="{843F7684-8F79-464D-8D4F-0683C00C0A13}">
       <text>
         <r>
           <rPr>
@@ -1632,7 +1661,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F55" authorId="0" shapeId="0" xr:uid="{36363EF2-6EAC-4355-AEC8-861A67E5E666}">
+    <comment ref="F56" authorId="0" shapeId="0" xr:uid="{36363EF2-6EAC-4355-AEC8-861A67E5E666}">
       <text>
         <r>
           <rPr>
@@ -1653,6 +1682,127 @@
           </rPr>
           <t xml:space="preserve">
 Anam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F57" authorId="0" shapeId="0" xr:uid="{854E33E1-B48B-4E68-855D-B4133D5929CE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F58" authorId="0" shapeId="0" xr:uid="{A2F0D07D-635E-4FB2-A023-0C71F26CFC7F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Anam</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F60" authorId="0" shapeId="0" xr:uid="{58C6029F-973B-43B1-8AEF-56F0B806C866}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bathroom Magnet, door stopper, Glass for furniture
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F61" authorId="0" shapeId="0" xr:uid="{5CFB1A10-4981-4FE1-BDE6-AFD2ABBFDD37}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F62" authorId="0" shapeId="0" xr:uid="{E50C6E48-2FBB-465F-AB0E-8557AF48B415}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Bikas da</t>
         </r>
       </text>
     </comment>
@@ -2268,7 +2418,7 @@
             <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Sandeep da last one
+Sandeep da last one - paid to jacky
 </t>
         </r>
       </text>
@@ -2318,6 +2468,30 @@
           </rPr>
           <t xml:space="preserve">
 Sahid da</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F41" authorId="0" shapeId="0" xr:uid="{21CC6AAF-0E8E-4DFE-9810-3991493CA2E5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>sounak nandi:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Jacky</t>
         </r>
       </text>
     </comment>
@@ -2326,7 +2500,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="219">
   <si>
     <t>Provider</t>
   </si>
@@ -2941,6 +3115,49 @@
   </si>
   <si>
     <t>Electrical Additional (Last buys)</t>
+  </si>
+  <si>
+    <t>Baba-Extra(20000) &amp; Bank(5000)</t>
+  </si>
+  <si>
+    <t>Extra ceiling</t>
+  </si>
+  <si>
+    <t>Baba</t>
+  </si>
+  <si>
+    <t>Payment - 36</t>
+  </si>
+  <si>
+    <t>Payment - 37</t>
+  </si>
+  <si>
+    <t>Self - 11070
+Bank - 5592</t>
+  </si>
+  <si>
+    <t>Bathroom Magnet, Door stopper, Glass work</t>
+  </si>
+  <si>
+    <t>Payment - 38</t>
+  </si>
+  <si>
+    <t>Payment - 39</t>
+  </si>
+  <si>
+    <t>Self-No Receipt</t>
+  </si>
+  <si>
+    <t>Payment - 40</t>
+  </si>
+  <si>
+    <t>Payment - 41</t>
+  </si>
+  <si>
+    <t>Payment - 42</t>
+  </si>
+  <si>
+    <t>Payment - 43</t>
   </si>
 </sst>
 </file>
@@ -3448,7 +3665,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -3564,6 +3781,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3648,6 +3868,22 @@
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
+<file path=xl/persons/person100.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person101.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person102.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person103.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/persons/person11.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -4005,6 +4241,34 @@
 </file>
 
 <file path=xl/persons/person92.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person93.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person94.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person95.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person96.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person97.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person98.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/persons/person99.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
@@ -4307,8 +4571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C736B24-9BE5-46F3-B4DC-24087C579173}">
   <dimension ref="C7:Q28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C8" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="C6" zoomScale="80" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4385,11 +4649,11 @@
       </c>
       <c r="F10">
         <f>Paint!F10</f>
-        <v>75000</v>
+        <v>70000</v>
       </c>
       <c r="G10">
-        <f>SUM(Paint!F11:F20)</f>
-        <v>66930</v>
+        <f>SUM(Paint!F11:F21)</f>
+        <v>70000</v>
       </c>
       <c r="H10">
         <v>9283</v>
@@ -4399,11 +4663,11 @@
       </c>
       <c r="J10">
         <f>SUM(H25:H28)</f>
-        <v>33717</v>
+        <v>36787</v>
       </c>
       <c r="K10" s="4">
         <f t="shared" si="0"/>
-        <v>8070</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.3">
@@ -4414,26 +4678,26 @@
         <v>14</v>
       </c>
       <c r="F11">
-        <f>'False Ceiling'!F12</f>
-        <v>131550</v>
+        <f>'False Ceiling'!F13</f>
+        <v>139550</v>
       </c>
       <c r="G11">
-        <f>SUM('False Ceiling'!F13:F19)</f>
-        <v>128750</v>
+        <f>SUM('False Ceiling'!F14:F22)</f>
+        <v>139550</v>
       </c>
       <c r="H11">
-        <v>4000</v>
+        <v>10000</v>
       </c>
       <c r="I11">
         <v>4750</v>
       </c>
       <c r="J11">
         <f>SUM(J25:J28)</f>
-        <v>120000</v>
+        <v>124800</v>
       </c>
       <c r="K11" s="4">
         <f t="shared" si="0"/>
-        <v>2800</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.3">
@@ -4479,10 +4743,10 @@
       </c>
       <c r="G13">
         <f>SUM(Grill!F16:F22)</f>
-        <v>99000</v>
+        <v>109000</v>
       </c>
       <c r="H13">
-        <v>36300</v>
+        <v>46300</v>
       </c>
       <c r="I13">
         <v>10000</v>
@@ -4493,7 +4757,7 @@
       </c>
       <c r="K13" s="4">
         <f t="shared" si="0"/>
-        <v>10000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.3">
@@ -4504,26 +4768,26 @@
         <v>26</v>
       </c>
       <c r="F14">
-        <f>Furniture!F22</f>
-        <v>807585</v>
+        <f>Furniture!F23</f>
+        <v>807615</v>
       </c>
       <c r="G14">
-        <f>SUM(Furniture!F23:F58)</f>
-        <v>707615</v>
+        <f>SUM(Furniture!F24:F65)</f>
+        <v>807615</v>
       </c>
       <c r="H14">
-        <v>63840</v>
+        <v>110090</v>
       </c>
       <c r="I14">
         <v>228720</v>
       </c>
       <c r="J14">
         <f>SUM(M25:M28)</f>
-        <v>415055</v>
+        <v>443835</v>
       </c>
       <c r="K14" s="4">
         <f t="shared" si="0"/>
-        <v>99970</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.3">
@@ -4535,25 +4799,25 @@
       </c>
       <c r="F15">
         <f>'Bathroom-Kitchen-Barandah'!F22</f>
-        <v>345150</v>
+        <v>356250</v>
       </c>
       <c r="G15">
-        <f>SUM('Bathroom-Kitchen-Barandah'!F23:F42)</f>
-        <v>324588</v>
+        <f>SUM('Bathroom-Kitchen-Barandah'!F23:F43)</f>
+        <v>356250</v>
       </c>
       <c r="H15">
-        <v>129000</v>
+        <v>165040</v>
       </c>
       <c r="I15">
         <v>92988</v>
       </c>
       <c r="J15">
         <f>SUM(N25:N28)</f>
-        <v>102600</v>
+        <v>123192</v>
       </c>
       <c r="K15" s="4">
         <f t="shared" si="0"/>
-        <v>20562</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="4:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -4593,15 +4857,15 @@
       </c>
       <c r="F17" s="2">
         <f>SUM(F9:F16)</f>
-        <v>2007933</v>
+        <v>2022063</v>
       </c>
       <c r="G17" s="2">
         <f>SUM(G9:G16)</f>
-        <v>1866531</v>
+        <v>2022063</v>
       </c>
       <c r="H17" s="2">
         <f>SUM(H9:H16)</f>
-        <v>321458</v>
+        <v>419748</v>
       </c>
       <c r="I17" s="2">
         <f>SUM(I9:I16)</f>
@@ -4609,11 +4873,11 @@
       </c>
       <c r="J17" s="2">
         <f>SUM(J9:J16)</f>
-        <v>1155700</v>
+        <v>1212942</v>
       </c>
       <c r="K17" s="3">
         <f t="shared" si="0"/>
-        <v>141402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:17" x14ac:dyDescent="0.3">
@@ -4630,7 +4894,7 @@
       </c>
       <c r="F19" s="28">
         <f>SUM(H17,I17)</f>
-        <v>710831</v>
+        <v>809121</v>
       </c>
     </row>
     <row r="20" spans="3:17" x14ac:dyDescent="0.3">
@@ -4639,11 +4903,11 @@
       </c>
       <c r="F20" s="28">
         <f>F17-SUM(F18:F19)</f>
-        <v>84102</v>
+        <v>-58</v>
       </c>
       <c r="G20" s="61">
         <f>F20-SUM('Extra Source'!G68,'Extra Source'!G55)</f>
-        <v>73032</v>
+        <v>-58</v>
       </c>
       <c r="H20" s="28" t="s">
         <v>189</v>
@@ -4655,7 +4919,7 @@
       </c>
       <c r="F21" s="28">
         <f>K17</f>
-        <v>141402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="3:17" x14ac:dyDescent="0.3">
@@ -4664,27 +4928,27 @@
       </c>
       <c r="F22" s="28">
         <f>F21-F20</f>
-        <v>57300</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="3:17" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="63" t="s">
+      <c r="C23" s="64" t="s">
         <v>44</v>
       </c>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
-      <c r="J23" s="63"/>
-      <c r="K23" s="63"/>
-      <c r="L23" s="63"/>
-      <c r="M23" s="63"/>
-      <c r="N23" s="63"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="63"/>
-      <c r="Q23" s="63"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="64"/>
+      <c r="F23" s="64"/>
+      <c r="G23" s="64"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="64"/>
+      <c r="J23" s="64"/>
+      <c r="K23" s="64"/>
+      <c r="L23" s="64"/>
+      <c r="M23" s="64"/>
+      <c r="N23" s="64"/>
+      <c r="O23" s="64"/>
+      <c r="P23" s="64"/>
+      <c r="Q23" s="64"/>
     </row>
     <row r="24" spans="3:17" x14ac:dyDescent="0.3">
       <c r="C24" s="33" t="s">
@@ -4877,10 +5141,12 @@
         <v>45322</v>
       </c>
       <c r="G28" s="28"/>
-      <c r="H28" s="40"/>
+      <c r="H28" s="40">
+        <v>3070</v>
+      </c>
       <c r="I28" s="40"/>
       <c r="J28" s="40">
-        <v>0</v>
+        <v>4800</v>
       </c>
       <c r="K28" s="40">
         <v>3000</v>
@@ -4889,19 +5155,19 @@
         <v>0</v>
       </c>
       <c r="M28" s="40">
-        <v>20000</v>
+        <v>48780</v>
       </c>
       <c r="N28" s="40">
-        <v>2700</v>
+        <v>23292</v>
       </c>
       <c r="O28" s="28"/>
       <c r="P28" s="28">
         <f>SUM(G28:O28)</f>
-        <v>25700</v>
+        <v>82942</v>
       </c>
       <c r="Q28" s="28">
         <f>SUM(E28,D28)-P28</f>
-        <v>57300</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -4915,10 +5181,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD019853-AAD7-4C4A-AE9D-387A8C77D1D3}">
-  <dimension ref="D7:N43"/>
+  <dimension ref="D7:N44"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40:E42"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="I38" activeCellId="1" sqref="M38 I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4946,19 +5212,19 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="72" t="s">
         <v>60</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>41</v>
       </c>
       <c r="F9" s="10">
-        <v>121000</v>
+        <v>132100</v>
       </c>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="11" t="s">
         <v>23</v>
       </c>
@@ -4968,7 +5234,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="11" t="s">
         <v>65</v>
       </c>
@@ -4978,7 +5244,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="72"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="11" t="s">
         <v>78</v>
       </c>
@@ -4988,7 +5254,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="11" t="s">
         <v>79</v>
       </c>
@@ -4998,7 +5264,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="72"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="11" t="s">
         <v>81</v>
       </c>
@@ -5008,7 +5274,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="11" t="s">
         <v>80</v>
       </c>
@@ -5018,7 +5284,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="72"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="11" t="s">
         <v>133</v>
       </c>
@@ -5028,7 +5294,7 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D17" s="72"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="11" t="s">
         <v>135</v>
       </c>
@@ -5038,7 +5304,7 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D18" s="72"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="11" t="s">
         <v>148</v>
       </c>
@@ -5048,7 +5314,7 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D19" s="72"/>
+      <c r="D19" s="73"/>
       <c r="E19" s="11" t="s">
         <v>203</v>
       </c>
@@ -5058,7 +5324,7 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D20" s="72"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="11" t="s">
         <v>136</v>
       </c>
@@ -5068,7 +5334,7 @@
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="72"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="11" t="s">
         <v>19</v>
       </c>
@@ -5078,18 +5344,18 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="72"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F22" s="14">
         <f>SUM(F9:F21)</f>
-        <v>345150</v>
+        <v>356250</v>
       </c>
       <c r="G22" s="20"/>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D23" s="72"/>
+      <c r="D23" s="73"/>
       <c r="E23" s="11" t="s">
         <v>31</v>
       </c>
@@ -5101,7 +5367,7 @@
       </c>
     </row>
     <row r="24" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D24" s="72"/>
+      <c r="D24" s="73"/>
       <c r="E24" s="11" t="s">
         <v>33</v>
       </c>
@@ -5113,7 +5379,7 @@
       </c>
     </row>
     <row r="25" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D25" s="72"/>
+      <c r="D25" s="73"/>
       <c r="E25" s="11" t="s">
         <v>32</v>
       </c>
@@ -5125,7 +5391,7 @@
       </c>
     </row>
     <row r="26" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D26" s="72"/>
+      <c r="D26" s="73"/>
       <c r="E26" s="11" t="s">
         <v>34</v>
       </c>
@@ -5137,7 +5403,7 @@
       </c>
     </row>
     <row r="27" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D27" s="72"/>
+      <c r="D27" s="73"/>
       <c r="E27" s="11" t="s">
         <v>67</v>
       </c>
@@ -5149,7 +5415,7 @@
       </c>
     </row>
     <row r="28" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D28" s="72"/>
+      <c r="D28" s="73"/>
       <c r="E28" s="11" t="s">
         <v>68</v>
       </c>
@@ -5161,7 +5427,7 @@
       </c>
     </row>
     <row r="29" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D29" s="72"/>
+      <c r="D29" s="73"/>
       <c r="E29" s="11" t="s">
         <v>74</v>
       </c>
@@ -5173,7 +5439,7 @@
       </c>
     </row>
     <row r="30" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D30" s="72"/>
+      <c r="D30" s="73"/>
       <c r="E30" s="11" t="s">
         <v>76</v>
       </c>
@@ -5191,7 +5457,7 @@
       </c>
     </row>
     <row r="31" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D31" s="72"/>
+      <c r="D31" s="73"/>
       <c r="E31" s="11" t="s">
         <v>77</v>
       </c>
@@ -5203,7 +5469,7 @@
       </c>
     </row>
     <row r="32" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D32" s="72"/>
+      <c r="D32" s="73"/>
       <c r="E32" s="11" t="s">
         <v>93</v>
       </c>
@@ -5215,7 +5481,7 @@
       </c>
     </row>
     <row r="33" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D33" s="72"/>
+      <c r="D33" s="73"/>
       <c r="E33" s="11" t="s">
         <v>94</v>
       </c>
@@ -5227,7 +5493,7 @@
       </c>
     </row>
     <row r="34" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D34" s="72"/>
+      <c r="D34" s="73"/>
       <c r="E34" s="11" t="s">
         <v>95</v>
       </c>
@@ -5239,7 +5505,7 @@
       </c>
     </row>
     <row r="35" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D35" s="72"/>
+      <c r="D35" s="73"/>
       <c r="E35" s="11" t="s">
         <v>96</v>
       </c>
@@ -5251,7 +5517,7 @@
       </c>
     </row>
     <row r="36" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D36" s="72"/>
+      <c r="D36" s="73"/>
       <c r="E36" s="11" t="s">
         <v>97</v>
       </c>
@@ -5263,7 +5529,7 @@
       </c>
     </row>
     <row r="37" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D37" s="72"/>
+      <c r="D37" s="73"/>
       <c r="E37" s="11" t="s">
         <v>105</v>
       </c>
@@ -5281,7 +5547,7 @@
       </c>
     </row>
     <row r="38" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D38" s="72"/>
+      <c r="D38" s="73"/>
       <c r="E38" s="11" t="s">
         <v>106</v>
       </c>
@@ -5299,7 +5565,7 @@
       </c>
       <c r="J38">
         <f>F9-I38</f>
-        <v>20562</v>
+        <v>31662</v>
       </c>
       <c r="L38" s="62" t="s">
         <v>190</v>
@@ -5313,7 +5579,7 @@
       </c>
     </row>
     <row r="39" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D39" s="72"/>
+      <c r="D39" s="73"/>
       <c r="E39" s="11" t="s">
         <v>107</v>
       </c>
@@ -5331,7 +5597,7 @@
       </c>
     </row>
     <row r="40" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D40" s="72"/>
+      <c r="D40" s="73"/>
       <c r="E40" s="11" t="s">
         <v>108</v>
       </c>
@@ -5343,35 +5609,61 @@
       </c>
     </row>
     <row r="41" spans="4:14" x14ac:dyDescent="0.3">
-      <c r="D41" s="72"/>
+      <c r="D41" s="73"/>
       <c r="E41" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="F41" s="41"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D42" s="72"/>
+      <c r="F41" s="41">
+        <v>15000</v>
+      </c>
+      <c r="G41" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" t="s">
+        <v>186</v>
+      </c>
+      <c r="I41">
+        <v>115438</v>
+      </c>
+      <c r="J41">
+        <f>F9-I41</f>
+        <v>16662</v>
+      </c>
+    </row>
+    <row r="42" spans="4:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D42" s="73"/>
       <c r="E42" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="F42" s="12"/>
-      <c r="G42" s="20"/>
+      <c r="F42" s="41">
+        <v>16662</v>
+      </c>
+      <c r="G42" s="63" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="43" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D43" s="73"/>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="F43" s="12"/>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="4:14" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D44" s="74"/>
+      <c r="E44" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="14">
-        <f>F22-SUM(F23:F42)</f>
-        <v>20562</v>
-      </c>
-      <c r="G43" s="21"/>
+      <c r="F44" s="14">
+        <f>F22-SUM(F23:F43)</f>
+        <v>0</v>
+      </c>
+      <c r="G44" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D43"/>
+    <mergeCell ref="D9:D44"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5381,10 +5673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F170B8EE-4C33-4613-A889-5080BF8B5D70}">
-  <dimension ref="D6:I80"/>
+  <dimension ref="D6:I82"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="G68" sqref="G68"/>
+    <sheetView topLeftCell="A22" zoomScale="72" workbookViewId="0">
+      <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5396,18 +5688,18 @@
   <sheetData>
     <row r="6" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D7" s="68" t="s">
+      <c r="D7" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="70"/>
+      <c r="E7" s="70"/>
+      <c r="F7" s="70"/>
+      <c r="G7" s="71"/>
     </row>
     <row r="8" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D8" s="64" t="s">
+      <c r="D8" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="66">
+      <c r="E8" s="67">
         <v>45000</v>
       </c>
       <c r="F8" s="48" t="s">
@@ -5418,8 +5710,8 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="65"/>
-      <c r="E9" s="67"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="68"/>
       <c r="F9" s="28" t="s">
         <v>16</v>
       </c>
@@ -5428,8 +5720,8 @@
       </c>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="65"/>
-      <c r="E10" s="67"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="47" t="s">
         <v>55</v>
       </c>
@@ -5882,7 +6174,7 @@
       </c>
       <c r="I62">
         <f>SUM(G62:G67)</f>
-        <v>68930</v>
+        <v>80000</v>
       </c>
     </row>
     <row r="63" spans="4:9" x14ac:dyDescent="0.3">
@@ -5907,7 +6199,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="65" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F65" t="s">
         <v>194</v>
       </c>
@@ -5918,7 +6210,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F66" t="s">
         <v>195</v>
       </c>
@@ -5929,19 +6221,65 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="6:8" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>186</v>
+      </c>
+      <c r="G67">
+        <v>11070</v>
+      </c>
+      <c r="H67" s="59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="68" spans="4:9" x14ac:dyDescent="0.3">
       <c r="F68" t="s">
         <v>10</v>
       </c>
       <c r="G68">
         <f>E61-I62</f>
-        <v>11070</v>
-      </c>
-    </row>
-    <row r="80" spans="6:8" x14ac:dyDescent="0.3">
-      <c r="G80">
-        <f>E61-SUM(G62:G79)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="74" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D74" s="56" t="s">
+        <v>207</v>
+      </c>
+      <c r="E74" s="57">
+        <v>80000</v>
+      </c>
+      <c r="F74" s="57"/>
+      <c r="G74" s="57"/>
+      <c r="H74" s="57" t="s">
+        <v>127</v>
+      </c>
+      <c r="I74" s="58" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="75" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="F75" s="29" t="s">
+        <v>123</v>
+      </c>
+      <c r="G75" s="29">
+        <v>20000</v>
+      </c>
+      <c r="H75" s="29" t="s">
+        <v>26</v>
+      </c>
+      <c r="I75">
+        <f>SUM(G75:G81)</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="82" spans="6:7" x14ac:dyDescent="0.3">
+      <c r="F82" t="s">
+        <v>10</v>
+      </c>
+      <c r="G82">
+        <f>E74-I75</f>
+        <v>60000</v>
       </c>
     </row>
   </sheetData>
@@ -5959,7 +6297,7 @@
   <dimension ref="D7:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5987,7 +6325,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="72" t="s">
         <v>2</v>
       </c>
       <c r="E9" t="s">
@@ -5999,7 +6337,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" t="s">
         <v>4</v>
       </c>
@@ -6009,7 +6347,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="1" t="s">
         <v>6</v>
       </c>
@@ -6020,7 +6358,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="72"/>
+      <c r="D12" s="73"/>
       <c r="E12" t="s">
         <v>7</v>
       </c>
@@ -6032,7 +6370,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" t="s">
         <v>8</v>
       </c>
@@ -6044,7 +6382,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="72"/>
+      <c r="D14" s="73"/>
       <c r="E14" t="s">
         <v>9</v>
       </c>
@@ -6056,7 +6394,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="73"/>
+      <c r="D15" s="74"/>
       <c r="E15" s="1" t="s">
         <v>10</v>
       </c>
@@ -6077,10 +6415,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5512692-EDEE-4A22-9F00-43BA354170EF}">
-  <dimension ref="D7:G21"/>
+  <dimension ref="D7:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6107,30 +6445,30 @@
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="72" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="10">
-        <v>75000</v>
+        <v>70000</v>
       </c>
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="13" t="s">
         <v>6</v>
       </c>
       <c r="F10" s="14">
         <f>F9</f>
-        <v>75000</v>
+        <v>70000</v>
       </c>
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="11" t="s">
         <v>31</v>
       </c>
@@ -6142,7 +6480,7 @@
       </c>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="72"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="11" t="s">
         <v>30</v>
       </c>
@@ -6154,7 +6492,7 @@
       </c>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="11" t="s">
         <v>98</v>
       </c>
@@ -6166,7 +6504,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="72"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="11" t="s">
         <v>99</v>
       </c>
@@ -6178,7 +6516,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="11" t="s">
         <v>100</v>
       </c>
@@ -6190,7 +6528,7 @@
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="72"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="11" t="s">
         <v>121</v>
       </c>
@@ -6202,7 +6540,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="72"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="11" t="s">
         <v>122</v>
       </c>
@@ -6214,7 +6552,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="72"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="11" t="s">
         <v>174</v>
       </c>
@@ -6226,7 +6564,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="72"/>
+      <c r="D19" s="73"/>
       <c r="E19" s="11" t="s">
         <v>175</v>
       </c>
@@ -6237,13 +6575,11 @@
         <v>119</v>
       </c>
     </row>
-    <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="72"/>
-      <c r="E20" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="F20" s="12">
-        <v>0</v>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="73"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="41">
+        <v>3070</v>
       </c>
       <c r="G20" s="20" t="s">
         <v>35</v>
@@ -6251,18 +6587,30 @@
     </row>
     <row r="21" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D21" s="73"/>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="F21" s="12">
+        <v>0</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="74"/>
+      <c r="E22" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F21" s="14">
-        <f>F10-SUM(F11:F20)</f>
-        <v>8070</v>
-      </c>
-      <c r="G21" s="21"/>
+      <c r="F22" s="14">
+        <f>F10-SUM(F11:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="G22" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D21"/>
+    <mergeCell ref="D9:D22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6272,10 +6620,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB69F67B-3322-470C-8A9C-70E95A023898}">
-  <dimension ref="D7:G20"/>
+  <dimension ref="D7:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6302,7 +6650,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="72" t="s">
         <v>15</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -6314,7 +6662,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="9" t="s">
         <v>196</v>
       </c>
@@ -6324,120 +6672,158 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="9" t="s">
+        <v>206</v>
+      </c>
+      <c r="F11" s="10">
+        <v>8000</v>
+      </c>
+      <c r="G11" s="20"/>
+    </row>
+    <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D12" s="73"/>
+      <c r="E12" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="F11" s="10">
+      <c r="F12" s="10">
         <v>2000</v>
       </c>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="72"/>
-      <c r="E12" s="13" t="s">
+      <c r="G12" s="20"/>
+    </row>
+    <row r="13" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D13" s="73"/>
+      <c r="E13" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="14">
-        <f>SUM(F9:F11)</f>
-        <v>131550</v>
-      </c>
-      <c r="G12" s="20"/>
-    </row>
-    <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
-      <c r="E13" s="11" t="s">
+      <c r="F13" s="14">
+        <f>SUM(F9:F12)</f>
+        <v>139550</v>
+      </c>
+      <c r="G13" s="20"/>
+    </row>
+    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D14" s="73"/>
+      <c r="E14" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F14" s="42">
         <v>50000</v>
-      </c>
-      <c r="G13" s="20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="72"/>
-      <c r="E14" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="F14" s="42">
-        <v>40000</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="11" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F15" s="42">
-        <v>30000</v>
+        <v>40000</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="72"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F16" s="42">
+        <v>30000</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D17" s="73"/>
+      <c r="E17" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="42">
+      <c r="F17" s="42">
         <v>4750</v>
       </c>
-      <c r="G16" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="72"/>
-      <c r="E17" s="11" t="s">
+    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D18" s="73"/>
+      <c r="E18" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="42">
+      <c r="F18" s="42">
         <v>1800</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="72"/>
-      <c r="E18" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="42">
-        <v>2200</v>
       </c>
       <c r="G18" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D19" s="72"/>
+    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D19" s="73"/>
       <c r="E19" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F19" s="42">
+        <v>2200</v>
+      </c>
+      <c r="G19" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D20" s="73"/>
+      <c r="E20" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="42"/>
-      <c r="G19" s="20"/>
-    </row>
-    <row r="20" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D20" s="73"/>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="42">
+        <v>4800</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="D21" s="73"/>
+      <c r="E21" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="42">
+        <v>4000</v>
+      </c>
+      <c r="G21" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="73"/>
+      <c r="E22" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="42">
+        <v>2000</v>
+      </c>
+      <c r="G22" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="74"/>
+      <c r="E23" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="14">
-        <f>F12-SUM(F13:F19)</f>
-        <v>2800</v>
-      </c>
-      <c r="G20" s="21"/>
+      <c r="F23" s="14">
+        <f>F13-SUM(F14:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D20"/>
+    <mergeCell ref="D9:D23"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6449,8 +6835,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D1544B4-216C-4DA0-B248-9403EAEF3872}">
   <dimension ref="D7:G54"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6477,7 +6863,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="74" t="s">
+      <c r="D9" s="75" t="s">
         <v>159</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -6489,7 +6875,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="75"/>
+      <c r="D10" s="76"/>
       <c r="E10" s="11" t="s">
         <v>141</v>
       </c>
@@ -6499,7 +6885,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="75"/>
+      <c r="D11" s="76"/>
       <c r="E11" t="s">
         <v>72</v>
       </c>
@@ -6509,7 +6895,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="75"/>
+      <c r="D12" s="76"/>
       <c r="E12" t="s">
         <v>101</v>
       </c>
@@ -6519,7 +6905,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="75"/>
+      <c r="D13" s="76"/>
       <c r="E13" t="s">
         <v>142</v>
       </c>
@@ -6529,7 +6915,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="75"/>
+      <c r="D14" s="76"/>
       <c r="E14" t="s">
         <v>73</v>
       </c>
@@ -6539,7 +6925,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="75"/>
+      <c r="D15" s="76"/>
       <c r="E15" t="s">
         <v>84</v>
       </c>
@@ -6549,7 +6935,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="75"/>
+      <c r="D16" s="76"/>
       <c r="E16" t="s">
         <v>83</v>
       </c>
@@ -6559,7 +6945,7 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="75"/>
+      <c r="D17" s="76"/>
       <c r="E17" t="s">
         <v>143</v>
       </c>
@@ -6569,7 +6955,7 @@
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="75"/>
+      <c r="D18" s="76"/>
       <c r="E18" t="s">
         <v>144</v>
       </c>
@@ -6579,7 +6965,7 @@
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="75"/>
+      <c r="D19" s="76"/>
       <c r="E19" t="s">
         <v>85</v>
       </c>
@@ -6589,7 +6975,7 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="75"/>
+      <c r="D20" s="76"/>
       <c r="E20" t="s">
         <v>145</v>
       </c>
@@ -6599,7 +6985,7 @@
       <c r="G20" s="20"/>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="75"/>
+      <c r="D21" s="76"/>
       <c r="E21" t="s">
         <v>89</v>
       </c>
@@ -6607,7 +6993,7 @@
       <c r="G21" s="20"/>
     </row>
     <row r="22" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D22" s="75"/>
+      <c r="D22" s="76"/>
       <c r="E22" t="s">
         <v>87</v>
       </c>
@@ -6617,7 +7003,7 @@
       <c r="G22" s="20"/>
     </row>
     <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="75"/>
+      <c r="D23" s="76"/>
       <c r="E23" t="s">
         <v>155</v>
       </c>
@@ -6627,7 +7013,7 @@
       <c r="G23" s="20"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D24" s="75"/>
+      <c r="D24" s="76"/>
       <c r="E24" t="s">
         <v>86</v>
       </c>
@@ -6637,7 +7023,7 @@
       <c r="G24" s="20"/>
     </row>
     <row r="25" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D25" s="75"/>
+      <c r="D25" s="76"/>
       <c r="E25" t="s">
         <v>146</v>
       </c>
@@ -6647,7 +7033,7 @@
       <c r="G25" s="20"/>
     </row>
     <row r="26" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D26" s="75"/>
+      <c r="D26" s="76"/>
       <c r="E26" t="s">
         <v>147</v>
       </c>
@@ -6657,7 +7043,7 @@
       <c r="G26" s="20"/>
     </row>
     <row r="27" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D27" s="75"/>
+      <c r="D27" s="76"/>
       <c r="E27" t="s">
         <v>69</v>
       </c>
@@ -6667,7 +7053,7 @@
       <c r="G27" s="20"/>
     </row>
     <row r="28" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D28" s="75"/>
+      <c r="D28" s="76"/>
       <c r="E28" t="s">
         <v>70</v>
       </c>
@@ -6677,7 +7063,7 @@
       <c r="G28" s="20"/>
     </row>
     <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="75"/>
+      <c r="D29" s="76"/>
       <c r="E29" t="s">
         <v>29</v>
       </c>
@@ -6687,7 +7073,7 @@
       <c r="G29" s="20"/>
     </row>
     <row r="30" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D30" s="75"/>
+      <c r="D30" s="76"/>
       <c r="E30" t="s">
         <v>170</v>
       </c>
@@ -6697,7 +7083,7 @@
       <c r="G30" s="20"/>
     </row>
     <row r="31" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D31" s="75"/>
+      <c r="D31" s="76"/>
       <c r="E31" t="s">
         <v>171</v>
       </c>
@@ -6707,7 +7093,7 @@
       <c r="G31" s="20"/>
     </row>
     <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="75"/>
+      <c r="D32" s="76"/>
       <c r="E32" t="s">
         <v>204</v>
       </c>
@@ -6717,7 +7103,7 @@
       <c r="G32" s="20"/>
     </row>
     <row r="33" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D33" s="75"/>
+      <c r="D33" s="76"/>
       <c r="E33" t="s">
         <v>88</v>
       </c>
@@ -6727,7 +7113,7 @@
       <c r="G33" s="20"/>
     </row>
     <row r="34" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D34" s="75"/>
+      <c r="D34" s="76"/>
       <c r="E34" s="1" t="s">
         <v>6</v>
       </c>
@@ -6738,7 +7124,7 @@
       <c r="G34" s="20"/>
     </row>
     <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="75"/>
+      <c r="D35" s="76"/>
       <c r="E35" t="s">
         <v>31</v>
       </c>
@@ -6750,7 +7136,7 @@
       </c>
     </row>
     <row r="36" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D36" s="75"/>
+      <c r="D36" s="76"/>
       <c r="E36" t="s">
         <v>33</v>
       </c>
@@ -6762,7 +7148,7 @@
       </c>
     </row>
     <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="75"/>
+      <c r="D37" s="76"/>
       <c r="E37" t="s">
         <v>32</v>
       </c>
@@ -6774,7 +7160,7 @@
       </c>
     </row>
     <row r="38" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D38" s="75"/>
+      <c r="D38" s="76"/>
       <c r="E38" t="s">
         <v>34</v>
       </c>
@@ -6786,7 +7172,7 @@
       </c>
     </row>
     <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D39" s="75"/>
+      <c r="D39" s="76"/>
       <c r="E39" t="s">
         <v>67</v>
       </c>
@@ -6798,7 +7184,7 @@
       </c>
     </row>
     <row r="40" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D40" s="75"/>
+      <c r="D40" s="76"/>
       <c r="E40" t="s">
         <v>68</v>
       </c>
@@ -6810,7 +7196,7 @@
       </c>
     </row>
     <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D41" s="75"/>
+      <c r="D41" s="76"/>
       <c r="E41" t="s">
         <v>74</v>
       </c>
@@ -6822,7 +7208,7 @@
       </c>
     </row>
     <row r="42" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D42" s="75"/>
+      <c r="D42" s="76"/>
       <c r="E42" t="s">
         <v>76</v>
       </c>
@@ -6834,7 +7220,7 @@
       </c>
     </row>
     <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="75"/>
+      <c r="D43" s="76"/>
       <c r="E43" t="s">
         <v>77</v>
       </c>
@@ -6846,7 +7232,7 @@
       </c>
     </row>
     <row r="44" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D44" s="75"/>
+      <c r="D44" s="76"/>
       <c r="E44" t="s">
         <v>93</v>
       </c>
@@ -6858,7 +7244,7 @@
       </c>
     </row>
     <row r="45" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D45" s="75"/>
+      <c r="D45" s="76"/>
       <c r="E45" t="s">
         <v>94</v>
       </c>
@@ -6870,7 +7256,7 @@
       </c>
     </row>
     <row r="46" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D46" s="75"/>
+      <c r="D46" s="76"/>
       <c r="E46" t="s">
         <v>95</v>
       </c>
@@ -6882,7 +7268,7 @@
       </c>
     </row>
     <row r="47" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D47" s="75"/>
+      <c r="D47" s="76"/>
       <c r="E47" t="s">
         <v>96</v>
       </c>
@@ -6894,7 +7280,7 @@
       </c>
     </row>
     <row r="48" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D48" s="75"/>
+      <c r="D48" s="76"/>
       <c r="E48" t="s">
         <v>97</v>
       </c>
@@ -6906,7 +7292,7 @@
       </c>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D49" s="75"/>
+      <c r="D49" s="76"/>
       <c r="E49" t="s">
         <v>105</v>
       </c>
@@ -6918,7 +7304,7 @@
       </c>
     </row>
     <row r="50" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D50" s="75"/>
+      <c r="D50" s="76"/>
       <c r="E50" t="s">
         <v>106</v>
       </c>
@@ -6930,7 +7316,7 @@
       </c>
     </row>
     <row r="51" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D51" s="75"/>
+      <c r="D51" s="76"/>
       <c r="E51" t="s">
         <v>107</v>
       </c>
@@ -6942,7 +7328,7 @@
       </c>
     </row>
     <row r="52" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D52" s="75"/>
+      <c r="D52" s="76"/>
       <c r="E52" t="s">
         <v>108</v>
       </c>
@@ -6950,7 +7336,7 @@
       <c r="G52" s="20"/>
     </row>
     <row r="53" spans="4:7" ht="13.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D53" s="75"/>
+      <c r="D53" s="76"/>
       <c r="E53" t="s">
         <v>114</v>
       </c>
@@ -6958,7 +7344,7 @@
       <c r="G53" s="20"/>
     </row>
     <row r="54" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D54" s="76"/>
+      <c r="D54" s="77"/>
       <c r="E54" s="1" t="s">
         <v>10</v>
       </c>
@@ -6983,7 +7369,7 @@
   <dimension ref="D7:G23"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7010,7 +7396,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="72" t="s">
         <v>137</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -7022,7 +7408,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="11" t="s">
         <v>18</v>
       </c>
@@ -7032,7 +7418,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="11" t="s">
         <v>43</v>
       </c>
@@ -7042,7 +7428,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="72"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="11" t="s">
         <v>102</v>
       </c>
@@ -7052,7 +7438,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="11" t="s">
         <v>178</v>
       </c>
@@ -7062,7 +7448,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D14" s="72"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="11" t="s">
         <v>19</v>
       </c>
@@ -7072,7 +7458,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="13" t="s">
         <v>6</v>
       </c>
@@ -7083,7 +7469,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="72"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="11" t="s">
         <v>31</v>
       </c>
@@ -7095,7 +7481,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D17" s="72"/>
+      <c r="D17" s="73"/>
       <c r="E17" s="11" t="s">
         <v>33</v>
       </c>
@@ -7107,7 +7493,7 @@
       </c>
     </row>
     <row r="18" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D18" s="72"/>
+      <c r="D18" s="73"/>
       <c r="E18" s="11" t="s">
         <v>32</v>
       </c>
@@ -7119,7 +7505,7 @@
       </c>
     </row>
     <row r="19" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D19" s="72"/>
+      <c r="D19" s="73"/>
       <c r="E19" s="11" t="s">
         <v>34</v>
       </c>
@@ -7131,7 +7517,7 @@
       </c>
     </row>
     <row r="20" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D20" s="72"/>
+      <c r="D20" s="73"/>
       <c r="E20" s="11" t="s">
         <v>67</v>
       </c>
@@ -7143,7 +7529,7 @@
       </c>
     </row>
     <row r="21" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D21" s="72"/>
+      <c r="D21" s="73"/>
       <c r="E21" s="11" t="s">
         <v>74</v>
       </c>
@@ -7155,21 +7541,25 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="72"/>
+      <c r="D22" s="73"/>
       <c r="E22" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="4"/>
+      <c r="F22" s="43">
+        <v>10000</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="23" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D23" s="73"/>
+      <c r="D23" s="74"/>
       <c r="E23" s="13" t="s">
         <v>13</v>
       </c>
       <c r="F23" s="44">
         <f>F15-SUM(F16:F22)</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="G23" s="21"/>
     </row>
@@ -7214,7 +7604,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="71" t="s">
+      <c r="D9" s="72" t="s">
         <v>103</v>
       </c>
       <c r="E9" s="9" t="s">
@@ -7226,7 +7616,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D10" s="72"/>
+      <c r="D10" s="73"/>
       <c r="E10" s="31" t="s">
         <v>42</v>
       </c>
@@ -7236,7 +7626,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D11" s="72"/>
+      <c r="D11" s="73"/>
       <c r="E11" s="11" t="s">
         <v>197</v>
       </c>
@@ -7246,7 +7636,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D12" s="72"/>
+      <c r="D12" s="73"/>
       <c r="E12" s="13" t="s">
         <v>6</v>
       </c>
@@ -7257,7 +7647,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="72"/>
+      <c r="D13" s="73"/>
       <c r="E13" s="11" t="s">
         <v>31</v>
       </c>
@@ -7269,7 +7659,7 @@
       </c>
     </row>
     <row r="14" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D14" s="72"/>
+      <c r="D14" s="73"/>
       <c r="E14" s="11" t="s">
         <v>33</v>
       </c>
@@ -7281,7 +7671,7 @@
       </c>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="72"/>
+      <c r="D15" s="73"/>
       <c r="E15" s="11" t="s">
         <v>32</v>
       </c>
@@ -7293,7 +7683,7 @@
       </c>
     </row>
     <row r="16" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D16" s="72"/>
+      <c r="D16" s="73"/>
       <c r="E16" s="11" t="s">
         <v>34</v>
       </c>
@@ -7305,7 +7695,7 @@
       </c>
     </row>
     <row r="17" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D17" s="73"/>
+      <c r="D17" s="74"/>
       <c r="E17" s="13" t="s">
         <v>13</v>
       </c>
@@ -7325,10 +7715,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD5D84FA-9CC3-4824-9FF8-8D618F1A4440}">
-  <dimension ref="D7:I59"/>
+  <dimension ref="D7:J66"/>
   <sheetViews>
-    <sheetView topLeftCell="C42" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C57" sqref="A57:XFD57"/>
+    <sheetView topLeftCell="C46" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F64" activeCellId="2" sqref="F63 F64 F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7336,7 +7726,7 @@
     <col min="4" max="4" width="27.33203125" customWidth="1"/>
     <col min="5" max="5" width="45.44140625" customWidth="1"/>
     <col min="6" max="6" width="32.88671875" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="7" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -7355,7 +7745,7 @@
       </c>
     </row>
     <row r="9" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D9" s="77" t="s">
+      <c r="D9" s="78" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="18" t="s">
@@ -7367,7 +7757,7 @@
       <c r="G9" s="20"/>
     </row>
     <row r="10" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D10" s="78"/>
+      <c r="D10" s="79"/>
       <c r="E10" s="19" t="s">
         <v>104</v>
       </c>
@@ -7377,7 +7767,7 @@
       <c r="G10" s="20"/>
     </row>
     <row r="11" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="78"/>
+      <c r="D11" s="79"/>
       <c r="E11" s="19" t="s">
         <v>91</v>
       </c>
@@ -7387,7 +7777,7 @@
       <c r="G11" s="20"/>
     </row>
     <row r="12" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D12" s="78"/>
+      <c r="D12" s="79"/>
       <c r="E12" s="19" t="s">
         <v>21</v>
       </c>
@@ -7397,7 +7787,7 @@
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D13" s="78"/>
+      <c r="D13" s="79"/>
       <c r="E13" s="19" t="s">
         <v>125</v>
       </c>
@@ -7407,7 +7797,7 @@
       <c r="G13" s="20"/>
     </row>
     <row r="14" spans="4:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="D14" s="78"/>
+      <c r="D14" s="79"/>
       <c r="E14" s="60" t="s">
         <v>183</v>
       </c>
@@ -7417,7 +7807,7 @@
       <c r="G14" s="20"/>
     </row>
     <row r="15" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D15" s="78"/>
+      <c r="D15" s="79"/>
       <c r="E15" s="19" t="s">
         <v>134</v>
       </c>
@@ -7427,7 +7817,7 @@
       <c r="G15" s="20"/>
     </row>
     <row r="16" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D16" s="78"/>
+      <c r="D16" s="79"/>
       <c r="E16" s="19" t="s">
         <v>182</v>
       </c>
@@ -7437,27 +7827,27 @@
       <c r="G16" s="20"/>
     </row>
     <row r="17" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D17" s="78"/>
+      <c r="D17" s="79"/>
       <c r="E17" s="19" t="s">
         <v>116</v>
       </c>
       <c r="F17" s="12">
-        <v>71000</v>
+        <v>74780</v>
       </c>
       <c r="G17" s="20"/>
     </row>
     <row r="18" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D18" s="78"/>
+      <c r="D18" s="79"/>
       <c r="E18" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F18" s="12">
-        <v>300000</v>
+        <v>290000</v>
       </c>
       <c r="G18" s="20"/>
     </row>
     <row r="19" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D19" s="78"/>
+      <c r="D19" s="79"/>
       <c r="E19" s="19" t="s">
         <v>177</v>
       </c>
@@ -7467,7 +7857,7 @@
       <c r="G19" s="20"/>
     </row>
     <row r="20" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D20" s="78"/>
+      <c r="D20" s="79"/>
       <c r="E20" s="19" t="s">
         <v>198</v>
       </c>
@@ -7476,509 +7866,657 @@
       </c>
       <c r="G20" s="20"/>
     </row>
-    <row r="21" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D21" s="78"/>
+    <row r="21" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D21" s="79"/>
       <c r="E21" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="F21" s="12">
+        <v>6250</v>
+      </c>
+      <c r="G21" s="20"/>
+    </row>
+    <row r="22" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D22" s="79"/>
+      <c r="E22" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="F21" s="12">
+      <c r="F22" s="12">
         <v>54100</v>
       </c>
-      <c r="G21" s="20"/>
-    </row>
-    <row r="22" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D22" s="78"/>
-      <c r="E22" s="13" t="s">
+      <c r="G22" s="20"/>
+    </row>
+    <row r="23" spans="4:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D23" s="79"/>
+      <c r="E23" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="14">
-        <f>SUM(F9:F21)</f>
-        <v>807585</v>
-      </c>
-      <c r="G22" s="20"/>
-    </row>
-    <row r="23" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D23" s="78"/>
-      <c r="E23" s="19" t="s">
+      <c r="F23" s="14">
+        <f>SUM(F9:F22)</f>
+        <v>807615</v>
+      </c>
+      <c r="G23" s="20"/>
+    </row>
+    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D24" s="79"/>
+      <c r="E24" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="F23" s="41">
+      <c r="F24" s="41">
         <v>80000</v>
       </c>
-      <c r="G23" s="20" t="s">
+      <c r="G24" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D24" s="78"/>
-      <c r="E24" s="19" t="s">
+    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D25" s="79"/>
+      <c r="E25" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="41">
+      <c r="F25" s="41">
         <v>26500</v>
       </c>
-      <c r="G24" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="H24" t="s">
+      <c r="H25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D25" s="78"/>
-      <c r="E25" s="19" t="s">
+    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D26" s="79"/>
+      <c r="E26" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="41">
+      <c r="F26" s="41">
         <v>50000</v>
       </c>
-      <c r="G25" s="20" t="s">
+      <c r="G26" s="20" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D26" s="78"/>
-      <c r="E26" s="19" t="s">
+    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D27" s="79"/>
+      <c r="E27" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F27" s="41">
         <v>14000</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D27" s="78"/>
-      <c r="E27" s="19" t="s">
+    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="D28" s="79"/>
+      <c r="E28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="F27" s="41">
+      <c r="F28" s="41">
         <v>5000</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="28" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D28" s="78"/>
-      <c r="E28" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="41">
-        <v>27000</v>
       </c>
       <c r="G28" s="20" t="s">
         <v>35</v>
       </c>
+      <c r="H28" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="29" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D29" s="78"/>
+      <c r="D29" s="79"/>
       <c r="E29" s="19" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F29" s="41">
-        <v>50000</v>
+        <v>27000</v>
       </c>
       <c r="G29" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H29" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="30" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D30" s="78"/>
+      <c r="D30" s="79"/>
       <c r="E30" s="19" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F30" s="41">
-        <v>11270</v>
+        <v>50000</v>
       </c>
       <c r="G30" s="20" t="s">
         <v>35</v>
       </c>
+      <c r="H30" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="31" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D31" s="78"/>
+      <c r="D31" s="79"/>
       <c r="E31" s="19" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="F31" s="41">
-        <v>21725</v>
+        <v>11270</v>
       </c>
       <c r="G31" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="32" spans="4:8" x14ac:dyDescent="0.3">
-      <c r="D32" s="78"/>
+      <c r="D32" s="79"/>
       <c r="E32" s="19" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F32" s="41">
-        <v>44325</v>
+        <v>21725</v>
       </c>
       <c r="G32" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="33" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D33" s="78"/>
+      <c r="D33" s="79"/>
       <c r="E33" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F33" s="41">
-        <v>21560</v>
+        <v>44325</v>
       </c>
       <c r="G33" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="34" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D34" s="78"/>
+      <c r="D34" s="79"/>
       <c r="E34" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F34" s="41">
-        <v>7250</v>
+        <v>21560</v>
       </c>
       <c r="G34" s="20" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="35" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D35" s="78"/>
+      <c r="D35" s="79"/>
       <c r="E35" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F35" s="41">
-        <v>18600</v>
+        <v>7250</v>
       </c>
       <c r="G35" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H35" t="s">
-        <v>123</v>
-      </c>
     </row>
     <row r="36" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D36" s="78"/>
+      <c r="D36" s="79"/>
       <c r="E36" s="19" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F36" s="41">
-        <v>44325</v>
+        <v>18600</v>
       </c>
       <c r="G36" s="20" t="s">
         <v>35</v>
       </c>
+      <c r="H36" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="37" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D37" s="78"/>
+      <c r="D37" s="79"/>
       <c r="E37" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F37" s="41">
+        <v>44325</v>
+      </c>
+      <c r="G37" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D38" s="79"/>
+      <c r="E38" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="F37" s="41">
+      <c r="F38" s="41">
         <v>1800</v>
       </c>
-      <c r="G37" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D38" s="78"/>
-      <c r="E38" s="19" t="s">
+    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D39" s="79"/>
+      <c r="E39" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="F38" s="41">
+      <c r="F39" s="41">
         <v>1750</v>
       </c>
-      <c r="G38" s="20" t="s">
+      <c r="G39" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D39" s="78"/>
-      <c r="E39" s="19" t="s">
+    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D40" s="79"/>
+      <c r="E40" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="F39" s="41">
+      <c r="F40" s="41">
         <v>21300</v>
       </c>
-      <c r="G39" s="20" t="s">
+      <c r="G40" s="20" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D40" s="78"/>
-      <c r="E40" s="19" t="s">
+    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
+      <c r="D41" s="79"/>
+      <c r="E41" s="19" t="s">
         <v>114</v>
       </c>
-      <c r="F40" s="41">
+      <c r="F41" s="41">
         <v>4700</v>
-      </c>
-      <c r="G40" s="20" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="41" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D41" s="78"/>
-      <c r="E41" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="F41" s="41">
-        <v>5590</v>
       </c>
       <c r="G41" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="42" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D42" s="78"/>
+      <c r="D42" s="79"/>
       <c r="E42" s="19" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F42" s="41">
-        <v>30000</v>
+        <v>5590</v>
       </c>
       <c r="G42" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H42" t="s">
-        <v>123</v>
-      </c>
-      <c r="I42">
-        <v>126500</v>
-      </c>
     </row>
     <row r="43" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D43" s="78"/>
+      <c r="D43" s="79"/>
       <c r="E43" s="19" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F43" s="41">
-        <v>3730</v>
+        <v>30000</v>
       </c>
       <c r="G43" s="20" t="s">
         <v>119</v>
       </c>
+      <c r="H43" t="s">
+        <v>123</v>
+      </c>
+      <c r="I43">
+        <v>126500</v>
+      </c>
     </row>
     <row r="44" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D44" s="78"/>
+      <c r="D44" s="79"/>
       <c r="E44" s="19" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="F44" s="41">
-        <v>10000</v>
+        <v>3730</v>
       </c>
       <c r="G44" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H44" t="s">
-        <v>123</v>
-      </c>
-      <c r="I44">
-        <v>136500</v>
-      </c>
     </row>
     <row r="45" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D45" s="78"/>
+      <c r="D45" s="79"/>
       <c r="E45" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F45" s="41">
-        <v>4200</v>
+        <v>10000</v>
       </c>
       <c r="G45" s="20" t="s">
         <v>119</v>
       </c>
+      <c r="H45" t="s">
+        <v>123</v>
+      </c>
+      <c r="I45">
+        <v>136500</v>
+      </c>
     </row>
     <row r="46" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D46" s="78"/>
+      <c r="D46" s="79"/>
       <c r="E46" s="19" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="F46" s="41">
-        <v>35000</v>
+        <v>4200</v>
       </c>
       <c r="G46" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="47" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D47" s="78"/>
+      <c r="D47" s="79"/>
       <c r="E47" s="19" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="F47" s="41">
-        <v>16000</v>
+        <v>35000</v>
       </c>
       <c r="G47" s="20" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="48" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D48" s="78"/>
+      <c r="D48" s="79"/>
       <c r="E48" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F48" s="41">
-        <v>63500</v>
+        <v>16000</v>
       </c>
       <c r="G48" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H48" t="s">
-        <v>123</v>
-      </c>
-      <c r="I48">
-        <v>200000</v>
-      </c>
-    </row>
-    <row r="49" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D49" s="78"/>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D49" s="79"/>
       <c r="E49" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F49" s="41">
-        <v>11350</v>
+        <v>63500</v>
       </c>
       <c r="G49" s="20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="50" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D50" s="78"/>
+      <c r="H49" t="s">
+        <v>123</v>
+      </c>
+      <c r="I49">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D50" s="79"/>
       <c r="E50" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="F50" s="41">
+        <v>11350</v>
+      </c>
+      <c r="G50" s="20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D51" s="79"/>
+      <c r="E51" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="F50" s="41">
+      <c r="F51" s="41">
         <v>14900</v>
       </c>
-      <c r="G50" s="20" t="s">
+      <c r="G51" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="51" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D51" s="78"/>
-      <c r="E51" s="19" t="s">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D52" s="79"/>
+      <c r="E52" s="19" t="s">
         <v>167</v>
       </c>
-      <c r="F51" s="41">
+      <c r="F52" s="41">
         <v>20000</v>
-      </c>
-      <c r="G51" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="H51" t="s">
-        <v>181</v>
-      </c>
-      <c r="I51">
-        <v>220000</v>
-      </c>
-    </row>
-    <row r="52" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D52" s="78"/>
-      <c r="E52" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="F52" s="41">
-        <v>4350</v>
       </c>
       <c r="G52" s="20" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="53" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D53" s="78"/>
+      <c r="H52" t="s">
+        <v>181</v>
+      </c>
+      <c r="I52">
+        <v>220000</v>
+      </c>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D53" s="79"/>
       <c r="E53" s="19" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="F53" s="41">
-        <v>15000</v>
+        <v>4350</v>
       </c>
       <c r="G53" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="H53" t="s">
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D54" s="79"/>
+      <c r="E54" s="19" t="s">
+        <v>180</v>
+      </c>
+      <c r="F54" s="41">
+        <v>15000</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="H54" t="s">
         <v>190</v>
       </c>
-      <c r="I53">
+      <c r="I54">
         <v>50000</v>
       </c>
     </row>
-    <row r="54" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D54" s="78"/>
-      <c r="E54" s="19" t="s">
+    <row r="55" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D55" s="79"/>
+      <c r="E55" s="19" t="s">
         <v>191</v>
       </c>
-      <c r="F54" s="41">
+      <c r="F55" s="41">
         <v>2890</v>
       </c>
-      <c r="G54" s="20" t="s">
+      <c r="G55" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="55" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D55" s="78"/>
-      <c r="E55" s="19" t="s">
+    <row r="56" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D56" s="79"/>
+      <c r="E56" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="F55" s="41">
+      <c r="F56" s="41">
         <v>20000</v>
       </c>
-      <c r="G55" s="20" t="s">
+      <c r="G56" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="H55" t="s">
+      <c r="H56" t="s">
         <v>190</v>
       </c>
-      <c r="I55">
+      <c r="I56">
         <v>70000</v>
       </c>
     </row>
-    <row r="56" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D56" s="78"/>
-      <c r="E56" s="19"/>
-      <c r="F56" s="41"/>
-      <c r="G56" s="20"/>
-    </row>
-    <row r="57" spans="4:9" x14ac:dyDescent="0.3">
-      <c r="D57" s="78"/>
-      <c r="E57" s="19"/>
-      <c r="F57" s="41"/>
-      <c r="G57" s="20"/>
-    </row>
-    <row r="58" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="D58" s="78"/>
+    <row r="57" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D57" s="79"/>
+      <c r="E57" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F57" s="41">
+        <v>25000</v>
+      </c>
+      <c r="G57" s="63" t="s">
+        <v>205</v>
+      </c>
+      <c r="H57" t="s">
+        <v>123</v>
+      </c>
+      <c r="I57">
+        <f>I52+F57</f>
+        <v>245000</v>
+      </c>
+      <c r="J57">
+        <f>F18-I57</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="58" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D58" s="79"/>
       <c r="E58" s="19" t="s">
-        <v>193</v>
-      </c>
-      <c r="F58" s="12">
-        <v>0</v>
+        <v>208</v>
+      </c>
+      <c r="F58" s="41">
+        <v>10000</v>
       </c>
       <c r="G58" s="20" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="59" spans="4:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H58" t="s">
+        <v>190</v>
+      </c>
+      <c r="I58">
+        <v>80000</v>
+      </c>
+      <c r="J58">
+        <f>SUM(F16:F17)-I58</f>
+        <v>13780</v>
+      </c>
+    </row>
+    <row r="59" spans="4:10" x14ac:dyDescent="0.3">
       <c r="D59" s="79"/>
-      <c r="E59" s="1" t="s">
+      <c r="E59" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="F59" s="41">
+        <v>13780</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H59" t="s">
+        <v>190</v>
+      </c>
+      <c r="I59">
+        <f>I58+J58</f>
+        <v>93780</v>
+      </c>
+      <c r="J59">
+        <f>SUM(F16:F17)-I59</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D60" s="79"/>
+      <c r="E60" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="F60" s="41">
+        <v>6250</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D61" s="79"/>
+      <c r="E61" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="F61" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H61" t="s">
+        <v>129</v>
+      </c>
+      <c r="I61">
+        <f>I57+F61</f>
+        <v>255000</v>
+      </c>
+      <c r="J61">
+        <f>$F$18-I61</f>
+        <v>35000</v>
+      </c>
+    </row>
+    <row r="62" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D62" s="79"/>
+      <c r="E62" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="F62" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="H62" t="s">
+        <v>129</v>
+      </c>
+      <c r="I62">
+        <f>I61+F62</f>
+        <v>265000</v>
+      </c>
+      <c r="J62">
+        <f>$F$18-I62</f>
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D63" s="79"/>
+      <c r="E63" s="19" t="s">
+        <v>216</v>
+      </c>
+      <c r="F63" s="41">
+        <v>10000</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="64" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D64" s="79"/>
+      <c r="E64" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="F64" s="41">
+        <v>14970</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="65" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D65" s="79"/>
+      <c r="E65" s="19" t="s">
+        <v>218</v>
+      </c>
+      <c r="F65" s="12">
+        <v>0</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="66" spans="4:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="D66" s="80"/>
+      <c r="E66" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F59" s="14">
-        <f>F22-SUM(F23:F58)</f>
-        <v>99970</v>
-      </c>
-      <c r="G59" s="21"/>
+      <c r="F66" s="14">
+        <f>F23-SUM(F24:F65)</f>
+        <v>0</v>
+      </c>
+      <c r="G66" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D9:D59"/>
+    <mergeCell ref="D9:D66"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>